<commit_message>
changes opcode order for jumps and calls
</commit_message>
<xml_diff>
--- a/doc/instruction-set.xlsx
+++ b/doc/instruction-set.xlsx
@@ -773,184 +773,184 @@
     <t xml:space="preserve">Compare accumulator (A register) with given data</t>
   </si>
   <si>
+    <t xml:space="preserve">JMP M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump unconditionally</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump to memory address in H and L registers</t>
+  </si>
+  <si>
     <t xml:space="preserve">JMP addr</t>
   </si>
   <si>
-    <t xml:space="preserve">Jump unconditionally</t>
-  </si>
-  <si>
     <t xml:space="preserve">JMP FFF0h</t>
   </si>
   <si>
     <t xml:space="preserve">Jump to given address</t>
   </si>
   <si>
-    <t xml:space="preserve">JMP M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jump to memory address in H and L registers</t>
+    <t xml:space="preserve">JC M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump on carry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump to memory address in H and L registers if carry flag is set</t>
   </si>
   <si>
     <t xml:space="preserve">JC addr</t>
   </si>
   <si>
-    <t xml:space="preserve">Jump on carry</t>
-  </si>
-  <si>
     <t xml:space="preserve">JC FFF0h</t>
   </si>
   <si>
     <t xml:space="preserve">Jump to given address if carry flag is set</t>
   </si>
   <si>
-    <t xml:space="preserve">JC M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jump to memory address in H and L registers if carry flag is set</t>
+    <t xml:space="preserve">JNC M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump on no carry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump to memory address in H and L registers if carry flag is clear</t>
   </si>
   <si>
     <t xml:space="preserve">JNC addr</t>
   </si>
   <si>
-    <t xml:space="preserve">Jump on no carry</t>
-  </si>
-  <si>
     <t xml:space="preserve">JNC FFF0h</t>
   </si>
   <si>
     <t xml:space="preserve">Jump to given address if carry flag is clear</t>
   </si>
   <si>
-    <t xml:space="preserve">JNC M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jump to memory address in H and L registers if carry flag is clear</t>
+    <t xml:space="preserve">JZ M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump on zero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump to memory address in H and L registers if zero flag is set</t>
   </si>
   <si>
     <t xml:space="preserve">JZ addr</t>
   </si>
   <si>
-    <t xml:space="preserve">Jump on zero</t>
-  </si>
-  <si>
     <t xml:space="preserve">JZ FFF0h</t>
   </si>
   <si>
     <t xml:space="preserve">Jump to given address if zero flag is set</t>
   </si>
   <si>
-    <t xml:space="preserve">JZ M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jump to memory address in H and L registers if zero flag is set</t>
+    <t xml:space="preserve">JNZ M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump on no zero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump to memory address in H and L registers if zero flag is clear</t>
   </si>
   <si>
     <t xml:space="preserve">JNZ addr</t>
   </si>
   <si>
-    <t xml:space="preserve">Jump on no zero</t>
-  </si>
-  <si>
     <t xml:space="preserve">JNZ FFF0h</t>
   </si>
   <si>
     <t xml:space="preserve">Jump to given address if zero flag is clear</t>
   </si>
   <si>
-    <t xml:space="preserve">JNZ M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jump to memory address in H and L registers if zero flag is clear</t>
+    <t xml:space="preserve">CALL M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call unconditionally</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call memory address in H and L registers</t>
   </si>
   <si>
     <t xml:space="preserve">CALL addr</t>
   </si>
   <si>
-    <t xml:space="preserve">Call unconditionally</t>
-  </si>
-  <si>
     <t xml:space="preserve">CALL FFF0h</t>
   </si>
   <si>
     <t xml:space="preserve">Call given address</t>
   </si>
   <si>
-    <t xml:space="preserve">CALL M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Call memory address in H and L registers</t>
+    <t xml:space="preserve">CC M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call on carry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call memory address in H and L registers if carry flag is set</t>
   </si>
   <si>
     <t xml:space="preserve">CC addr</t>
   </si>
   <si>
-    <t xml:space="preserve">Call on carry</t>
-  </si>
-  <si>
     <t xml:space="preserve">CC FFF0h</t>
   </si>
   <si>
     <t xml:space="preserve">Call given address if carry flag is set</t>
   </si>
   <si>
-    <t xml:space="preserve">CC M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Call memory address in H and L registers if carry flag is set</t>
+    <t xml:space="preserve">CNC M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call on no carry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call memory address in H and L registers if carry flag is clear</t>
   </si>
   <si>
     <t xml:space="preserve">CNC addr</t>
   </si>
   <si>
-    <t xml:space="preserve">Call on no carry</t>
-  </si>
-  <si>
     <t xml:space="preserve">CNC FFF0h</t>
   </si>
   <si>
     <t xml:space="preserve">Call given address if carry flag is clear</t>
   </si>
   <si>
-    <t xml:space="preserve">CNC M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Call memory address in H and L registers if carry flag is clear</t>
+    <t xml:space="preserve">CZ M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call on zero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call memory address in H and L registers if zero flag is set</t>
   </si>
   <si>
     <t xml:space="preserve">CZ addr</t>
   </si>
   <si>
-    <t xml:space="preserve">Call on zero</t>
-  </si>
-  <si>
     <t xml:space="preserve">CZ FFF0h</t>
   </si>
   <si>
     <t xml:space="preserve">Call given address if zero flag is set</t>
   </si>
   <si>
-    <t xml:space="preserve">CZ M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Call memory address in H and L registers if zero flag is set</t>
+    <t xml:space="preserve">CNZ M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call on no zero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call memory address in H and L registers if zero flag is clear</t>
   </si>
   <si>
     <t xml:space="preserve">CNZ addr</t>
   </si>
   <si>
-    <t xml:space="preserve">Call on no zero</t>
-  </si>
-  <si>
     <t xml:space="preserve">CNZ FFF0h</t>
   </si>
   <si>
     <t xml:space="preserve">Call given address if zero flag is clear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CNZ M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Call memory address in H and L registers if zero flag is clear</t>
   </si>
   <si>
     <t xml:space="preserve">RET</t>
@@ -3489,10 +3489,10 @@
         <v>251</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>136</v>
+        <v>68</v>
       </c>
       <c r="F110" s="6" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G110" s="6" t="s">
         <v>250</v>
@@ -3504,14 +3504,8 @@
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H110),2)</f>
         <v>83</v>
       </c>
-      <c r="J110" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="K110" s="6" t="s">
-        <v>124</v>
-      </c>
       <c r="L110" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3519,16 +3513,16 @@
         <v>110</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>68</v>
+        <v>136</v>
       </c>
       <c r="F111" s="0" t="s">
         <v>254</v>
       </c>
       <c r="G111" s="0" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H111" s="1" t="n">
         <v>10000101</v>
@@ -3537,6 +3531,12 @@
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H111),2)</f>
         <v>85</v>
       </c>
+      <c r="J111" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="K111" s="0" t="s">
+        <v>124</v>
+      </c>
       <c r="L111" s="0" t="s">
         <v>255</v>
       </c>
@@ -3552,10 +3552,10 @@
         <v>257</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>136</v>
+        <v>68</v>
       </c>
       <c r="F112" s="6" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="G112" s="6" t="s">
         <v>256</v>
@@ -3567,14 +3567,8 @@
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H112),2)</f>
         <v>87</v>
       </c>
-      <c r="J112" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="K112" s="6" t="s">
-        <v>124</v>
-      </c>
       <c r="L112" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3582,16 +3576,16 @@
         <v>112</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>68</v>
+        <v>136</v>
       </c>
       <c r="F113" s="0" t="s">
         <v>260</v>
       </c>
       <c r="G113" s="0" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H113" s="1" t="n">
         <v>10001001</v>
@@ -3600,6 +3594,12 @@
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H113),2)</f>
         <v>89</v>
       </c>
+      <c r="J113" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="K113" s="0" t="s">
+        <v>124</v>
+      </c>
       <c r="L113" s="0" t="s">
         <v>261</v>
       </c>
@@ -3615,10 +3615,10 @@
         <v>263</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>136</v>
+        <v>68</v>
       </c>
       <c r="F114" s="6" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G114" s="6" t="s">
         <v>262</v>
@@ -3630,14 +3630,8 @@
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H114),2)</f>
         <v>8B</v>
       </c>
-      <c r="J114" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="K114" s="6" t="s">
-        <v>124</v>
-      </c>
       <c r="L114" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3645,16 +3639,16 @@
         <v>114</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>68</v>
+        <v>136</v>
       </c>
       <c r="F115" s="0" t="s">
         <v>266</v>
       </c>
       <c r="G115" s="0" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H115" s="1" t="n">
         <v>10010001</v>
@@ -3663,6 +3657,12 @@
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H115),2)</f>
         <v>91</v>
       </c>
+      <c r="J115" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="K115" s="0" t="s">
+        <v>124</v>
+      </c>
       <c r="L115" s="0" t="s">
         <v>267</v>
       </c>
@@ -3678,10 +3678,10 @@
         <v>269</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>136</v>
+        <v>68</v>
       </c>
       <c r="F116" s="6" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G116" s="6" t="s">
         <v>268</v>
@@ -3693,14 +3693,8 @@
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H116),2)</f>
         <v>95</v>
       </c>
-      <c r="J116" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="K116" s="6" t="s">
-        <v>124</v>
-      </c>
       <c r="L116" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3708,16 +3702,16 @@
         <v>116</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D117" s="0" t="s">
-        <v>68</v>
+        <v>136</v>
       </c>
       <c r="F117" s="0" t="s">
         <v>272</v>
       </c>
       <c r="G117" s="0" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H117" s="1" t="n">
         <v>10010111</v>
@@ -3726,6 +3720,12 @@
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H117),2)</f>
         <v>97</v>
       </c>
+      <c r="J117" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="K117" s="0" t="s">
+        <v>124</v>
+      </c>
       <c r="L117" s="0" t="s">
         <v>273</v>
       </c>
@@ -3741,10 +3741,10 @@
         <v>275</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>136</v>
+        <v>68</v>
       </c>
       <c r="F118" s="6" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G118" s="6" t="s">
         <v>274</v>
@@ -3756,14 +3756,8 @@
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H118),2)</f>
         <v>99</v>
       </c>
-      <c r="J118" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="K118" s="6" t="s">
-        <v>124</v>
-      </c>
       <c r="L118" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3771,16 +3765,16 @@
         <v>118</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>68</v>
+        <v>136</v>
       </c>
       <c r="F119" s="0" t="s">
         <v>278</v>
       </c>
       <c r="G119" s="0" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H119" s="1" t="n">
         <v>10011011</v>
@@ -3789,6 +3783,12 @@
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H119),2)</f>
         <v>9B</v>
       </c>
+      <c r="J119" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="K119" s="0" t="s">
+        <v>124</v>
+      </c>
       <c r="L119" s="0" t="s">
         <v>279</v>
       </c>
@@ -3804,10 +3804,10 @@
         <v>281</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>136</v>
+        <v>68</v>
       </c>
       <c r="F120" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="G120" s="6" t="s">
         <v>280</v>
@@ -3819,14 +3819,8 @@
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H120),2)</f>
         <v>A1</v>
       </c>
-      <c r="J120" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="K120" s="6" t="s">
-        <v>124</v>
-      </c>
       <c r="L120" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3834,16 +3828,16 @@
         <v>120</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D121" s="0" t="s">
-        <v>68</v>
+        <v>136</v>
       </c>
       <c r="F121" s="0" t="s">
         <v>284</v>
       </c>
       <c r="G121" s="0" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H121" s="1" t="n">
         <v>10100011</v>
@@ -3852,6 +3846,12 @@
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H121),2)</f>
         <v>A3</v>
       </c>
+      <c r="J121" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="K121" s="0" t="s">
+        <v>124</v>
+      </c>
       <c r="L121" s="0" t="s">
         <v>285</v>
       </c>
@@ -3867,10 +3867,10 @@
         <v>287</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>136</v>
+        <v>68</v>
       </c>
       <c r="F122" s="6" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G122" s="6" t="s">
         <v>286</v>
@@ -3882,14 +3882,8 @@
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H122),2)</f>
         <v>A7</v>
       </c>
-      <c r="J122" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="K122" s="6" t="s">
-        <v>124</v>
-      </c>
       <c r="L122" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3897,16 +3891,16 @@
         <v>122</v>
       </c>
       <c r="B123" s="0" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D123" s="0" t="s">
-        <v>68</v>
+        <v>136</v>
       </c>
       <c r="F123" s="0" t="s">
         <v>290</v>
       </c>
       <c r="G123" s="0" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H123" s="1" t="n">
         <v>10101001</v>
@@ -3915,6 +3909,12 @@
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H123),2)</f>
         <v>A9</v>
       </c>
+      <c r="J123" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="K123" s="0" t="s">
+        <v>124</v>
+      </c>
       <c r="L123" s="0" t="s">
         <v>291</v>
       </c>
@@ -3930,10 +3930,10 @@
         <v>293</v>
       </c>
       <c r="D124" s="6" t="s">
-        <v>136</v>
+        <v>68</v>
       </c>
       <c r="F124" s="6" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G124" s="6" t="s">
         <v>292</v>
@@ -3945,14 +3945,8 @@
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H124),2)</f>
         <v>AB</v>
       </c>
-      <c r="J124" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="K124" s="6" t="s">
-        <v>124</v>
-      </c>
       <c r="L124" s="6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3960,16 +3954,16 @@
         <v>124</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D125" s="0" t="s">
-        <v>68</v>
+        <v>136</v>
       </c>
       <c r="F125" s="0" t="s">
         <v>296</v>
       </c>
       <c r="G125" s="0" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H125" s="1" t="n">
         <v>10110001</v>
@@ -3978,6 +3972,12 @@
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H125),2)</f>
         <v>B1</v>
       </c>
+      <c r="J125" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="K125" s="0" t="s">
+        <v>124</v>
+      </c>
       <c r="L125" s="0" t="s">
         <v>297</v>
       </c>
@@ -3993,10 +3993,10 @@
         <v>299</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>136</v>
+        <v>68</v>
       </c>
       <c r="F126" s="6" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G126" s="6" t="s">
         <v>298</v>
@@ -4008,14 +4008,8 @@
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H126),2)</f>
         <v>B3</v>
       </c>
-      <c r="J126" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="K126" s="6" t="s">
-        <v>124</v>
-      </c>
       <c r="L126" s="6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4023,16 +4017,16 @@
         <v>126</v>
       </c>
       <c r="B127" s="0" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D127" s="0" t="s">
-        <v>68</v>
+        <v>136</v>
       </c>
       <c r="F127" s="0" t="s">
         <v>302</v>
       </c>
       <c r="G127" s="0" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H127" s="1" t="n">
         <v>10110101</v>
@@ -4041,6 +4035,12 @@
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H127),2)</f>
         <v>B5</v>
       </c>
+      <c r="J127" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="K127" s="0" t="s">
+        <v>124</v>
+      </c>
       <c r="L127" s="0" t="s">
         <v>303</v>
       </c>
@@ -4056,10 +4056,10 @@
         <v>305</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>136</v>
+        <v>68</v>
       </c>
       <c r="F128" s="6" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="G128" s="6" t="s">
         <v>304</v>
@@ -4071,14 +4071,8 @@
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H128),2)</f>
         <v>B9</v>
       </c>
-      <c r="J128" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="K128" s="6" t="s">
-        <v>124</v>
-      </c>
       <c r="L128" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4086,16 +4080,16 @@
         <v>128</v>
       </c>
       <c r="B129" s="0" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D129" s="0" t="s">
-        <v>68</v>
+        <v>136</v>
       </c>
       <c r="F129" s="0" t="s">
         <v>308</v>
       </c>
       <c r="G129" s="0" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H129" s="1" t="n">
         <v>10111011</v>
@@ -4103,6 +4097,12 @@
       <c r="I129" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H129),2)</f>
         <v>BB</v>
+      </c>
+      <c r="J129" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="K129" s="0" t="s">
+        <v>124</v>
       </c>
       <c r="L129" s="0" t="s">
         <v>309</v>
@@ -6532,7 +6532,7 @@
       </c>
       <c r="B133" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D133,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D133,'Instruction Set'!I:I,0)))</f>
-        <v>JMP addr</v>
+        <v>JMP M</v>
       </c>
       <c r="C133" s="2" t="str">
         <f aca="false">DEC2BIN(A133,8)</f>
@@ -6566,7 +6566,7 @@
       </c>
       <c r="B135" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D135,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D135,'Instruction Set'!I:I,0)))</f>
-        <v>JMP M</v>
+        <v>JMP addr</v>
       </c>
       <c r="C135" s="2" t="str">
         <f aca="false">DEC2BIN(A135,8)</f>
@@ -6600,7 +6600,7 @@
       </c>
       <c r="B137" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D137,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D137,'Instruction Set'!I:I,0)))</f>
-        <v>JC addr</v>
+        <v>JC M</v>
       </c>
       <c r="C137" s="2" t="str">
         <f aca="false">DEC2BIN(A137,8)</f>
@@ -6634,7 +6634,7 @@
       </c>
       <c r="B139" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D139,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D139,'Instruction Set'!I:I,0)))</f>
-        <v>JC M</v>
+        <v>JC addr</v>
       </c>
       <c r="C139" s="2" t="str">
         <f aca="false">DEC2BIN(A139,8)</f>
@@ -6668,7 +6668,7 @@
       </c>
       <c r="B141" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D141,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D141,'Instruction Set'!I:I,0)))</f>
-        <v>JNC addr</v>
+        <v>JNC M</v>
       </c>
       <c r="C141" s="2" t="str">
         <f aca="false">DEC2BIN(A141,8)</f>
@@ -6770,7 +6770,7 @@
       </c>
       <c r="B147" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D147,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D147,'Instruction Set'!I:I,0)))</f>
-        <v>JNC M</v>
+        <v>JNC addr</v>
       </c>
       <c r="C147" s="2" t="str">
         <f aca="false">DEC2BIN(A147,8)</f>
@@ -6838,7 +6838,7 @@
       </c>
       <c r="B151" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D151,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D151,'Instruction Set'!I:I,0)))</f>
-        <v>JZ addr</v>
+        <v>JZ M</v>
       </c>
       <c r="C151" s="2" t="str">
         <f aca="false">DEC2BIN(A151,8)</f>
@@ -6872,7 +6872,7 @@
       </c>
       <c r="B153" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D153,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D153,'Instruction Set'!I:I,0)))</f>
-        <v>JZ M</v>
+        <v>JZ addr</v>
       </c>
       <c r="C153" s="2" t="str">
         <f aca="false">DEC2BIN(A153,8)</f>
@@ -6906,7 +6906,7 @@
       </c>
       <c r="B155" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D155,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D155,'Instruction Set'!I:I,0)))</f>
-        <v>JNZ addr</v>
+        <v>JNZ M</v>
       </c>
       <c r="C155" s="2" t="str">
         <f aca="false">DEC2BIN(A155,8)</f>
@@ -6940,7 +6940,7 @@
       </c>
       <c r="B157" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D157,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D157,'Instruction Set'!I:I,0)))</f>
-        <v>JNZ M</v>
+        <v>JNZ addr</v>
       </c>
       <c r="C157" s="2" t="str">
         <f aca="false">DEC2BIN(A157,8)</f>
@@ -7042,7 +7042,7 @@
       </c>
       <c r="B163" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D163,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D163,'Instruction Set'!I:I,0)))</f>
-        <v>CALL addr</v>
+        <v>CALL M</v>
       </c>
       <c r="C163" s="2" t="str">
         <f aca="false">DEC2BIN(A163,8)</f>
@@ -7076,7 +7076,7 @@
       </c>
       <c r="B165" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D165,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D165,'Instruction Set'!I:I,0)))</f>
-        <v>CALL M</v>
+        <v>CALL addr</v>
       </c>
       <c r="C165" s="2" t="str">
         <f aca="false">DEC2BIN(A165,8)</f>
@@ -7144,7 +7144,7 @@
       </c>
       <c r="B169" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D169,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D169,'Instruction Set'!I:I,0)))</f>
-        <v>CC addr</v>
+        <v>CC M</v>
       </c>
       <c r="C169" s="2" t="str">
         <f aca="false">DEC2BIN(A169,8)</f>
@@ -7178,7 +7178,7 @@
       </c>
       <c r="B171" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D171,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D171,'Instruction Set'!I:I,0)))</f>
-        <v>CC M</v>
+        <v>CC addr</v>
       </c>
       <c r="C171" s="2" t="str">
         <f aca="false">DEC2BIN(A171,8)</f>
@@ -7212,7 +7212,7 @@
       </c>
       <c r="B173" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D173,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D173,'Instruction Set'!I:I,0)))</f>
-        <v>CNC addr</v>
+        <v>CNC M</v>
       </c>
       <c r="C173" s="2" t="str">
         <f aca="false">DEC2BIN(A173,8)</f>
@@ -7314,7 +7314,7 @@
       </c>
       <c r="B179" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D179,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D179,'Instruction Set'!I:I,0)))</f>
-        <v>CNC M</v>
+        <v>CNC addr</v>
       </c>
       <c r="C179" s="2" t="str">
         <f aca="false">DEC2BIN(A179,8)</f>
@@ -7348,7 +7348,7 @@
       </c>
       <c r="B181" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D181,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D181,'Instruction Set'!I:I,0)))</f>
-        <v>CZ addr</v>
+        <v>CZ M</v>
       </c>
       <c r="C181" s="2" t="str">
         <f aca="false">DEC2BIN(A181,8)</f>
@@ -7382,7 +7382,7 @@
       </c>
       <c r="B183" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D183,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D183,'Instruction Set'!I:I,0)))</f>
-        <v>CZ M</v>
+        <v>CZ addr</v>
       </c>
       <c r="C183" s="2" t="str">
         <f aca="false">DEC2BIN(A183,8)</f>
@@ -7450,7 +7450,7 @@
       </c>
       <c r="B187" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D187,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D187,'Instruction Set'!I:I,0)))</f>
-        <v>CNZ addr</v>
+        <v>CNZ M</v>
       </c>
       <c r="C187" s="2" t="str">
         <f aca="false">DEC2BIN(A187,8)</f>
@@ -7484,7 +7484,7 @@
       </c>
       <c r="B189" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D189,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D189,'Instruction Set'!I:I,0)))</f>
-        <v>CNZ M</v>
+        <v>CNZ addr</v>
       </c>
       <c r="C189" s="2" t="str">
         <f aca="false">DEC2BIN(A189,8)</f>

</xml_diff>

<commit_message>
optimized jump and call opcodes
</commit_message>
<xml_diff>
--- a/doc/instruction-set.xlsx
+++ b/doc/instruction-set.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="350">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -779,6 +779,9 @@
     <t xml:space="preserve">Jump unconditionally</t>
   </si>
   <si>
+    <t xml:space="preserve">01110101</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jump to memory address in H and L registers</t>
   </si>
   <si>
@@ -788,6 +791,9 @@
     <t xml:space="preserve">JMP FFF0h</t>
   </si>
   <si>
+    <t xml:space="preserve">01110111</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jump to given address</t>
   </si>
   <si>
@@ -797,6 +803,9 @@
     <t xml:space="preserve">Jump on carry</t>
   </si>
   <si>
+    <t xml:space="preserve">01111001</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jump to memory address in H and L registers if carry flag is set</t>
   </si>
   <si>
@@ -806,6 +815,9 @@
     <t xml:space="preserve">JC FFF0h</t>
   </si>
   <si>
+    <t xml:space="preserve">01111011</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jump to given address if carry flag is set</t>
   </si>
   <si>
@@ -815,6 +827,9 @@
     <t xml:space="preserve">Jump on no carry</t>
   </si>
   <si>
+    <t xml:space="preserve">01111101</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jump to memory address in H and L registers if carry flag is clear</t>
   </si>
   <si>
@@ -824,6 +839,9 @@
     <t xml:space="preserve">JNC FFF0h</t>
   </si>
   <si>
+    <t xml:space="preserve">01111111</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jump to given address if carry flag is clear</t>
   </si>
   <si>
@@ -833,6 +851,9 @@
     <t xml:space="preserve">Jump on zero</t>
   </si>
   <si>
+    <t xml:space="preserve">10001111</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jump to memory address in H and L registers if zero flag is set</t>
   </si>
   <si>
@@ -842,6 +863,9 @@
     <t xml:space="preserve">JZ FFF0h</t>
   </si>
   <si>
+    <t xml:space="preserve">10011111</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jump to given address if zero flag is set</t>
   </si>
   <si>
@@ -851,6 +875,9 @@
     <t xml:space="preserve">Jump on no zero</t>
   </si>
   <si>
+    <t xml:space="preserve">10101111</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jump to memory address in H and L registers if zero flag is clear</t>
   </si>
   <si>
@@ -860,6 +887,9 @@
     <t xml:space="preserve">JNZ FFF0h</t>
   </si>
   <si>
+    <t xml:space="preserve">10111111</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jump to given address if zero flag is clear</t>
   </si>
   <si>
@@ -869,6 +899,9 @@
     <t xml:space="preserve">Call unconditionally</t>
   </si>
   <si>
+    <t xml:space="preserve">11000001</t>
+  </si>
+  <si>
     <t xml:space="preserve">Call memory address in H and L registers</t>
   </si>
   <si>
@@ -878,6 +911,9 @@
     <t xml:space="preserve">CALL FFF0h</t>
   </si>
   <si>
+    <t xml:space="preserve">11000011</t>
+  </si>
+  <si>
     <t xml:space="preserve">Call given address</t>
   </si>
   <si>
@@ -887,6 +923,9 @@
     <t xml:space="preserve">Call on carry</t>
   </si>
   <si>
+    <t xml:space="preserve">11000101</t>
+  </si>
+  <si>
     <t xml:space="preserve">Call memory address in H and L registers if carry flag is set</t>
   </si>
   <si>
@@ -896,6 +935,9 @@
     <t xml:space="preserve">CC FFF0h</t>
   </si>
   <si>
+    <t xml:space="preserve">11000111</t>
+  </si>
+  <si>
     <t xml:space="preserve">Call given address if carry flag is set</t>
   </si>
   <si>
@@ -905,6 +947,9 @@
     <t xml:space="preserve">Call on no carry</t>
   </si>
   <si>
+    <t xml:space="preserve">11001011</t>
+  </si>
+  <si>
     <t xml:space="preserve">Call memory address in H and L registers if carry flag is clear</t>
   </si>
   <si>
@@ -914,6 +959,9 @@
     <t xml:space="preserve">CNC FFF0h</t>
   </si>
   <si>
+    <t xml:space="preserve">11001111</t>
+  </si>
+  <si>
     <t xml:space="preserve">Call given address if carry flag is clear</t>
   </si>
   <si>
@@ -923,6 +971,9 @@
     <t xml:space="preserve">Call on zero</t>
   </si>
   <si>
+    <t xml:space="preserve">11010001</t>
+  </si>
+  <si>
     <t xml:space="preserve">Call memory address in H and L registers if zero flag is set</t>
   </si>
   <si>
@@ -932,6 +983,9 @@
     <t xml:space="preserve">CZ FFF0h</t>
   </si>
   <si>
+    <t xml:space="preserve">11010011</t>
+  </si>
+  <si>
     <t xml:space="preserve">Call given address if zero flag is set</t>
   </si>
   <si>
@@ -941,6 +995,9 @@
     <t xml:space="preserve">Call on no zero</t>
   </si>
   <si>
+    <t xml:space="preserve">11010101</t>
+  </si>
+  <si>
     <t xml:space="preserve">Call memory address in H and L registers if zero flag is clear</t>
   </si>
   <si>
@@ -948,6 +1005,9 @@
   </si>
   <si>
     <t xml:space="preserve">CNZ FFF0h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11010111</t>
   </si>
   <si>
     <t xml:space="preserve">Call given address if zero flag is clear</t>
@@ -3497,15 +3557,15 @@
       <c r="G110" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="H110" s="7" t="n">
-        <v>10000011</v>
+      <c r="H110" s="7" t="s">
+        <v>252</v>
       </c>
       <c r="I110" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H110),2)</f>
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="L110" s="6" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3513,23 +3573,23 @@
         <v>110</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D111" s="0" t="s">
         <v>136</v>
       </c>
       <c r="F111" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="G111" s="0" t="s">
         <v>254</v>
       </c>
-      <c r="G111" s="0" t="s">
-        <v>253</v>
-      </c>
-      <c r="H111" s="1" t="n">
-        <v>10000101</v>
+      <c r="H111" s="1" t="s">
+        <v>256</v>
       </c>
       <c r="I111" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H111),2)</f>
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="J111" s="0" t="s">
         <v>123</v>
@@ -3538,7 +3598,7 @@
         <v>124</v>
       </c>
       <c r="L111" s="0" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="112" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3546,29 +3606,29 @@
         <v>111</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D112" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F112" s="6" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="G112" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="H112" s="7" t="n">
-        <v>10000111</v>
+        <v>258</v>
+      </c>
+      <c r="H112" s="7" t="s">
+        <v>260</v>
       </c>
       <c r="I112" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H112),2)</f>
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="L112" s="6" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3576,23 +3636,23 @@
         <v>112</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="D113" s="0" t="s">
         <v>136</v>
       </c>
       <c r="F113" s="0" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="G113" s="0" t="s">
-        <v>259</v>
-      </c>
-      <c r="H113" s="1" t="n">
-        <v>10001001</v>
+        <v>262</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>264</v>
       </c>
       <c r="I113" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H113),2)</f>
-        <v>89</v>
+        <v>7B</v>
       </c>
       <c r="J113" s="0" t="s">
         <v>123</v>
@@ -3601,7 +3661,7 @@
         <v>124</v>
       </c>
       <c r="L113" s="0" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="114" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3609,29 +3669,29 @@
         <v>113</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="D114" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F114" s="6" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="G114" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="H114" s="7" t="n">
-        <v>10001011</v>
+        <v>266</v>
+      </c>
+      <c r="H114" s="7" t="s">
+        <v>268</v>
       </c>
       <c r="I114" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H114),2)</f>
-        <v>8B</v>
+        <v>7D</v>
       </c>
       <c r="L114" s="6" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3639,23 +3699,23 @@
         <v>114</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="D115" s="0" t="s">
         <v>136</v>
       </c>
       <c r="F115" s="0" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="G115" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="H115" s="1" t="n">
-        <v>10010001</v>
+        <v>270</v>
+      </c>
+      <c r="H115" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="I115" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H115),2)</f>
-        <v>91</v>
+        <v>7F</v>
       </c>
       <c r="J115" s="0" t="s">
         <v>123</v>
@@ -3664,7 +3724,7 @@
         <v>124</v>
       </c>
       <c r="L115" s="0" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
     </row>
     <row r="116" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3672,29 +3732,29 @@
         <v>115</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="D116" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F116" s="6" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="G116" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="H116" s="7" t="n">
-        <v>10010101</v>
+        <v>274</v>
+      </c>
+      <c r="H116" s="7" t="s">
+        <v>276</v>
       </c>
       <c r="I116" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H116),2)</f>
-        <v>95</v>
+        <v>8F</v>
       </c>
       <c r="L116" s="6" t="s">
-        <v>270</v>
+        <v>277</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3702,23 +3762,23 @@
         <v>116</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="D117" s="0" t="s">
         <v>136</v>
       </c>
       <c r="F117" s="0" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="G117" s="0" t="s">
-        <v>271</v>
-      </c>
-      <c r="H117" s="1" t="n">
-        <v>10010111</v>
+        <v>278</v>
+      </c>
+      <c r="H117" s="1" t="s">
+        <v>280</v>
       </c>
       <c r="I117" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H117),2)</f>
-        <v>97</v>
+        <v>9F</v>
       </c>
       <c r="J117" s="0" t="s">
         <v>123</v>
@@ -3727,7 +3787,7 @@
         <v>124</v>
       </c>
       <c r="L117" s="0" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
     </row>
     <row r="118" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3735,29 +3795,29 @@
         <v>117</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="D118" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F118" s="6" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="G118" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="H118" s="7" t="n">
-        <v>10011001</v>
+        <v>282</v>
+      </c>
+      <c r="H118" s="7" t="s">
+        <v>284</v>
       </c>
       <c r="I118" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H118),2)</f>
-        <v>99</v>
+        <v>AF</v>
       </c>
       <c r="L118" s="6" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3765,23 +3825,23 @@
         <v>118</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
       <c r="D119" s="0" t="s">
         <v>136</v>
       </c>
       <c r="F119" s="0" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
       <c r="G119" s="0" t="s">
-        <v>277</v>
-      </c>
-      <c r="H119" s="1" t="n">
-        <v>10011011</v>
+        <v>286</v>
+      </c>
+      <c r="H119" s="1" t="s">
+        <v>288</v>
       </c>
       <c r="I119" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H119),2)</f>
-        <v>9B</v>
+        <v>BF</v>
       </c>
       <c r="J119" s="0" t="s">
         <v>123</v>
@@ -3790,7 +3850,7 @@
         <v>124</v>
       </c>
       <c r="L119" s="0" t="s">
-        <v>279</v>
+        <v>289</v>
       </c>
     </row>
     <row r="120" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3798,29 +3858,29 @@
         <v>119</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>280</v>
+        <v>290</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>281</v>
+        <v>291</v>
       </c>
       <c r="D120" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F120" s="6" t="s">
-        <v>280</v>
+        <v>290</v>
       </c>
       <c r="G120" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H120" s="7" t="n">
-        <v>10100001</v>
+        <v>290</v>
+      </c>
+      <c r="H120" s="7" t="s">
+        <v>292</v>
       </c>
       <c r="I120" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H120),2)</f>
-        <v>A1</v>
+        <v>C1</v>
       </c>
       <c r="L120" s="6" t="s">
-        <v>282</v>
+        <v>293</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3828,23 +3888,23 @@
         <v>120</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>283</v>
+        <v>294</v>
       </c>
       <c r="D121" s="0" t="s">
         <v>136</v>
       </c>
       <c r="F121" s="0" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
       <c r="G121" s="0" t="s">
-        <v>283</v>
-      </c>
-      <c r="H121" s="1" t="n">
-        <v>10100011</v>
+        <v>294</v>
+      </c>
+      <c r="H121" s="1" t="s">
+        <v>296</v>
       </c>
       <c r="I121" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H121),2)</f>
-        <v>A3</v>
+        <v>C3</v>
       </c>
       <c r="J121" s="0" t="s">
         <v>123</v>
@@ -3853,7 +3913,7 @@
         <v>124</v>
       </c>
       <c r="L121" s="0" t="s">
-        <v>285</v>
+        <v>297</v>
       </c>
     </row>
     <row r="122" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3861,29 +3921,29 @@
         <v>121</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>286</v>
+        <v>298</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>287</v>
+        <v>299</v>
       </c>
       <c r="D122" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F122" s="6" t="s">
-        <v>286</v>
+        <v>298</v>
       </c>
       <c r="G122" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="H122" s="7" t="n">
-        <v>10100111</v>
+        <v>298</v>
+      </c>
+      <c r="H122" s="7" t="s">
+        <v>300</v>
       </c>
       <c r="I122" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H122),2)</f>
-        <v>A7</v>
+        <v>C5</v>
       </c>
       <c r="L122" s="6" t="s">
-        <v>288</v>
+        <v>301</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3891,23 +3951,23 @@
         <v>122</v>
       </c>
       <c r="B123" s="0" t="s">
-        <v>289</v>
+        <v>302</v>
       </c>
       <c r="D123" s="0" t="s">
         <v>136</v>
       </c>
       <c r="F123" s="0" t="s">
-        <v>290</v>
+        <v>303</v>
       </c>
       <c r="G123" s="0" t="s">
-        <v>289</v>
-      </c>
-      <c r="H123" s="1" t="n">
-        <v>10101001</v>
+        <v>302</v>
+      </c>
+      <c r="H123" s="1" t="s">
+        <v>304</v>
       </c>
       <c r="I123" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H123),2)</f>
-        <v>A9</v>
+        <v>C7</v>
       </c>
       <c r="J123" s="0" t="s">
         <v>123</v>
@@ -3916,7 +3976,7 @@
         <v>124</v>
       </c>
       <c r="L123" s="0" t="s">
-        <v>291</v>
+        <v>305</v>
       </c>
     </row>
     <row r="124" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3924,29 +3984,29 @@
         <v>123</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>292</v>
+        <v>306</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>293</v>
+        <v>307</v>
       </c>
       <c r="D124" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F124" s="6" t="s">
-        <v>292</v>
+        <v>306</v>
       </c>
       <c r="G124" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="H124" s="7" t="n">
-        <v>10101011</v>
+        <v>306</v>
+      </c>
+      <c r="H124" s="7" t="s">
+        <v>308</v>
       </c>
       <c r="I124" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H124),2)</f>
-        <v>AB</v>
+        <v>CB</v>
       </c>
       <c r="L124" s="6" t="s">
-        <v>294</v>
+        <v>309</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3954,23 +4014,23 @@
         <v>124</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>295</v>
+        <v>310</v>
       </c>
       <c r="D125" s="0" t="s">
         <v>136</v>
       </c>
       <c r="F125" s="0" t="s">
-        <v>296</v>
+        <v>311</v>
       </c>
       <c r="G125" s="0" t="s">
-        <v>295</v>
-      </c>
-      <c r="H125" s="1" t="n">
-        <v>10110001</v>
+        <v>310</v>
+      </c>
+      <c r="H125" s="1" t="s">
+        <v>312</v>
       </c>
       <c r="I125" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H125),2)</f>
-        <v>B1</v>
+        <v>CF</v>
       </c>
       <c r="J125" s="0" t="s">
         <v>123</v>
@@ -3979,7 +4039,7 @@
         <v>124</v>
       </c>
       <c r="L125" s="0" t="s">
-        <v>297</v>
+        <v>313</v>
       </c>
     </row>
     <row r="126" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3987,29 +4047,29 @@
         <v>125</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>298</v>
+        <v>314</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>299</v>
+        <v>315</v>
       </c>
       <c r="D126" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F126" s="6" t="s">
-        <v>298</v>
+        <v>314</v>
       </c>
       <c r="G126" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="H126" s="7" t="n">
-        <v>10110011</v>
+        <v>314</v>
+      </c>
+      <c r="H126" s="7" t="s">
+        <v>316</v>
       </c>
       <c r="I126" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H126),2)</f>
-        <v>B3</v>
+        <v>D1</v>
       </c>
       <c r="L126" s="6" t="s">
-        <v>300</v>
+        <v>317</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4017,23 +4077,23 @@
         <v>126</v>
       </c>
       <c r="B127" s="0" t="s">
-        <v>301</v>
+        <v>318</v>
       </c>
       <c r="D127" s="0" t="s">
         <v>136</v>
       </c>
       <c r="F127" s="0" t="s">
-        <v>302</v>
+        <v>319</v>
       </c>
       <c r="G127" s="0" t="s">
-        <v>301</v>
-      </c>
-      <c r="H127" s="1" t="n">
-        <v>10110101</v>
+        <v>318</v>
+      </c>
+      <c r="H127" s="1" t="s">
+        <v>320</v>
       </c>
       <c r="I127" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H127),2)</f>
-        <v>B5</v>
+        <v>D3</v>
       </c>
       <c r="J127" s="0" t="s">
         <v>123</v>
@@ -4042,7 +4102,7 @@
         <v>124</v>
       </c>
       <c r="L127" s="0" t="s">
-        <v>303</v>
+        <v>321</v>
       </c>
     </row>
     <row r="128" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4050,29 +4110,29 @@
         <v>127</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>304</v>
+        <v>322</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>305</v>
+        <v>323</v>
       </c>
       <c r="D128" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F128" s="6" t="s">
-        <v>304</v>
+        <v>322</v>
       </c>
       <c r="G128" s="6" t="s">
-        <v>304</v>
-      </c>
-      <c r="H128" s="7" t="n">
-        <v>10111001</v>
+        <v>322</v>
+      </c>
+      <c r="H128" s="7" t="s">
+        <v>324</v>
       </c>
       <c r="I128" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H128),2)</f>
-        <v>B9</v>
+        <v>D5</v>
       </c>
       <c r="L128" s="6" t="s">
-        <v>306</v>
+        <v>325</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4080,23 +4140,23 @@
         <v>128</v>
       </c>
       <c r="B129" s="0" t="s">
-        <v>307</v>
+        <v>326</v>
       </c>
       <c r="D129" s="0" t="s">
         <v>136</v>
       </c>
       <c r="F129" s="0" t="s">
-        <v>308</v>
+        <v>327</v>
       </c>
       <c r="G129" s="0" t="s">
-        <v>307</v>
-      </c>
-      <c r="H129" s="1" t="n">
-        <v>10111011</v>
+        <v>326</v>
+      </c>
+      <c r="H129" s="1" t="s">
+        <v>328</v>
       </c>
       <c r="I129" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H129),2)</f>
-        <v>BB</v>
+        <v>D7</v>
       </c>
       <c r="J129" s="0" t="s">
         <v>123</v>
@@ -4105,7 +4165,7 @@
         <v>124</v>
       </c>
       <c r="L129" s="0" t="s">
-        <v>309</v>
+        <v>329</v>
       </c>
     </row>
     <row r="130" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4113,26 +4173,26 @@
         <v>129</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>310</v>
+        <v>330</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>311</v>
+        <v>331</v>
       </c>
       <c r="F130" s="6" t="s">
-        <v>310</v>
+        <v>330</v>
       </c>
       <c r="G130" s="6" t="s">
-        <v>310</v>
+        <v>330</v>
       </c>
       <c r="H130" s="7" t="s">
-        <v>312</v>
+        <v>332</v>
       </c>
       <c r="I130" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H130),2)</f>
         <v>05</v>
       </c>
       <c r="L130" s="6" t="s">
-        <v>313</v>
+        <v>333</v>
       </c>
     </row>
     <row r="131" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4140,26 +4200,26 @@
         <v>130</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>314</v>
+        <v>334</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>315</v>
+        <v>335</v>
       </c>
       <c r="F131" s="6" t="s">
-        <v>314</v>
+        <v>334</v>
       </c>
       <c r="G131" s="6" t="s">
-        <v>314</v>
+        <v>334</v>
       </c>
       <c r="H131" s="7" t="s">
-        <v>316</v>
+        <v>336</v>
       </c>
       <c r="I131" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H131),2)</f>
         <v>0F</v>
       </c>
       <c r="L131" s="6" t="s">
-        <v>317</v>
+        <v>337</v>
       </c>
     </row>
     <row r="132" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4167,26 +4227,26 @@
         <v>131</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>318</v>
+        <v>338</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>319</v>
+        <v>339</v>
       </c>
       <c r="F132" s="6" t="s">
-        <v>318</v>
+        <v>338</v>
       </c>
       <c r="G132" s="6" t="s">
-        <v>318</v>
+        <v>338</v>
       </c>
       <c r="H132" s="7" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="I132" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H132),2)</f>
         <v>11</v>
       </c>
       <c r="L132" s="6" t="s">
-        <v>321</v>
+        <v>341</v>
       </c>
     </row>
     <row r="133" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4194,26 +4254,26 @@
         <v>132</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>323</v>
+        <v>343</v>
       </c>
       <c r="F133" s="6" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="G133" s="6" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="H133" s="7" t="s">
-        <v>324</v>
+        <v>344</v>
       </c>
       <c r="I133" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H133),2)</f>
         <v>15</v>
       </c>
       <c r="L133" s="6" t="s">
-        <v>325</v>
+        <v>345</v>
       </c>
     </row>
     <row r="134" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4221,26 +4281,26 @@
         <v>133</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>326</v>
+        <v>346</v>
       </c>
       <c r="C134" s="6" t="s">
-        <v>327</v>
+        <v>347</v>
       </c>
       <c r="F134" s="6" t="s">
-        <v>326</v>
+        <v>346</v>
       </c>
       <c r="G134" s="6" t="s">
-        <v>326</v>
+        <v>346</v>
       </c>
       <c r="H134" s="7" t="s">
-        <v>328</v>
+        <v>348</v>
       </c>
       <c r="I134" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H134),2)</f>
         <v>1F</v>
       </c>
       <c r="L134" s="6" t="s">
-        <v>329</v>
+        <v>349</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6294,7 +6354,7 @@
       </c>
       <c r="B119" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D119,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D119,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>JMP M</v>
       </c>
       <c r="C119" s="2" t="str">
         <f aca="false">DEC2BIN(A119,8)</f>
@@ -6328,7 +6388,7 @@
       </c>
       <c r="B121" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D121,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D121,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>JMP addr</v>
       </c>
       <c r="C121" s="2" t="str">
         <f aca="false">DEC2BIN(A121,8)</f>
@@ -6362,7 +6422,7 @@
       </c>
       <c r="B123" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D123,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D123,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>JC M</v>
       </c>
       <c r="C123" s="2" t="str">
         <f aca="false">DEC2BIN(A123,8)</f>
@@ -6396,7 +6456,7 @@
       </c>
       <c r="B125" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D125,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D125,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>JC addr</v>
       </c>
       <c r="C125" s="2" t="str">
         <f aca="false">DEC2BIN(A125,8)</f>
@@ -6430,7 +6490,7 @@
       </c>
       <c r="B127" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D127,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D127,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>JNC M</v>
       </c>
       <c r="C127" s="2" t="str">
         <f aca="false">DEC2BIN(A127,8)</f>
@@ -6464,7 +6524,7 @@
       </c>
       <c r="B129" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D129,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D129,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>JNC addr</v>
       </c>
       <c r="C129" s="2" t="str">
         <f aca="false">DEC2BIN(A129,8)</f>
@@ -6532,7 +6592,7 @@
       </c>
       <c r="B133" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D133,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D133,'Instruction Set'!I:I,0)))</f>
-        <v>JMP M</v>
+        <v/>
       </c>
       <c r="C133" s="2" t="str">
         <f aca="false">DEC2BIN(A133,8)</f>
@@ -6566,7 +6626,7 @@
       </c>
       <c r="B135" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D135,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D135,'Instruction Set'!I:I,0)))</f>
-        <v>JMP addr</v>
+        <v/>
       </c>
       <c r="C135" s="2" t="str">
         <f aca="false">DEC2BIN(A135,8)</f>
@@ -6600,7 +6660,7 @@
       </c>
       <c r="B137" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D137,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D137,'Instruction Set'!I:I,0)))</f>
-        <v>JC M</v>
+        <v/>
       </c>
       <c r="C137" s="2" t="str">
         <f aca="false">DEC2BIN(A137,8)</f>
@@ -6634,7 +6694,7 @@
       </c>
       <c r="B139" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D139,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D139,'Instruction Set'!I:I,0)))</f>
-        <v>JC addr</v>
+        <v/>
       </c>
       <c r="C139" s="2" t="str">
         <f aca="false">DEC2BIN(A139,8)</f>
@@ -6668,7 +6728,7 @@
       </c>
       <c r="B141" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D141,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D141,'Instruction Set'!I:I,0)))</f>
-        <v>JNC M</v>
+        <v/>
       </c>
       <c r="C141" s="2" t="str">
         <f aca="false">DEC2BIN(A141,8)</f>
@@ -6736,7 +6796,7 @@
       </c>
       <c r="B145" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D145,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D145,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>JZ M</v>
       </c>
       <c r="C145" s="2" t="str">
         <f aca="false">DEC2BIN(A145,8)</f>
@@ -6770,7 +6830,7 @@
       </c>
       <c r="B147" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D147,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D147,'Instruction Set'!I:I,0)))</f>
-        <v>JNC addr</v>
+        <v/>
       </c>
       <c r="C147" s="2" t="str">
         <f aca="false">DEC2BIN(A147,8)</f>
@@ -6838,7 +6898,7 @@
       </c>
       <c r="B151" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D151,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D151,'Instruction Set'!I:I,0)))</f>
-        <v>JZ M</v>
+        <v/>
       </c>
       <c r="C151" s="2" t="str">
         <f aca="false">DEC2BIN(A151,8)</f>
@@ -6872,7 +6932,7 @@
       </c>
       <c r="B153" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D153,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D153,'Instruction Set'!I:I,0)))</f>
-        <v>JZ addr</v>
+        <v/>
       </c>
       <c r="C153" s="2" t="str">
         <f aca="false">DEC2BIN(A153,8)</f>
@@ -6906,7 +6966,7 @@
       </c>
       <c r="B155" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D155,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D155,'Instruction Set'!I:I,0)))</f>
-        <v>JNZ M</v>
+        <v/>
       </c>
       <c r="C155" s="2" t="str">
         <f aca="false">DEC2BIN(A155,8)</f>
@@ -6940,7 +7000,7 @@
       </c>
       <c r="B157" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D157,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D157,'Instruction Set'!I:I,0)))</f>
-        <v>JNZ addr</v>
+        <v/>
       </c>
       <c r="C157" s="2" t="str">
         <f aca="false">DEC2BIN(A157,8)</f>
@@ -7008,7 +7068,7 @@
       </c>
       <c r="B161" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D161,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D161,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>JZ addr</v>
       </c>
       <c r="C161" s="2" t="str">
         <f aca="false">DEC2BIN(A161,8)</f>
@@ -7042,7 +7102,7 @@
       </c>
       <c r="B163" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D163,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D163,'Instruction Set'!I:I,0)))</f>
-        <v>CALL M</v>
+        <v/>
       </c>
       <c r="C163" s="2" t="str">
         <f aca="false">DEC2BIN(A163,8)</f>
@@ -7076,7 +7136,7 @@
       </c>
       <c r="B165" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D165,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D165,'Instruction Set'!I:I,0)))</f>
-        <v>CALL addr</v>
+        <v/>
       </c>
       <c r="C165" s="2" t="str">
         <f aca="false">DEC2BIN(A165,8)</f>
@@ -7144,7 +7204,7 @@
       </c>
       <c r="B169" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D169,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D169,'Instruction Set'!I:I,0)))</f>
-        <v>CC M</v>
+        <v/>
       </c>
       <c r="C169" s="2" t="str">
         <f aca="false">DEC2BIN(A169,8)</f>
@@ -7178,7 +7238,7 @@
       </c>
       <c r="B171" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D171,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D171,'Instruction Set'!I:I,0)))</f>
-        <v>CC addr</v>
+        <v/>
       </c>
       <c r="C171" s="2" t="str">
         <f aca="false">DEC2BIN(A171,8)</f>
@@ -7212,7 +7272,7 @@
       </c>
       <c r="B173" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D173,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D173,'Instruction Set'!I:I,0)))</f>
-        <v>CNC M</v>
+        <v/>
       </c>
       <c r="C173" s="2" t="str">
         <f aca="false">DEC2BIN(A173,8)</f>
@@ -7280,7 +7340,7 @@
       </c>
       <c r="B177" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D177,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D177,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>JNZ M</v>
       </c>
       <c r="C177" s="2" t="str">
         <f aca="false">DEC2BIN(A177,8)</f>
@@ -7314,7 +7374,7 @@
       </c>
       <c r="B179" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D179,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D179,'Instruction Set'!I:I,0)))</f>
-        <v>CNC addr</v>
+        <v/>
       </c>
       <c r="C179" s="2" t="str">
         <f aca="false">DEC2BIN(A179,8)</f>
@@ -7348,7 +7408,7 @@
       </c>
       <c r="B181" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D181,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D181,'Instruction Set'!I:I,0)))</f>
-        <v>CZ M</v>
+        <v/>
       </c>
       <c r="C181" s="2" t="str">
         <f aca="false">DEC2BIN(A181,8)</f>
@@ -7382,7 +7442,7 @@
       </c>
       <c r="B183" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D183,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D183,'Instruction Set'!I:I,0)))</f>
-        <v>CZ addr</v>
+        <v/>
       </c>
       <c r="C183" s="2" t="str">
         <f aca="false">DEC2BIN(A183,8)</f>
@@ -7450,7 +7510,7 @@
       </c>
       <c r="B187" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D187,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D187,'Instruction Set'!I:I,0)))</f>
-        <v>CNZ M</v>
+        <v/>
       </c>
       <c r="C187" s="2" t="str">
         <f aca="false">DEC2BIN(A187,8)</f>
@@ -7484,7 +7544,7 @@
       </c>
       <c r="B189" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D189,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D189,'Instruction Set'!I:I,0)))</f>
-        <v>CNZ addr</v>
+        <v/>
       </c>
       <c r="C189" s="2" t="str">
         <f aca="false">DEC2BIN(A189,8)</f>
@@ -7552,7 +7612,7 @@
       </c>
       <c r="B193" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D193,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D193,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>JNZ addr</v>
       </c>
       <c r="C193" s="2" t="str">
         <f aca="false">DEC2BIN(A193,8)</f>
@@ -7586,7 +7646,7 @@
       </c>
       <c r="B195" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D195,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D195,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>CALL M</v>
       </c>
       <c r="C195" s="2" t="str">
         <f aca="false">DEC2BIN(A195,8)</f>
@@ -7620,7 +7680,7 @@
       </c>
       <c r="B197" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D197,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D197,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>CALL addr</v>
       </c>
       <c r="C197" s="2" t="str">
         <f aca="false">DEC2BIN(A197,8)</f>
@@ -7654,7 +7714,7 @@
       </c>
       <c r="B199" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D199,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D199,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>CC M</v>
       </c>
       <c r="C199" s="2" t="str">
         <f aca="false">DEC2BIN(A199,8)</f>
@@ -7688,7 +7748,7 @@
       </c>
       <c r="B201" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D201,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D201,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>CC addr</v>
       </c>
       <c r="C201" s="2" t="str">
         <f aca="false">DEC2BIN(A201,8)</f>
@@ -7756,7 +7816,7 @@
       </c>
       <c r="B205" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D205,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D205,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>CNC M</v>
       </c>
       <c r="C205" s="2" t="str">
         <f aca="false">DEC2BIN(A205,8)</f>
@@ -7824,7 +7884,7 @@
       </c>
       <c r="B209" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D209,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D209,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>CNC addr</v>
       </c>
       <c r="C209" s="2" t="str">
         <f aca="false">DEC2BIN(A209,8)</f>
@@ -7858,7 +7918,7 @@
       </c>
       <c r="B211" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D211,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D211,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>CZ M</v>
       </c>
       <c r="C211" s="2" t="str">
         <f aca="false">DEC2BIN(A211,8)</f>
@@ -7892,7 +7952,7 @@
       </c>
       <c r="B213" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D213,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D213,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>CZ addr</v>
       </c>
       <c r="C213" s="2" t="str">
         <f aca="false">DEC2BIN(A213,8)</f>
@@ -7926,7 +7986,7 @@
       </c>
       <c r="B215" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D215,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D215,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>CNZ M</v>
       </c>
       <c r="C215" s="2" t="str">
         <f aca="false">DEC2BIN(A215,8)</f>
@@ -7960,7 +8020,7 @@
       </c>
       <c r="B217" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D217,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D217,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>CNZ addr</v>
       </c>
       <c r="C217" s="2" t="str">
         <f aca="false">DEC2BIN(A217,8)</f>

</xml_diff>

<commit_message>
bit schemas for jumps and calls
</commit_message>
<xml_diff>
--- a/doc/instruction-set.xlsx
+++ b/doc/instruction-set.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="360">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -788,6 +788,9 @@
     <t xml:space="preserve">JMP addr</t>
   </si>
   <si>
+    <t xml:space="preserve">011101&lt;x&gt;1</t>
+  </si>
+  <si>
     <t xml:space="preserve">JMP FFF0h</t>
   </si>
   <si>
@@ -812,6 +815,9 @@
     <t xml:space="preserve">JC addr</t>
   </si>
   <si>
+    <t xml:space="preserve">011110&lt;x&gt;1</t>
+  </si>
+  <si>
     <t xml:space="preserve">JC FFF0h</t>
   </si>
   <si>
@@ -836,6 +842,9 @@
     <t xml:space="preserve">JNC addr</t>
   </si>
   <si>
+    <t xml:space="preserve">011111&lt;x&gt;1</t>
+  </si>
+  <si>
     <t xml:space="preserve">JNC FFF0h</t>
   </si>
   <si>
@@ -860,6 +869,9 @@
     <t xml:space="preserve">JZ addr</t>
   </si>
   <si>
+    <t xml:space="preserve">100&lt;x&gt;1111</t>
+  </si>
+  <si>
     <t xml:space="preserve">JZ FFF0h</t>
   </si>
   <si>
@@ -884,6 +896,9 @@
     <t xml:space="preserve">JNZ addr</t>
   </si>
   <si>
+    <t xml:space="preserve">101&lt;x&gt;1111</t>
+  </si>
+  <si>
     <t xml:space="preserve">JNZ FFF0h</t>
   </si>
   <si>
@@ -908,6 +923,9 @@
     <t xml:space="preserve">CALL addr</t>
   </si>
   <si>
+    <t xml:space="preserve">110000&lt;x&gt;1</t>
+  </si>
+  <si>
     <t xml:space="preserve">CALL FFF0h</t>
   </si>
   <si>
@@ -932,6 +950,9 @@
     <t xml:space="preserve">CC addr</t>
   </si>
   <si>
+    <t xml:space="preserve">110001&lt;x&gt;1</t>
+  </si>
+  <si>
     <t xml:space="preserve">CC FFF0h</t>
   </si>
   <si>
@@ -956,6 +977,9 @@
     <t xml:space="preserve">CNC addr</t>
   </si>
   <si>
+    <t xml:space="preserve">11001&lt;x&gt;11</t>
+  </si>
+  <si>
     <t xml:space="preserve">CNC FFF0h</t>
   </si>
   <si>
@@ -980,6 +1004,9 @@
     <t xml:space="preserve">CZ addr</t>
   </si>
   <si>
+    <t xml:space="preserve">110100&lt;x&gt;1</t>
+  </si>
+  <si>
     <t xml:space="preserve">CZ FFF0h</t>
   </si>
   <si>
@@ -1002,6 +1029,9 @@
   </si>
   <si>
     <t xml:space="preserve">CNZ addr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">110101&lt;x&gt;1</t>
   </si>
   <si>
     <t xml:space="preserve">CNZ FFF0h</t>
@@ -3575,17 +3605,20 @@
       <c r="B111" s="0" t="s">
         <v>254</v>
       </c>
+      <c r="C111" s="9" t="s">
+        <v>255</v>
+      </c>
       <c r="D111" s="0" t="s">
         <v>136</v>
       </c>
       <c r="F111" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="G111" s="0" t="s">
         <v>254</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="I111" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H111),2)</f>
@@ -3598,7 +3631,7 @@
         <v>124</v>
       </c>
       <c r="L111" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="112" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3606,29 +3639,29 @@
         <v>111</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D112" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F112" s="6" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="G112" s="6" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="H112" s="7" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="I112" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H112),2)</f>
         <v>79</v>
       </c>
       <c r="L112" s="6" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3636,19 +3669,22 @@
         <v>112</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
+      </c>
+      <c r="C113" s="9" t="s">
+        <v>264</v>
       </c>
       <c r="D113" s="0" t="s">
         <v>136</v>
       </c>
       <c r="F113" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="G113" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="G113" s="0" t="s">
-        <v>262</v>
-      </c>
       <c r="H113" s="1" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="I113" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H113),2)</f>
@@ -3661,7 +3697,7 @@
         <v>124</v>
       </c>
       <c r="L113" s="0" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="114" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3669,29 +3705,29 @@
         <v>113</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="D114" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F114" s="6" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="G114" s="6" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="H114" s="7" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="I114" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H114),2)</f>
         <v>7D</v>
       </c>
       <c r="L114" s="6" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3699,19 +3735,22 @@
         <v>114</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>270</v>
+        <v>272</v>
+      </c>
+      <c r="C115" s="9" t="s">
+        <v>273</v>
       </c>
       <c r="D115" s="0" t="s">
         <v>136</v>
       </c>
       <c r="F115" s="0" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="G115" s="0" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="H115" s="1" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="I115" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H115),2)</f>
@@ -3724,7 +3763,7 @@
         <v>124</v>
       </c>
       <c r="L115" s="0" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="116" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3732,29 +3771,29 @@
         <v>115</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="D116" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F116" s="6" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="G116" s="6" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="H116" s="7" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="I116" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H116),2)</f>
         <v>8F</v>
       </c>
       <c r="L116" s="6" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3762,19 +3801,22 @@
         <v>116</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>278</v>
+        <v>281</v>
+      </c>
+      <c r="C117" s="9" t="s">
+        <v>282</v>
       </c>
       <c r="D117" s="0" t="s">
         <v>136</v>
       </c>
       <c r="F117" s="0" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="G117" s="0" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="H117" s="1" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="I117" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H117),2)</f>
@@ -3787,7 +3829,7 @@
         <v>124</v>
       </c>
       <c r="L117" s="0" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
     </row>
     <row r="118" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3795,29 +3837,29 @@
         <v>117</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="D118" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F118" s="6" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="G118" s="6" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="H118" s="7" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="I118" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H118),2)</f>
         <v>AF</v>
       </c>
       <c r="L118" s="6" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3825,19 +3867,22 @@
         <v>118</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>286</v>
+        <v>290</v>
+      </c>
+      <c r="C119" s="9" t="s">
+        <v>291</v>
       </c>
       <c r="D119" s="0" t="s">
         <v>136</v>
       </c>
       <c r="F119" s="0" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="G119" s="0" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="H119" s="1" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="I119" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H119),2)</f>
@@ -3850,7 +3895,7 @@
         <v>124</v>
       </c>
       <c r="L119" s="0" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
     </row>
     <row r="120" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3858,29 +3903,29 @@
         <v>119</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="D120" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F120" s="6" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="G120" s="6" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="H120" s="7" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="I120" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H120),2)</f>
         <v>C1</v>
       </c>
       <c r="L120" s="6" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3888,19 +3933,22 @@
         <v>120</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>294</v>
+        <v>299</v>
+      </c>
+      <c r="C121" s="9" t="s">
+        <v>300</v>
       </c>
       <c r="D121" s="0" t="s">
         <v>136</v>
       </c>
       <c r="F121" s="0" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="G121" s="0" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="H121" s="1" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="I121" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H121),2)</f>
@@ -3913,7 +3961,7 @@
         <v>124</v>
       </c>
       <c r="L121" s="0" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
     </row>
     <row r="122" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3921,29 +3969,29 @@
         <v>121</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="D122" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F122" s="6" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="G122" s="6" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="H122" s="7" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="I122" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H122),2)</f>
         <v>C5</v>
       </c>
       <c r="L122" s="6" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3951,19 +3999,22 @@
         <v>122</v>
       </c>
       <c r="B123" s="0" t="s">
-        <v>302</v>
+        <v>308</v>
+      </c>
+      <c r="C123" s="9" t="s">
+        <v>309</v>
       </c>
       <c r="D123" s="0" t="s">
         <v>136</v>
       </c>
       <c r="F123" s="0" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="G123" s="0" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="H123" s="1" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="I123" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H123),2)</f>
@@ -3976,7 +4027,7 @@
         <v>124</v>
       </c>
       <c r="L123" s="0" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
     </row>
     <row r="124" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3984,29 +4035,29 @@
         <v>123</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="D124" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F124" s="6" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="G124" s="6" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="H124" s="7" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="I124" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H124),2)</f>
         <v>CB</v>
       </c>
       <c r="L124" s="6" t="s">
-        <v>309</v>
+        <v>316</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4014,19 +4065,22 @@
         <v>124</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>310</v>
+        <v>317</v>
+      </c>
+      <c r="C125" s="9" t="s">
+        <v>318</v>
       </c>
       <c r="D125" s="0" t="s">
         <v>136</v>
       </c>
       <c r="F125" s="0" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="G125" s="0" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
       <c r="H125" s="1" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="I125" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H125),2)</f>
@@ -4039,7 +4093,7 @@
         <v>124</v>
       </c>
       <c r="L125" s="0" t="s">
-        <v>313</v>
+        <v>321</v>
       </c>
     </row>
     <row r="126" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4047,29 +4101,29 @@
         <v>125</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="D126" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F126" s="6" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="G126" s="6" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="H126" s="7" t="s">
-        <v>316</v>
+        <v>324</v>
       </c>
       <c r="I126" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H126),2)</f>
         <v>D1</v>
       </c>
       <c r="L126" s="6" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4077,19 +4131,22 @@
         <v>126</v>
       </c>
       <c r="B127" s="0" t="s">
-        <v>318</v>
+        <v>326</v>
+      </c>
+      <c r="C127" s="9" t="s">
+        <v>327</v>
       </c>
       <c r="D127" s="0" t="s">
         <v>136</v>
       </c>
       <c r="F127" s="0" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="G127" s="0" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="H127" s="1" t="s">
-        <v>320</v>
+        <v>329</v>
       </c>
       <c r="I127" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H127),2)</f>
@@ -4102,7 +4159,7 @@
         <v>124</v>
       </c>
       <c r="L127" s="0" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
     </row>
     <row r="128" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4110,29 +4167,29 @@
         <v>127</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
       <c r="D128" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F128" s="6" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
       <c r="G128" s="6" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
       <c r="H128" s="7" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="I128" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H128),2)</f>
         <v>D5</v>
       </c>
       <c r="L128" s="6" t="s">
-        <v>325</v>
+        <v>334</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4140,19 +4197,22 @@
         <v>128</v>
       </c>
       <c r="B129" s="0" t="s">
-        <v>326</v>
+        <v>335</v>
+      </c>
+      <c r="C129" s="9" t="s">
+        <v>336</v>
       </c>
       <c r="D129" s="0" t="s">
         <v>136</v>
       </c>
       <c r="F129" s="0" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="G129" s="0" t="s">
-        <v>326</v>
+        <v>335</v>
       </c>
       <c r="H129" s="1" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="I129" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H129),2)</f>
@@ -4165,7 +4225,7 @@
         <v>124</v>
       </c>
       <c r="L129" s="0" t="s">
-        <v>329</v>
+        <v>339</v>
       </c>
     </row>
     <row r="130" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4173,26 +4233,26 @@
         <v>129</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>331</v>
+        <v>341</v>
       </c>
       <c r="F130" s="6" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="G130" s="6" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="H130" s="7" t="s">
-        <v>332</v>
+        <v>342</v>
       </c>
       <c r="I130" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H130),2)</f>
         <v>05</v>
       </c>
       <c r="L130" s="6" t="s">
-        <v>333</v>
+        <v>343</v>
       </c>
     </row>
     <row r="131" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4200,26 +4260,26 @@
         <v>130</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>335</v>
+        <v>345</v>
       </c>
       <c r="F131" s="6" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="G131" s="6" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="H131" s="7" t="s">
-        <v>336</v>
+        <v>346</v>
       </c>
       <c r="I131" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H131),2)</f>
         <v>0F</v>
       </c>
       <c r="L131" s="6" t="s">
-        <v>337</v>
+        <v>347</v>
       </c>
     </row>
     <row r="132" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4227,26 +4287,26 @@
         <v>131</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>339</v>
+        <v>349</v>
       </c>
       <c r="F132" s="6" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="G132" s="6" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="H132" s="7" t="s">
-        <v>340</v>
+        <v>350</v>
       </c>
       <c r="I132" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H132),2)</f>
         <v>11</v>
       </c>
       <c r="L132" s="6" t="s">
-        <v>341</v>
+        <v>351</v>
       </c>
     </row>
     <row r="133" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4254,26 +4314,26 @@
         <v>132</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>343</v>
+        <v>353</v>
       </c>
       <c r="F133" s="6" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="G133" s="6" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="H133" s="7" t="s">
-        <v>344</v>
+        <v>354</v>
       </c>
       <c r="I133" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H133),2)</f>
         <v>15</v>
       </c>
       <c r="L133" s="6" t="s">
-        <v>345</v>
+        <v>355</v>
       </c>
     </row>
     <row r="134" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4281,26 +4341,26 @@
         <v>133</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="C134" s="6" t="s">
-        <v>347</v>
+        <v>357</v>
       </c>
       <c r="F134" s="6" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="G134" s="6" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="H134" s="7" t="s">
-        <v>348</v>
+        <v>358</v>
       </c>
       <c r="I134" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H134),2)</f>
         <v>1F</v>
       </c>
       <c r="L134" s="6" t="s">
-        <v>349</v>
+        <v>359</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
MOV address into HL,IP or SP
</commit_message>
<xml_diff>
--- a/doc/instruction-set.xlsx
+++ b/doc/instruction-set.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="364">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -377,13 +377,19 @@
     <t xml:space="preserve">MOV SP,IP</t>
   </si>
   <si>
+    <t xml:space="preserve">111 = addr/data</t>
+  </si>
+  <si>
     <t xml:space="preserve">00100010</t>
   </si>
   <si>
     <t xml:space="preserve">Move value of Instruction Pointer into Stack Pointer</t>
   </si>
   <si>
-    <t xml:space="preserve">MOV HL,data</t>
+    <t xml:space="preserve">MOV HL,addr/data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address/Data</t>
   </si>
   <si>
     <t xml:space="preserve">MOV HL,FFF0h</t>
@@ -392,52 +398,58 @@
     <t xml:space="preserve">00001110</t>
   </si>
   <si>
+    <t xml:space="preserve">Low-order byte of address/data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High-order byte of address/data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move given address/data into H and L registers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV IP,addr/data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV IP,FFF0h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00011110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move given address/data into Instruction Pointer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV SP,addr/data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV SP,FFF0h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00101110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move given address/data into Stack Pointer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LDA rd,addr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load from address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LDA A,FFF0h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LDA A,addr</t>
+  </si>
+  <si>
     <t xml:space="preserve">Low-order byte of address</t>
   </si>
   <si>
     <t xml:space="preserve">High-order byte of address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move given data into H and L registers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV IP,data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV IP,FFF0h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00011110</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move given data into Instruction Pointer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV SP,data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV SP,FFF0h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00101110</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move given data into Stack Pointer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LDA rd,addr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Load from address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LDA A,FFF0h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LDA A,addr</t>
   </si>
   <si>
     <t xml:space="preserve">Load value at given address into destination register</t>
@@ -1358,16 +1370,16 @@
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="12.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="22.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="22.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="26.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="26.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="69.51"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.52"/>
   </cols>
@@ -2474,7 +2486,7 @@
         <v>117</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>46</v>
+        <v>118</v>
       </c>
       <c r="D58" s="0" t="s">
         <v>102</v>
@@ -2489,14 +2501,14 @@
         <v>117</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I58" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H58),2)</f>
         <v>22</v>
       </c>
       <c r="L58" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2504,35 +2516,35 @@
         <v>58</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D59" s="0" t="s">
         <v>97</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="F59" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="G59" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="G59" s="0" t="s">
-        <v>120</v>
-      </c>
       <c r="H59" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="I59" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H59),2)</f>
         <v>0E</v>
       </c>
       <c r="J59" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="K59" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="L59" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2540,35 +2552,35 @@
         <v>59</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D60" s="0" t="s">
         <v>98</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="I60" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H60),2)</f>
         <v>1E</v>
       </c>
       <c r="J60" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="K60" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="L60" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2576,35 +2588,35 @@
         <v>60</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D61" s="0" t="s">
         <v>102</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="I61" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H61),2)</f>
         <v>2E</v>
       </c>
       <c r="J61" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="K61" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="L61" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="62" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2612,22 +2624,22 @@
         <v>61</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>25</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H62" s="7" t="n">
         <v>10001101</v>
@@ -2637,13 +2649,13 @@
         <v>8D</v>
       </c>
       <c r="J62" s="6" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="K62" s="6" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="L62" s="6" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2651,10 +2663,10 @@
         <v>62</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="H63" s="1" t="n">
         <v>10011101</v>
@@ -2669,7 +2681,7 @@
         <v>63</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="H64" s="1" t="n">
         <v>10101101</v>
@@ -2684,7 +2696,7 @@
         <v>64</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="H65" s="1" t="n">
         <v>10111101</v>
@@ -2699,7 +2711,7 @@
         <v>65</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="H66" s="1" t="n">
         <v>11001101</v>
@@ -2714,7 +2726,7 @@
         <v>66</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="H67" s="1" t="n">
         <v>11011101</v>
@@ -2729,22 +2741,22 @@
         <v>67</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E68" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="H68" s="7" t="n">
         <v>11100001</v>
@@ -2754,13 +2766,13 @@
         <v>E1</v>
       </c>
       <c r="J68" s="6" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="K68" s="6" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="L68" s="6" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2768,10 +2780,10 @@
         <v>68</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="G69" s="0" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="H69" s="1" t="n">
         <v>11100011</v>
@@ -2786,7 +2798,7 @@
         <v>69</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="H70" s="1" t="n">
         <v>11100101</v>
@@ -2801,7 +2813,7 @@
         <v>70</v>
       </c>
       <c r="G71" s="0" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="H71" s="1" t="n">
         <v>11100111</v>
@@ -2816,7 +2828,7 @@
         <v>71</v>
       </c>
       <c r="G72" s="0" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="H72" s="1" t="n">
         <v>11101001</v>
@@ -2831,7 +2843,7 @@
         <v>72</v>
       </c>
       <c r="G73" s="0" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="H73" s="1" t="n">
         <v>11101011</v>
@@ -2846,19 +2858,19 @@
         <v>73</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="H74" s="7" t="n">
         <v>10000000</v>
@@ -2868,7 +2880,7 @@
         <v>80</v>
       </c>
       <c r="L74" s="6" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2876,10 +2888,10 @@
         <v>74</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="G75" s="0" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="H75" s="1" t="n">
         <v>10010010</v>
@@ -2894,7 +2906,7 @@
         <v>75</v>
       </c>
       <c r="G76" s="0" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="H76" s="1" t="n">
         <v>10100100</v>
@@ -2909,7 +2921,7 @@
         <v>76</v>
       </c>
       <c r="G77" s="0" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="H77" s="1" t="n">
         <v>10110110</v>
@@ -2924,7 +2936,7 @@
         <v>77</v>
       </c>
       <c r="G78" s="0" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="H78" s="1" t="n">
         <v>11001000</v>
@@ -2939,7 +2951,7 @@
         <v>78</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="H79" s="1" t="n">
         <v>11011010</v>
@@ -2954,19 +2966,19 @@
         <v>79</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="F80" s="6" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="H80" s="7" t="n">
         <v>10000001</v>
@@ -2976,7 +2988,7 @@
         <v>81</v>
       </c>
       <c r="L80" s="6" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2984,10 +2996,10 @@
         <v>80</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="G81" s="0" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="H81" s="1" t="n">
         <v>10010011</v>
@@ -3002,7 +3014,7 @@
         <v>81</v>
       </c>
       <c r="G82" s="0" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="H82" s="1" t="n">
         <v>10100101</v>
@@ -3017,7 +3029,7 @@
         <v>82</v>
       </c>
       <c r="G83" s="0" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="H83" s="1" t="n">
         <v>10110111</v>
@@ -3032,7 +3044,7 @@
         <v>83</v>
       </c>
       <c r="G84" s="0" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="H84" s="1" t="n">
         <v>11001001</v>
@@ -3047,7 +3059,7 @@
         <v>84</v>
       </c>
       <c r="G85" s="0" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="H85" s="1" t="n">
         <v>11011011</v>
@@ -3062,29 +3074,29 @@
         <v>85</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="F86" s="6" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="H86" s="7" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="I86" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H86),2)</f>
         <v>60</v>
       </c>
       <c r="L86" s="6" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3092,13 +3104,13 @@
         <v>86</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="G87" s="0" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="I87" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H87),2)</f>
@@ -3111,10 +3123,10 @@
       </c>
       <c r="C88" s="9"/>
       <c r="G88" s="0" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="I88" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H88),2)</f>
@@ -3126,10 +3138,10 @@
         <v>88</v>
       </c>
       <c r="G89" s="0" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="I89" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H89),2)</f>
@@ -3141,10 +3153,10 @@
         <v>89</v>
       </c>
       <c r="G90" s="0" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="I90" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H90),2)</f>
@@ -3156,10 +3168,10 @@
         <v>90</v>
       </c>
       <c r="G91" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="I91" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H91),2)</f>
@@ -3171,26 +3183,26 @@
         <v>91</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="D92" s="0" t="s">
         <v>68</v>
       </c>
       <c r="F92" s="0" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="G92" s="0" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="I92" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H92),2)</f>
         <v>6C</v>
       </c>
       <c r="L92" s="0" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3198,22 +3210,22 @@
         <v>92</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="D93" s="0" t="s">
         <v>85</v>
       </c>
       <c r="F93" s="0" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="G93" s="0" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="I93" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H93),2)</f>
@@ -3223,7 +3235,7 @@
         <v>88</v>
       </c>
       <c r="L93" s="0" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="94" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3231,29 +3243,29 @@
         <v>93</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="F94" s="6" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="H94" s="7" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="I94" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H94),2)</f>
         <v>61</v>
       </c>
       <c r="L94" s="6" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3261,13 +3273,13 @@
         <v>94</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="G95" s="0" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="I95" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H95),2)</f>
@@ -3280,10 +3292,10 @@
       </c>
       <c r="C96" s="9"/>
       <c r="G96" s="0" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="I96" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H96),2)</f>
@@ -3295,10 +3307,10 @@
         <v>96</v>
       </c>
       <c r="G97" s="0" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I97" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H97),2)</f>
@@ -3310,10 +3322,10 @@
         <v>97</v>
       </c>
       <c r="G98" s="0" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="I98" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H98),2)</f>
@@ -3325,10 +3337,10 @@
         <v>98</v>
       </c>
       <c r="G99" s="0" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="I99" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H99),2)</f>
@@ -3340,26 +3352,26 @@
         <v>99</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="D100" s="0" t="s">
         <v>68</v>
       </c>
       <c r="F100" s="0" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="G100" s="0" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="I100" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H100),2)</f>
         <v>6D</v>
       </c>
       <c r="L100" s="0" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3367,22 +3379,22 @@
         <v>100</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="D101" s="0" t="s">
         <v>85</v>
       </c>
       <c r="F101" s="0" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="G101" s="0" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="I101" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H101),2)</f>
@@ -3392,7 +3404,7 @@
         <v>88</v>
       </c>
       <c r="L101" s="0" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="102" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3400,22 +3412,22 @@
         <v>101</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="C102" s="10" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="F102" s="6" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="G102" s="6" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="H102" s="7" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="I102" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H102),2)</f>
@@ -3427,20 +3439,20 @@
         <v>102</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="G103" s="0" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="I103" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H103),2)</f>
         <v>72</v>
       </c>
       <c r="L103" s="0" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3449,10 +3461,10 @@
       </c>
       <c r="C104" s="11"/>
       <c r="G104" s="0" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="I104" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H104),2)</f>
@@ -3465,10 +3477,10 @@
       </c>
       <c r="C105" s="11"/>
       <c r="G105" s="0" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="I105" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H105),2)</f>
@@ -3481,10 +3493,10 @@
       </c>
       <c r="C106" s="11"/>
       <c r="G106" s="0" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="I106" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H106),2)</f>
@@ -3497,10 +3509,10 @@
       </c>
       <c r="C107" s="11"/>
       <c r="G107" s="0" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="I107" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H107),2)</f>
@@ -3512,27 +3524,27 @@
         <v>107</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="C108" s="11"/>
       <c r="D108" s="0" t="s">
         <v>68</v>
       </c>
       <c r="F108" s="0" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="G108" s="0" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="I108" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H108),2)</f>
         <v>7C</v>
       </c>
       <c r="L108" s="0" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3540,22 +3552,22 @@
         <v>108</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="C109" s="9" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="D109" s="0" t="s">
         <v>85</v>
       </c>
       <c r="F109" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G109" s="0" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="I109" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H109),2)</f>
@@ -3565,7 +3577,7 @@
         <v>88</v>
       </c>
       <c r="L109" s="0" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="110" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3573,29 +3585,29 @@
         <v>109</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="D110" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F110" s="6" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="G110" s="6" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="H110" s="7" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="I110" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H110),2)</f>
         <v>75</v>
       </c>
       <c r="L110" s="6" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3603,35 +3615,35 @@
         <v>110</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="C111" s="9" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F111" s="0" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="G111" s="0" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="I111" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H111),2)</f>
         <v>77</v>
       </c>
       <c r="J111" s="0" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="K111" s="0" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="L111" s="0" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
     </row>
     <row r="112" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3639,29 +3651,29 @@
         <v>111</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="D112" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F112" s="6" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="G112" s="6" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="H112" s="7" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="I112" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H112),2)</f>
         <v>79</v>
       </c>
       <c r="L112" s="6" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3669,35 +3681,35 @@
         <v>112</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="C113" s="9" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F113" s="0" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="G113" s="0" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="I113" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H113),2)</f>
         <v>7B</v>
       </c>
       <c r="J113" s="0" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="K113" s="0" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="L113" s="0" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
     </row>
     <row r="114" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3705,29 +3717,29 @@
         <v>113</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="D114" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F114" s="6" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="G114" s="6" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="H114" s="7" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="I114" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H114),2)</f>
         <v>7D</v>
       </c>
       <c r="L114" s="6" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3735,35 +3747,35 @@
         <v>114</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="C115" s="9" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F115" s="0" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="G115" s="0" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="H115" s="1" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="I115" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H115),2)</f>
         <v>7F</v>
       </c>
       <c r="J115" s="0" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="K115" s="0" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="L115" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="116" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3771,29 +3783,29 @@
         <v>115</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="D116" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F116" s="6" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="G116" s="6" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H116" s="7" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="I116" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H116),2)</f>
         <v>8F</v>
       </c>
       <c r="L116" s="6" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3801,35 +3813,35 @@
         <v>116</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="D117" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F117" s="0" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="G117" s="0" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="H117" s="1" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="I117" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H117),2)</f>
         <v>9F</v>
       </c>
       <c r="J117" s="0" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="K117" s="0" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="L117" s="0" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
     </row>
     <row r="118" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3837,29 +3849,29 @@
         <v>117</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="D118" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F118" s="6" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="G118" s="6" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="H118" s="7" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="I118" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H118),2)</f>
         <v>AF</v>
       </c>
       <c r="L118" s="6" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3867,35 +3879,35 @@
         <v>118</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="C119" s="9" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F119" s="0" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="G119" s="0" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="H119" s="1" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="I119" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H119),2)</f>
         <v>BF</v>
       </c>
       <c r="J119" s="0" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="K119" s="0" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="L119" s="0" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
     </row>
     <row r="120" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3903,29 +3915,29 @@
         <v>119</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="D120" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F120" s="6" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="G120" s="6" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="H120" s="7" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="I120" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H120),2)</f>
         <v>C1</v>
       </c>
       <c r="L120" s="6" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3933,35 +3945,35 @@
         <v>120</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="C121" s="9" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="D121" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F121" s="0" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="G121" s="0" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="H121" s="1" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="I121" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H121),2)</f>
         <v>C3</v>
       </c>
       <c r="J121" s="0" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="K121" s="0" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="L121" s="0" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
     </row>
     <row r="122" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3969,29 +3981,29 @@
         <v>121</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="D122" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F122" s="6" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="G122" s="6" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="H122" s="7" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="I122" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H122),2)</f>
         <v>C5</v>
       </c>
       <c r="L122" s="6" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3999,35 +4011,35 @@
         <v>122</v>
       </c>
       <c r="B123" s="0" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="C123" s="9" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="D123" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F123" s="0" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="G123" s="0" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="H123" s="1" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="I123" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H123),2)</f>
         <v>C7</v>
       </c>
       <c r="J123" s="0" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="K123" s="0" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="L123" s="0" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
     </row>
     <row r="124" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4035,29 +4047,29 @@
         <v>123</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="D124" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F124" s="6" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="G124" s="6" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="H124" s="7" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="I124" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H124),2)</f>
         <v>CB</v>
       </c>
       <c r="L124" s="6" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4065,35 +4077,35 @@
         <v>124</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="C125" s="9" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="D125" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F125" s="0" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="G125" s="0" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="H125" s="1" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="I125" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H125),2)</f>
         <v>CF</v>
       </c>
       <c r="J125" s="0" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="K125" s="0" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="L125" s="0" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
     </row>
     <row r="126" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4101,29 +4113,29 @@
         <v>125</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="D126" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F126" s="6" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="G126" s="6" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="H126" s="7" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="I126" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H126),2)</f>
         <v>D1</v>
       </c>
       <c r="L126" s="6" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4131,35 +4143,35 @@
         <v>126</v>
       </c>
       <c r="B127" s="0" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="C127" s="9" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="D127" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F127" s="0" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="G127" s="0" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="H127" s="1" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="I127" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H127),2)</f>
         <v>D3</v>
       </c>
       <c r="J127" s="0" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="K127" s="0" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="L127" s="0" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
     </row>
     <row r="128" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4167,29 +4179,29 @@
         <v>127</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="D128" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F128" s="6" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="G128" s="6" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="H128" s="7" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="I128" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H128),2)</f>
         <v>D5</v>
       </c>
       <c r="L128" s="6" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4197,35 +4209,35 @@
         <v>128</v>
       </c>
       <c r="B129" s="0" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="C129" s="9" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="D129" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F129" s="0" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="G129" s="0" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="H129" s="1" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="I129" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H129),2)</f>
         <v>D7</v>
       </c>
       <c r="J129" s="0" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="K129" s="0" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="L129" s="0" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
     </row>
     <row r="130" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4233,26 +4245,26 @@
         <v>129</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="F130" s="6" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="G130" s="6" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="H130" s="7" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="I130" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H130),2)</f>
         <v>05</v>
       </c>
       <c r="L130" s="6" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
     </row>
     <row r="131" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4260,26 +4272,26 @@
         <v>130</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="F131" s="6" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="G131" s="6" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="H131" s="7" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="I131" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H131),2)</f>
         <v>0F</v>
       </c>
       <c r="L131" s="6" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
     </row>
     <row r="132" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4287,26 +4299,26 @@
         <v>131</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="F132" s="6" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="G132" s="6" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="H132" s="7" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="I132" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H132),2)</f>
         <v>11</v>
       </c>
       <c r="L132" s="6" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
     </row>
     <row r="133" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4314,26 +4326,26 @@
         <v>132</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="F133" s="6" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="G133" s="6" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="H133" s="7" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="I133" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H133),2)</f>
         <v>15</v>
       </c>
       <c r="L133" s="6" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
     </row>
     <row r="134" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4341,26 +4353,26 @@
         <v>133</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="C134" s="6" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="F134" s="6" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="G134" s="6" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="H134" s="7" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="I134" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H134),2)</f>
         <v>1F</v>
       </c>
       <c r="L134" s="6" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4663,7 +4675,7 @@
       </c>
       <c r="B16" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D16,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D16,'Instruction Set'!I:I,0)))</f>
-        <v>MOV HL,data</v>
+        <v>MOV HL,addr/data</v>
       </c>
       <c r="C16" s="2" t="str">
         <f aca="false">DEC2BIN(A16,8)</f>
@@ -4935,7 +4947,7 @@
       </c>
       <c r="B32" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D32,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D32,'Instruction Set'!I:I,0)))</f>
-        <v>MOV IP,data</v>
+        <v>MOV IP,addr/data</v>
       </c>
       <c r="C32" s="2" t="str">
         <f aca="false">DEC2BIN(A32,8)</f>
@@ -5207,7 +5219,7 @@
       </c>
       <c r="B48" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D48,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D48,'Instruction Set'!I:I,0)))</f>
-        <v>MOV SP,data</v>
+        <v>MOV SP,addr/data</v>
       </c>
       <c r="C48" s="2" t="str">
         <f aca="false">DEC2BIN(A48,8)</f>

</xml_diff>

<commit_message>
prepare ADC and SBB
</commit_message>
<xml_diff>
--- a/doc/instruction-set.xlsx
+++ b/doc/instruction-set.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="410">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -623,7 +623,7 @@
     <t xml:space="preserve">01101100</t>
   </si>
   <si>
-    <t xml:space="preserve">Increment accumulator (A register) by value at memory address in H and L registers </t>
+    <t xml:space="preserve">Increment accumulator (A register) by value at memory address in H and L registers</t>
   </si>
   <si>
     <t xml:space="preserve">ADD data</t>
@@ -713,6 +713,144 @@
     <t xml:space="preserve">Decrement accumulator (A register) by given data</t>
   </si>
   <si>
+    <t xml:space="preserve">ADC r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add with Carry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01010000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increment accumulator (A register) by value of register with carry if set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01010&lt;x&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01010001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01010010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01010011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01010100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01010101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01010110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increment accumulator (A register) by value at memory address in H and L registers with carry if set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC 10h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01010111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increment accumulator (A register) by given data with carry if set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBB r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subtract with Borrow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBB A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01011000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decrement accumulator (A register) by value of register with borrow if set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01011&lt;x&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBB B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01011001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBB C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01011010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBB D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01011011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBB H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01011100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBB L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01011101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBB M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01011110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decrement accumulator (A register) by value at memory address in H and L registers with borrow if set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBB data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBB 10h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01011111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decrement accumulator (A register) by given data with borrow if set</t>
+  </si>
+  <si>
     <t xml:space="preserve">CMP r</t>
   </si>
   <si>
@@ -725,6 +863,9 @@
     <t xml:space="preserve">01110000</t>
   </si>
   <si>
+    <t xml:space="preserve">Compare accumulator (A register) with value of register</t>
+  </si>
+  <si>
     <t xml:space="preserve">0&lt;data&gt;&lt;r&gt;0</t>
   </si>
   <si>
@@ -732,9 +873,6 @@
   </si>
   <si>
     <t xml:space="preserve">01110010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compare accumulator (A register) with value of register</t>
   </si>
   <si>
     <t xml:space="preserve">CMP C</t>
@@ -1119,9 +1257,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -1248,7 +1387,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1359,28 +1498,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:L135"/>
+  <dimension ref="A1:L151"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
+      <selection pane="bottomLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="12.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="26.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="26.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="69.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="82.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -3431,7 +3570,10 @@
       </c>
       <c r="I102" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H102),2)</f>
-        <v>70</v>
+        <v>50</v>
+      </c>
+      <c r="L102" s="6" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3439,20 +3581,17 @@
         <v>102</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G103" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="I103" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H103),2)</f>
-        <v>72</v>
-      </c>
-      <c r="L103" s="0" t="s">
-        <v>237</v>
+        <v>51</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3468,7 +3607,7 @@
       </c>
       <c r="I104" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H104),2)</f>
-        <v>74</v>
+        <v>52</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3484,7 +3623,7 @@
       </c>
       <c r="I105" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H105),2)</f>
-        <v>76</v>
+        <v>53</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3500,7 +3639,7 @@
       </c>
       <c r="I106" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H106),2)</f>
-        <v>78</v>
+        <v>54</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3516,7 +3655,7 @@
       </c>
       <c r="I107" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H107),2)</f>
-        <v>7A</v>
+        <v>55</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3527,9 +3666,6 @@
         <v>246</v>
       </c>
       <c r="C108" s="11"/>
-      <c r="D108" s="0" t="s">
-        <v>68</v>
-      </c>
       <c r="F108" s="0" t="s">
         <v>246</v>
       </c>
@@ -3541,7 +3677,7 @@
       </c>
       <c r="I108" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H108),2)</f>
-        <v>7C</v>
+        <v>56</v>
       </c>
       <c r="L108" s="0" t="s">
         <v>248</v>
@@ -3554,30 +3690,25 @@
       <c r="B109" s="0" t="s">
         <v>249</v>
       </c>
-      <c r="C109" s="9" t="s">
+      <c r="C109" s="11"/>
+      <c r="F109" s="0" t="s">
         <v>250</v>
-      </c>
-      <c r="D109" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="F109" s="0" t="s">
-        <v>251</v>
       </c>
       <c r="G109" s="0" t="s">
         <v>249</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I109" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H109),2)</f>
-        <v>7E</v>
+        <v>57</v>
       </c>
       <c r="J109" s="0" t="s">
         <v>88</v>
       </c>
       <c r="L109" s="0" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="110" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3585,26 +3716,26 @@
         <v>109</v>
       </c>
       <c r="B110" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="C110" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C110" s="6" t="s">
+      <c r="D110" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="F110" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="D110" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F110" s="6" t="s">
-        <v>254</v>
-      </c>
       <c r="G110" s="6" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H110" s="7" t="s">
         <v>256</v>
       </c>
       <c r="I110" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H110),2)</f>
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="L110" s="6" t="s">
         <v>257</v>
@@ -3614,198 +3745,107 @@
       <c r="A111" s="6" t="n">
         <v>110</v>
       </c>
-      <c r="B111" s="0" t="s">
+      <c r="C111" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="C111" s="9" t="s">
+      <c r="G111" s="0" t="s">
         <v>259</v>
       </c>
-      <c r="D111" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="F111" s="0" t="s">
+      <c r="H111" s="1" t="s">
         <v>260</v>
-      </c>
-      <c r="G111" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="H111" s="1" t="s">
-        <v>261</v>
       </c>
       <c r="I111" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H111),2)</f>
-        <v>77</v>
-      </c>
-      <c r="J111" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="K111" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="L111" s="0" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="112" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="6" t="n">
         <v>111</v>
       </c>
-      <c r="B112" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="C112" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="D112" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F112" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="G112" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="H112" s="7" t="s">
-        <v>265</v>
+      <c r="C112" s="11"/>
+      <c r="G112" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="H112" s="1" t="s">
+        <v>262</v>
       </c>
       <c r="I112" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H112),2)</f>
-        <v>79</v>
-      </c>
-      <c r="L112" s="6" t="s">
-        <v>266</v>
+        <v>5A</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="6" t="n">
         <v>112</v>
       </c>
-      <c r="B113" s="0" t="s">
-        <v>267</v>
-      </c>
-      <c r="C113" s="9" t="s">
-        <v>268</v>
-      </c>
-      <c r="D113" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="F113" s="0" t="s">
-        <v>269</v>
-      </c>
+      <c r="C113" s="11"/>
       <c r="G113" s="0" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="I113" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H113),2)</f>
-        <v>7B</v>
-      </c>
-      <c r="J113" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="K113" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="L113" s="0" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="114" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5B</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="6" t="n">
         <v>113</v>
       </c>
-      <c r="B114" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="C114" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="D114" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F114" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="G114" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="H114" s="7" t="s">
-        <v>274</v>
+      <c r="C114" s="11"/>
+      <c r="G114" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>266</v>
       </c>
       <c r="I114" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H114),2)</f>
-        <v>7D</v>
-      </c>
-      <c r="L114" s="6" t="s">
-        <v>275</v>
+        <v>5C</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="6" t="n">
         <v>114</v>
       </c>
-      <c r="B115" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="C115" s="9" t="s">
-        <v>277</v>
-      </c>
-      <c r="D115" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="F115" s="0" t="s">
-        <v>278</v>
-      </c>
+      <c r="C115" s="11"/>
       <c r="G115" s="0" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="H115" s="1" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="I115" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H115),2)</f>
-        <v>7F</v>
-      </c>
-      <c r="J115" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="K115" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="L115" s="0" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="116" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5D</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="6" t="n">
         <v>115</v>
       </c>
-      <c r="B116" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="C116" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="D116" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F116" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="G116" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="H116" s="7" t="s">
-        <v>283</v>
+      <c r="B116" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="C116" s="11"/>
+      <c r="F116" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="G116" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>270</v>
       </c>
       <c r="I116" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H116),2)</f>
-        <v>8F</v>
-      </c>
-      <c r="L116" s="6" t="s">
-        <v>284</v>
+        <v>5E</v>
+      </c>
+      <c r="L116" s="0" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3813,35 +3853,27 @@
         <v>116</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>285</v>
-      </c>
-      <c r="C117" s="9" t="s">
-        <v>286</v>
-      </c>
-      <c r="D117" s="0" t="s">
-        <v>138</v>
-      </c>
+        <v>272</v>
+      </c>
+      <c r="C117" s="11"/>
       <c r="F117" s="0" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="G117" s="0" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="H117" s="1" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="I117" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H117),2)</f>
-        <v>9F</v>
+        <v>5F</v>
       </c>
       <c r="J117" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="K117" s="0" t="s">
-        <v>142</v>
+        <v>88</v>
       </c>
       <c r="L117" s="0" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
     </row>
     <row r="118" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3849,227 +3881,139 @@
         <v>117</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="C118" s="6" t="s">
-        <v>291</v>
+        <v>276</v>
+      </c>
+      <c r="C118" s="10" t="s">
+        <v>277</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>68</v>
+        <v>163</v>
       </c>
       <c r="F118" s="6" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="G118" s="6" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="H118" s="7" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="I118" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H118),2)</f>
-        <v>AF</v>
+        <v>70</v>
       </c>
       <c r="L118" s="6" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="6" t="n">
         <v>118</v>
       </c>
-      <c r="B119" s="0" t="s">
-        <v>294</v>
-      </c>
       <c r="C119" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="D119" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="F119" s="0" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="G119" s="0" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="H119" s="1" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="I119" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H119),2)</f>
-        <v>BF</v>
-      </c>
-      <c r="J119" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="K119" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="L119" s="0" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="120" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="6" t="n">
         <v>119</v>
       </c>
-      <c r="B120" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="C120" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="D120" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F120" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="G120" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="H120" s="7" t="s">
-        <v>301</v>
+      <c r="C120" s="11"/>
+      <c r="G120" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="H120" s="1" t="s">
+        <v>285</v>
       </c>
       <c r="I120" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H120),2)</f>
-        <v>C1</v>
-      </c>
-      <c r="L120" s="6" t="s">
-        <v>302</v>
+        <v>74</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="6" t="n">
         <v>120</v>
       </c>
-      <c r="B121" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="C121" s="9" t="s">
-        <v>304</v>
-      </c>
-      <c r="D121" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="F121" s="0" t="s">
-        <v>305</v>
-      </c>
+      <c r="C121" s="11"/>
       <c r="G121" s="0" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
       <c r="H121" s="1" t="s">
-        <v>306</v>
+        <v>287</v>
       </c>
       <c r="I121" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H121),2)</f>
-        <v>C3</v>
-      </c>
-      <c r="J121" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="K121" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="L121" s="0" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="122" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="6" t="n">
         <v>121</v>
       </c>
-      <c r="B122" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="C122" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="D122" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F122" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="G122" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="H122" s="7" t="s">
-        <v>310</v>
+      <c r="C122" s="11"/>
+      <c r="G122" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="H122" s="1" t="s">
+        <v>289</v>
       </c>
       <c r="I122" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H122),2)</f>
-        <v>C5</v>
-      </c>
-      <c r="L122" s="6" t="s">
-        <v>311</v>
+        <v>78</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="6" t="n">
         <v>122</v>
       </c>
-      <c r="B123" s="0" t="s">
-        <v>312</v>
-      </c>
-      <c r="C123" s="9" t="s">
-        <v>313</v>
-      </c>
-      <c r="D123" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="F123" s="0" t="s">
-        <v>314</v>
-      </c>
+      <c r="C123" s="11"/>
       <c r="G123" s="0" t="s">
-        <v>312</v>
+        <v>290</v>
       </c>
       <c r="H123" s="1" t="s">
-        <v>315</v>
+        <v>291</v>
       </c>
       <c r="I123" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H123),2)</f>
-        <v>C7</v>
-      </c>
-      <c r="J123" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="K123" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="L123" s="0" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="124" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7A</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="6" t="n">
         <v>123</v>
       </c>
-      <c r="B124" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="C124" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="D124" s="6" t="s">
+      <c r="B124" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="C124" s="11"/>
+      <c r="D124" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="F124" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="G124" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="H124" s="7" t="s">
-        <v>319</v>
+      <c r="F124" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="G124" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="H124" s="1" t="s">
+        <v>293</v>
       </c>
       <c r="I124" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H124),2)</f>
-        <v>CB</v>
-      </c>
-      <c r="L124" s="6" t="s">
-        <v>320</v>
+        <v>7C</v>
+      </c>
+      <c r="L124" s="0" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4077,35 +4021,32 @@
         <v>124</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>321</v>
+        <v>295</v>
       </c>
       <c r="C125" s="9" t="s">
-        <v>322</v>
+        <v>296</v>
       </c>
       <c r="D125" s="0" t="s">
-        <v>138</v>
+        <v>85</v>
       </c>
       <c r="F125" s="0" t="s">
-        <v>323</v>
+        <v>297</v>
       </c>
       <c r="G125" s="0" t="s">
-        <v>321</v>
+        <v>295</v>
       </c>
       <c r="H125" s="1" t="s">
-        <v>324</v>
+        <v>298</v>
       </c>
       <c r="I125" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H125),2)</f>
-        <v>CF</v>
+        <v>7E</v>
       </c>
       <c r="J125" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="K125" s="0" t="s">
-        <v>142</v>
+        <v>88</v>
       </c>
       <c r="L125" s="0" t="s">
-        <v>325</v>
+        <v>299</v>
       </c>
     </row>
     <row r="126" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4113,29 +4054,29 @@
         <v>125</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>326</v>
+        <v>300</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>327</v>
+        <v>301</v>
       </c>
       <c r="D126" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F126" s="6" t="s">
-        <v>326</v>
+        <v>300</v>
       </c>
       <c r="G126" s="6" t="s">
-        <v>326</v>
+        <v>300</v>
       </c>
       <c r="H126" s="7" t="s">
-        <v>328</v>
+        <v>302</v>
       </c>
       <c r="I126" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H126),2)</f>
-        <v>D1</v>
+        <v>75</v>
       </c>
       <c r="L126" s="6" t="s">
-        <v>329</v>
+        <v>303</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4143,26 +4084,26 @@
         <v>126</v>
       </c>
       <c r="B127" s="0" t="s">
-        <v>330</v>
+        <v>304</v>
       </c>
       <c r="C127" s="9" t="s">
-        <v>331</v>
+        <v>305</v>
       </c>
       <c r="D127" s="0" t="s">
         <v>138</v>
       </c>
       <c r="F127" s="0" t="s">
-        <v>332</v>
+        <v>306</v>
       </c>
       <c r="G127" s="0" t="s">
-        <v>330</v>
+        <v>304</v>
       </c>
       <c r="H127" s="1" t="s">
-        <v>333</v>
+        <v>307</v>
       </c>
       <c r="I127" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H127),2)</f>
-        <v>D3</v>
+        <v>77</v>
       </c>
       <c r="J127" s="0" t="s">
         <v>141</v>
@@ -4171,7 +4112,7 @@
         <v>142</v>
       </c>
       <c r="L127" s="0" t="s">
-        <v>334</v>
+        <v>308</v>
       </c>
     </row>
     <row r="128" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4179,29 +4120,29 @@
         <v>127</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>335</v>
+        <v>309</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>336</v>
+        <v>310</v>
       </c>
       <c r="D128" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F128" s="6" t="s">
-        <v>335</v>
+        <v>309</v>
       </c>
       <c r="G128" s="6" t="s">
-        <v>335</v>
+        <v>309</v>
       </c>
       <c r="H128" s="7" t="s">
-        <v>337</v>
+        <v>311</v>
       </c>
       <c r="I128" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H128),2)</f>
-        <v>D5</v>
+        <v>79</v>
       </c>
       <c r="L128" s="6" t="s">
-        <v>338</v>
+        <v>312</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4209,26 +4150,26 @@
         <v>128</v>
       </c>
       <c r="B129" s="0" t="s">
-        <v>339</v>
+        <v>313</v>
       </c>
       <c r="C129" s="9" t="s">
-        <v>340</v>
+        <v>314</v>
       </c>
       <c r="D129" s="0" t="s">
         <v>138</v>
       </c>
       <c r="F129" s="0" t="s">
-        <v>341</v>
+        <v>315</v>
       </c>
       <c r="G129" s="0" t="s">
-        <v>339</v>
+        <v>313</v>
       </c>
       <c r="H129" s="1" t="s">
-        <v>342</v>
+        <v>316</v>
       </c>
       <c r="I129" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H129),2)</f>
-        <v>D7</v>
+        <v>7B</v>
       </c>
       <c r="J129" s="0" t="s">
         <v>141</v>
@@ -4237,7 +4178,7 @@
         <v>142</v>
       </c>
       <c r="L129" s="0" t="s">
-        <v>343</v>
+        <v>317</v>
       </c>
     </row>
     <row r="130" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4245,53 +4186,65 @@
         <v>129</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>344</v>
+        <v>318</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>345</v>
+        <v>319</v>
+      </c>
+      <c r="D130" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="F130" s="6" t="s">
-        <v>344</v>
+        <v>318</v>
       </c>
       <c r="G130" s="6" t="s">
-        <v>344</v>
+        <v>318</v>
       </c>
       <c r="H130" s="7" t="s">
-        <v>346</v>
+        <v>320</v>
       </c>
       <c r="I130" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H130),2)</f>
-        <v>05</v>
+        <v>7D</v>
       </c>
       <c r="L130" s="6" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="131" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="6" t="n">
         <v>130</v>
       </c>
-      <c r="B131" s="6" t="s">
-        <v>348</v>
-      </c>
-      <c r="C131" s="6" t="s">
-        <v>349</v>
-      </c>
-      <c r="F131" s="6" t="s">
-        <v>348</v>
-      </c>
-      <c r="G131" s="6" t="s">
-        <v>348</v>
-      </c>
-      <c r="H131" s="7" t="s">
-        <v>350</v>
+      <c r="B131" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="C131" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="D131" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="F131" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="G131" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="H131" s="1" t="s">
+        <v>325</v>
       </c>
       <c r="I131" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H131),2)</f>
-        <v>0F</v>
-      </c>
-      <c r="L131" s="6" t="s">
-        <v>351</v>
+        <v>7F</v>
+      </c>
+      <c r="J131" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="K131" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="L131" s="0" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="132" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4299,53 +4252,65 @@
         <v>131</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>352</v>
+        <v>327</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>353</v>
+        <v>328</v>
+      </c>
+      <c r="D132" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="F132" s="6" t="s">
-        <v>352</v>
+        <v>327</v>
       </c>
       <c r="G132" s="6" t="s">
-        <v>352</v>
+        <v>327</v>
       </c>
       <c r="H132" s="7" t="s">
-        <v>354</v>
+        <v>329</v>
       </c>
       <c r="I132" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H132),2)</f>
-        <v>11</v>
+        <v>8F</v>
       </c>
       <c r="L132" s="6" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="133" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="6" t="n">
         <v>132</v>
       </c>
-      <c r="B133" s="6" t="s">
-        <v>356</v>
-      </c>
-      <c r="C133" s="6" t="s">
-        <v>357</v>
-      </c>
-      <c r="F133" s="6" t="s">
-        <v>356</v>
-      </c>
-      <c r="G133" s="6" t="s">
-        <v>356</v>
-      </c>
-      <c r="H133" s="7" t="s">
-        <v>358</v>
+      <c r="B133" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="C133" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D133" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="F133" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="G133" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="H133" s="1" t="s">
+        <v>334</v>
       </c>
       <c r="I133" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H133),2)</f>
-        <v>15</v>
-      </c>
-      <c r="L133" s="6" t="s">
-        <v>359</v>
+        <v>9F</v>
+      </c>
+      <c r="J133" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="K133" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="L133" s="0" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="134" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4353,37 +4318,539 @@
         <v>133</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>360</v>
+        <v>336</v>
       </c>
       <c r="C134" s="6" t="s">
-        <v>361</v>
+        <v>337</v>
+      </c>
+      <c r="D134" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="F134" s="6" t="s">
-        <v>360</v>
+        <v>336</v>
       </c>
       <c r="G134" s="6" t="s">
-        <v>360</v>
+        <v>336</v>
       </c>
       <c r="H134" s="7" t="s">
-        <v>362</v>
+        <v>338</v>
       </c>
       <c r="I134" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H134),2)</f>
+        <v>AF</v>
+      </c>
+      <c r="L134" s="6" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="6" t="n">
+        <v>134</v>
+      </c>
+      <c r="B135" s="0" t="s">
+        <v>340</v>
+      </c>
+      <c r="C135" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="D135" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="F135" s="0" t="s">
+        <v>342</v>
+      </c>
+      <c r="G135" s="0" t="s">
+        <v>340</v>
+      </c>
+      <c r="H135" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="I135" s="8" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H135),2)</f>
+        <v>BF</v>
+      </c>
+      <c r="J135" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="K135" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="L135" s="0" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="136" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="6" t="n">
+        <v>135</v>
+      </c>
+      <c r="B136" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="C136" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="D136" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F136" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="G136" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="H136" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="I136" s="8" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H136),2)</f>
+        <v>C1</v>
+      </c>
+      <c r="L136" s="6" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="6" t="n">
+        <v>136</v>
+      </c>
+      <c r="B137" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="C137" s="9" t="s">
+        <v>350</v>
+      </c>
+      <c r="D137" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="F137" s="0" t="s">
+        <v>351</v>
+      </c>
+      <c r="G137" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="H137" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="I137" s="8" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H137),2)</f>
+        <v>C3</v>
+      </c>
+      <c r="J137" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="K137" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="L137" s="0" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="138" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="6" t="n">
+        <v>137</v>
+      </c>
+      <c r="B138" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="C138" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="D138" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F138" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="G138" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="H138" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="I138" s="8" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H138),2)</f>
+        <v>C5</v>
+      </c>
+      <c r="L138" s="6" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="6" t="n">
+        <v>138</v>
+      </c>
+      <c r="B139" s="0" t="s">
+        <v>358</v>
+      </c>
+      <c r="C139" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="D139" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="F139" s="0" t="s">
+        <v>360</v>
+      </c>
+      <c r="G139" s="0" t="s">
+        <v>358</v>
+      </c>
+      <c r="H139" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="I139" s="8" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H139),2)</f>
+        <v>C7</v>
+      </c>
+      <c r="J139" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="K139" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="L139" s="0" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="140" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="6" t="n">
+        <v>139</v>
+      </c>
+      <c r="B140" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="C140" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="D140" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F140" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="G140" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="H140" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="I140" s="8" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H140),2)</f>
+        <v>CB</v>
+      </c>
+      <c r="L140" s="6" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="6" t="n">
+        <v>140</v>
+      </c>
+      <c r="B141" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="C141" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="D141" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="F141" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="G141" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="H141" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="I141" s="8" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H141),2)</f>
+        <v>CF</v>
+      </c>
+      <c r="J141" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="K141" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="L141" s="0" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="142" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="6" t="n">
+        <v>141</v>
+      </c>
+      <c r="B142" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="C142" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="D142" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F142" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="G142" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="H142" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="I142" s="8" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H142),2)</f>
+        <v>D1</v>
+      </c>
+      <c r="L142" s="6" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="6" t="n">
+        <v>142</v>
+      </c>
+      <c r="B143" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="C143" s="9" t="s">
+        <v>377</v>
+      </c>
+      <c r="D143" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="F143" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="G143" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="H143" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="I143" s="8" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H143),2)</f>
+        <v>D3</v>
+      </c>
+      <c r="J143" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="K143" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="L143" s="0" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="144" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="6" t="n">
+        <v>143</v>
+      </c>
+      <c r="B144" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="C144" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="D144" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F144" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="G144" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="H144" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="I144" s="8" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H144),2)</f>
+        <v>D5</v>
+      </c>
+      <c r="L144" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="6" t="n">
+        <v>144</v>
+      </c>
+      <c r="B145" s="0" t="s">
+        <v>385</v>
+      </c>
+      <c r="C145" s="9" t="s">
+        <v>386</v>
+      </c>
+      <c r="D145" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="F145" s="0" t="s">
+        <v>387</v>
+      </c>
+      <c r="G145" s="0" t="s">
+        <v>385</v>
+      </c>
+      <c r="H145" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="I145" s="8" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H145),2)</f>
+        <v>D7</v>
+      </c>
+      <c r="J145" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="K145" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="L145" s="0" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="146" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="6" t="n">
+        <v>145</v>
+      </c>
+      <c r="B146" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="C146" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="F146" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="G146" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="H146" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="I146" s="8" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H146),2)</f>
+        <v>05</v>
+      </c>
+      <c r="L146" s="6" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="147" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="6" t="n">
+        <v>146</v>
+      </c>
+      <c r="B147" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="C147" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="F147" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="G147" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="H147" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="I147" s="8" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H147),2)</f>
+        <v>0F</v>
+      </c>
+      <c r="L147" s="6" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="148" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="6" t="n">
+        <v>147</v>
+      </c>
+      <c r="B148" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="C148" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="F148" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="G148" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="H148" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="I148" s="8" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H148),2)</f>
+        <v>11</v>
+      </c>
+      <c r="L148" s="6" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="149" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="6" t="n">
+        <v>148</v>
+      </c>
+      <c r="B149" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="C149" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="F149" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="G149" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="H149" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="I149" s="8" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H149),2)</f>
+        <v>15</v>
+      </c>
+      <c r="L149" s="6" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="150" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="6" t="n">
+        <v>149</v>
+      </c>
+      <c r="B150" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="C150" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="F150" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="G150" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="H150" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="I150" s="8" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H150),2)</f>
         <v>1F</v>
       </c>
-      <c r="L134" s="6" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H135" s="0"/>
-      <c r="I135" s="0"/>
+      <c r="L150" s="6" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H151" s="0"/>
+      <c r="I151" s="0"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>0</formula>
-    </cfRule>
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.39375" right="0.39375" top="0.659027777777778" bottom="0.659027777777778" header="0.39375" footer="0.39375"/>
@@ -4411,7 +4878,7 @@
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.59"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="12.96"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
@@ -5797,7 +6264,7 @@
       </c>
       <c r="B82" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D82,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D82,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>ADC A</v>
       </c>
       <c r="C82" s="2" t="str">
         <f aca="false">DEC2BIN(A82,8)</f>
@@ -5814,7 +6281,7 @@
       </c>
       <c r="B83" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D83,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D83,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>ADC B</v>
       </c>
       <c r="C83" s="2" t="str">
         <f aca="false">DEC2BIN(A83,8)</f>
@@ -5831,7 +6298,7 @@
       </c>
       <c r="B84" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D84,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D84,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>ADC C</v>
       </c>
       <c r="C84" s="2" t="str">
         <f aca="false">DEC2BIN(A84,8)</f>
@@ -5848,7 +6315,7 @@
       </c>
       <c r="B85" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D85,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D85,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>ADC D</v>
       </c>
       <c r="C85" s="2" t="str">
         <f aca="false">DEC2BIN(A85,8)</f>
@@ -5865,7 +6332,7 @@
       </c>
       <c r="B86" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D86,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D86,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>ADC H</v>
       </c>
       <c r="C86" s="2" t="str">
         <f aca="false">DEC2BIN(A86,8)</f>
@@ -5882,7 +6349,7 @@
       </c>
       <c r="B87" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D87,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D87,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>ADC L</v>
       </c>
       <c r="C87" s="2" t="str">
         <f aca="false">DEC2BIN(A87,8)</f>
@@ -5899,7 +6366,7 @@
       </c>
       <c r="B88" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D88,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D88,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>ADC M</v>
       </c>
       <c r="C88" s="2" t="str">
         <f aca="false">DEC2BIN(A88,8)</f>
@@ -5916,7 +6383,7 @@
       </c>
       <c r="B89" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D89,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D89,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>ADC data</v>
       </c>
       <c r="C89" s="2" t="str">
         <f aca="false">DEC2BIN(A89,8)</f>
@@ -5933,7 +6400,7 @@
       </c>
       <c r="B90" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D90,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D90,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>SBB A</v>
       </c>
       <c r="C90" s="2" t="str">
         <f aca="false">DEC2BIN(A90,8)</f>
@@ -5950,7 +6417,7 @@
       </c>
       <c r="B91" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D91,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D91,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>SBB B</v>
       </c>
       <c r="C91" s="2" t="str">
         <f aca="false">DEC2BIN(A91,8)</f>
@@ -5967,7 +6434,7 @@
       </c>
       <c r="B92" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D92,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D92,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>SBB C</v>
       </c>
       <c r="C92" s="2" t="str">
         <f aca="false">DEC2BIN(A92,8)</f>
@@ -5984,7 +6451,7 @@
       </c>
       <c r="B93" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D93,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D93,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>SBB D</v>
       </c>
       <c r="C93" s="2" t="str">
         <f aca="false">DEC2BIN(A93,8)</f>
@@ -6001,7 +6468,7 @@
       </c>
       <c r="B94" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D94,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D94,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>SBB H</v>
       </c>
       <c r="C94" s="2" t="str">
         <f aca="false">DEC2BIN(A94,8)</f>
@@ -6018,7 +6485,7 @@
       </c>
       <c r="B95" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D95,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D95,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>SBB L</v>
       </c>
       <c r="C95" s="2" t="str">
         <f aca="false">DEC2BIN(A95,8)</f>
@@ -6035,7 +6502,7 @@
       </c>
       <c r="B96" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D96,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D96,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>SBB M</v>
       </c>
       <c r="C96" s="2" t="str">
         <f aca="false">DEC2BIN(A96,8)</f>
@@ -6052,7 +6519,7 @@
       </c>
       <c r="B97" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D97,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D97,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>SBB data</v>
       </c>
       <c r="C97" s="2" t="str">
         <f aca="false">DEC2BIN(A97,8)</f>

</xml_diff>

<commit_message>
- add INC and DEC instructions - change opcode for RST instruction
</commit_message>
<xml_diff>
--- a/doc/instruction-set.xlsx
+++ b/doc/instruction-set.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="455">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -86,1192 +86,1306 @@
     <t xml:space="preserve">Reset</t>
   </si>
   <si>
+    <t xml:space="preserve">11110111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reset CPU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV rd,rs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Destination register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV A,B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move value of source register into destination register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1&lt;rd&gt;&lt;rs&gt;0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV A,C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV A,D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000 = A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV A,H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">001 = B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV A,L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">010 = C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV B,A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">011 = D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV B,C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 = H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV B,D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">101 = L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV B,H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">110 = M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV B,L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111 = data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV C,A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV C,B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV C,D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV C,H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV C,L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV D,A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV D,B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV D,C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV D,H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV D,L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV H,A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV H,B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV H,C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV H,D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV H,L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV L,A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV L,B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV L,C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV L,D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV L,H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV rd,M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV A,M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move value at memory address in H and L registers into destination register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV B,M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV C,M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV D,M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV H,M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV L,M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV M,rs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV M,A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move value of source register into memory address in H and L registers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV M,B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV M,C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV M,D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV M,H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV M,L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV rd,data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV A,10h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV A,data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Byte of data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move given data into destination register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV B,data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV C,data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV D,data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV H,data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV L,data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV HL,IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0&lt;rd&gt;&lt;rs&gt;0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H and L registers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instruction Pointer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00000010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move value of Instruction Pointer into H and L registers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV HL,SP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stack Pointer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00000100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move value of Stack Pointer into H and L registers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV IP,HL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000 = HL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00010000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move value of H and L registers into Instruction Pointer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV IP,SP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">001 = IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00010100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move value of Stack Pointer into Instruction Pointer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV SP,HL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">010 = SP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00100000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move value of H and L registers into Stack Pointer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV SP,IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111 = addr/data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00100010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move value of Instruction Pointer into Stack Pointer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV HL,addr/data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address/Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV HL,FFF0h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00001110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Low-order byte of address/data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High-order byte of address/data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move given address/data into H and L registers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV IP,addr/data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV IP,FFF0h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00011110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move given address/data into Instruction Pointer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV SP,addr/data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV SP,FFF0h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00101110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move given address/data into Stack Pointer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LDA rd,addr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load from address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LDA A,FFF0h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LDA A,addr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Low-order byte of address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High-order byte of address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load value at given address into destination register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1&lt;r&gt;&lt;M&gt;1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LDA B,addr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LDA C,addr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LDA D,addr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LDA H,addr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LDA L,addr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STA addr,rs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Store to address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STA FFF0h,A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STA addr,A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Store value of source register into given address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1&lt;M&gt;&lt;r&gt;1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STA addr,B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STA addr,C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STA addr,D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STA addr,H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STA addr,L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUSH r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Push</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUSH A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Push value of register to stack and decrease stack pointer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1&lt;r&gt;&lt;r&gt;0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUSH B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUSH C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUSH D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUSH H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUSH L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POP r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POP A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pop value from stack into register and increase stack pointer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1&lt;r&gt;&lt;r&gt;1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POP B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POP C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POP D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POP H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POP L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01100000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increment accumulator (A register) by value of register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0&lt;M&gt;&lt;r&gt;0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01100010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01100100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01100110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01101000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01101010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01101100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increment accumulator (A register) by value at memory address in H and L registers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0&lt;M&gt;&lt;data&gt;0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD 10h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01101110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increment accumulator (A register) by given data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUB r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subtract</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUB A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01100001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decrement accumulator (A register) by value of register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0&lt;M&gt;&lt;r&gt;1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUB B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01100011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUB C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01100101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUB D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01100111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUB H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01101001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUB L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01101011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUB M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01101101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decrement accumulator (A register) by value at memory address in H and L registers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUB data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0&lt;M&gt;&lt;data&gt;1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUB 10h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01101111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decrement accumulator (A register) by given data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMP r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMP A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01110000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compare accumulator (A register) with value of register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0&lt;data&gt;&lt;r&gt;0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMP B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01110010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMP C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01110100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMP D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01110110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMP H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01111000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMP L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01111010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMP M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01111100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compare accumulator (A register) with value at memory address in H and L registers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMP data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0&lt;data&gt;&lt;data&gt;0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMP 10h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01111110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compare accumulator (A register) with given data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add with Carry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01010000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increment accumulator (A register) by value of register with carry if set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01010&lt;x&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01010001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01010010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01010011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01010100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01010101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01010110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increment accumulator (A register) by value at memory address in H and L registers with carry if set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC 10h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01010111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increment accumulator (A register) by given data with carry if set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBB r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subtract with Borrow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBB A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01011000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decrement accumulator (A register) by value of register with borrow if set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01011&lt;x&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBB B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01011001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBB C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01011010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBB D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01011011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBB H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01011100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBB L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01011101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBB M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01011110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decrement accumulator (A register) by value at memory address in H and L registers with borrow if set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBB data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBB 10h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01011111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decrement accumulator (A register) by given data with borrow if set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JMP M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump unconditionally</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01110101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump to memory address in H and L registers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JMP addr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">011101&lt;x&gt;1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JMP FFF0h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01110111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump to given address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JC M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump on carry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01111001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump to memory address in H and L registers if carry flag is set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JC addr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">011110&lt;x&gt;1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JC FFF0h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01111011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump to given address if carry flag is set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JNC M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump on no carry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01111101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump to memory address in H and L registers if carry flag is clear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JNC addr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">011111&lt;x&gt;1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JNC FFF0h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01111111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump to given address if carry flag is clear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JZ M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump on zero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10001111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump to memory address in H and L registers if zero flag is set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JZ addr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100&lt;x&gt;1111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JZ FFF0h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10011111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump to given address if zero flag is set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JNZ M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump on no zero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10101111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump to memory address in H and L registers if zero flag is clear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JNZ addr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">101&lt;x&gt;1111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JNZ FFF0h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10111111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump to given address if zero flag is clear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALL M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call unconditionally</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11000001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call memory address in H and L registers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALL addr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">110000&lt;x&gt;1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALL FFF0h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11000011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call given address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call on carry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11000101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call memory address in H and L registers if carry flag is set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC addr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">110001&lt;x&gt;1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC FFF0h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11000111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call given address if carry flag is set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CNC M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call on no carry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11001011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call memory address in H and L registers if carry flag is clear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CNC addr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11001&lt;x&gt;11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CNC FFF0h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11001111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call given address if carry flag is clear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CZ M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call on zero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11010001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call memory address in H and L registers if zero flag is set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CZ addr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">110100&lt;x&gt;1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CZ FFF0h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11010011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call given address if zero flag is set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CNZ M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call on no zero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11010101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call memory address in H and L registers if zero flag is clear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CNZ addr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">110101&lt;x&gt;1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CNZ FFF0h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11010111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call given address if zero flag is clear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return unconditionally</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00000101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return on carry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00001111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return if carry flag is set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RNC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return on no carry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00010001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return if carry flag is clear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return on zero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00010101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return if zero flag is set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RNZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return on no zero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00011111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return if zero flag is clear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call Interrupt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interrupt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INT 10h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INT int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interrupt number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call given interrupt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INC r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INC A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11110000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increment register by 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11110&lt;r&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INC B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11110001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INC C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11110010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INC D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11110011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INC H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11110100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INC L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11110101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INC M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11110110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increment value at memory address in H and L registers by 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decrement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEC A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11111000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decrement register by 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11111&lt;r&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEC B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11111001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEC C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11111010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEC D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11111011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEC H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11111100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEC L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11111101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEC M</t>
+  </si>
+  <si>
     <t xml:space="preserve">11111110</t>
   </si>
   <si>
-    <t xml:space="preserve">Reset CPU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV rd,rs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Destination register</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source register</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV A,B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move value of source register into destination register</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1&lt;rd&gt;&lt;rs&gt;0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV A,C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV A,D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">000 = A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV A,H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">001 = B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV A,L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">010 = C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV B,A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">011 = D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV B,C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100 = H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV B,D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">101 = L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV B,H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">110 = M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV B,L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">111 = data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV C,A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV C,B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV C,D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV C,H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV C,L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV D,A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV D,B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV D,C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV D,H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV D,L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV H,A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV H,B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV H,C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV H,D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV H,L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV L,A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV L,B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV L,C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV L,D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV L,H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV rd,M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV A,M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move value at memory address in H and L registers into destination register</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV B,M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV C,M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV D,M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV H,M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV L,M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV M,rs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV M,A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move value of source register into memory address in H and L registers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV M,B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV M,C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV M,D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV M,H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV M,L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV rd,data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV A,10h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV A,data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Byte of data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move given data into destination register</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV B,data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV C,data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV D,data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV H,data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV L,data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV HL,IP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0&lt;rd&gt;&lt;rs&gt;0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H and L registers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Instruction Pointer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00000010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move value of Instruction Pointer into H and L registers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV HL,SP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stack Pointer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00000100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move value of Stack Pointer into H and L registers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV IP,HL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">000 = HL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00010000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move value of H and L registers into Instruction Pointer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV IP,SP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">001 = IP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00010100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move value of Stack Pointer into Instruction Pointer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV SP,HL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">010 = SP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00100000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move value of H and L registers into Stack Pointer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV SP,IP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">111 = addr/data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00100010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move value of Instruction Pointer into Stack Pointer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV HL,addr/data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Address/Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV HL,FFF0h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00001110</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Low-order byte of address/data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">High-order byte of address/data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move given address/data into H and L registers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV IP,addr/data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV IP,FFF0h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00011110</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move given address/data into Instruction Pointer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV SP,addr/data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV SP,FFF0h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00101110</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move given address/data into Stack Pointer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LDA rd,addr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Load from address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LDA A,FFF0h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LDA A,addr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Low-order byte of address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">High-order byte of address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Load value at given address into destination register</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1&lt;r&gt;&lt;M&gt;1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LDA B,addr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LDA C,addr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LDA D,addr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LDA H,addr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LDA L,addr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STA addr,rs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Store to address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STA FFF0h,A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STA addr,A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Store value of source register into given address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1&lt;M&gt;&lt;r&gt;1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STA addr,B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STA addr,C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STA addr,D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STA addr,H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STA addr,L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PUSH r</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Push</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Register</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PUSH A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Push value of register to stack and decrease stack pointer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1&lt;r&gt;&lt;r&gt;0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PUSH B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PUSH C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PUSH D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PUSH H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PUSH L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POP r</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POP A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pop value from stack into register and increase stack pointer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1&lt;r&gt;&lt;r&gt;1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POP B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POP C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POP D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POP H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POP L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADD r</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADD A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01100000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Increment accumulator (A register) by value of register</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0&lt;M&gt;&lt;r&gt;0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADD B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01100010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADD C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01100100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADD D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01100110</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADD H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01101000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADD L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01101010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADD M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01101100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Increment accumulator (A register) by value at memory address in H and L registers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADD data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0&lt;M&gt;&lt;data&gt;0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADD 10h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01101110</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Increment accumulator (A register) by given data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SUB r</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subtract</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SUB A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01100001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Decrement accumulator (A register) by value of register</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0&lt;M&gt;&lt;r&gt;1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SUB B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01100011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SUB C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01100101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SUB D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01100111</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SUB H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01101001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SUB L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01101011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SUB M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01101101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Decrement accumulator (A register) by value at memory address in H and L registers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SUB data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0&lt;M&gt;&lt;data&gt;1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SUB 10h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01101111</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Decrement accumulator (A register) by given data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CMP r</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compare</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CMP A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01110000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compare accumulator (A register) with value of register</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0&lt;data&gt;&lt;r&gt;0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CMP B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01110010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CMP C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01110100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CMP D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01110110</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CMP H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01111000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CMP L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01111010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CMP M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01111100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compare accumulator (A register) with value at memory address in H and L registers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CMP data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0&lt;data&gt;&lt;data&gt;0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CMP 10h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01111110</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compare accumulator (A register) with given data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADC r</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add with Carry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADC A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01010000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Increment accumulator (A register) by value of register with carry if set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01010&lt;x&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADC B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01010001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADC C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01010010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADC D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01010011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADC H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01010100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADC L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01010101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADC M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01010110</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Increment accumulator (A register) by value at memory address in H and L registers with carry if set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADC data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADC 10h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01010111</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Increment accumulator (A register) by given data with carry if set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SBB r</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subtract with Borrow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SBB A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01011000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Decrement accumulator (A register) by value of register with borrow if set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01011&lt;x&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SBB B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01011001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SBB C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01011010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SBB D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01011011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SBB H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01011100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SBB L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01011101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SBB M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01011110</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Decrement accumulator (A register) by value at memory address in H and L registers with borrow if set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SBB data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SBB 10h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01011111</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Decrement accumulator (A register) by given data with borrow if set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JMP M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jump unconditionally</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01110101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jump to memory address in H and L registers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JMP addr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">011101&lt;x&gt;1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JMP FFF0h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01110111</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jump to given address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JC M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jump on carry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01111001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jump to memory address in H and L registers if carry flag is set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JC addr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">011110&lt;x&gt;1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JC FFF0h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01111011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jump to given address if carry flag is set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JNC M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jump on no carry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01111101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jump to memory address in H and L registers if carry flag is clear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JNC addr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">011111&lt;x&gt;1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JNC FFF0h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01111111</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jump to given address if carry flag is clear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JZ M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jump on zero</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10001111</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jump to memory address in H and L registers if zero flag is set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JZ addr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100&lt;x&gt;1111</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JZ FFF0h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10011111</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jump to given address if zero flag is set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JNZ M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jump on no zero</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10101111</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jump to memory address in H and L registers if zero flag is clear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JNZ addr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">101&lt;x&gt;1111</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JNZ FFF0h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10111111</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jump to given address if zero flag is clear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CALL M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Call unconditionally</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11000001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Call memory address in H and L registers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CALL addr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">110000&lt;x&gt;1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CALL FFF0h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11000011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Call given address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CC M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Call on carry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11000101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Call memory address in H and L registers if carry flag is set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CC addr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">110001&lt;x&gt;1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CC FFF0h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11000111</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Call given address if carry flag is set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CNC M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Call on no carry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11001011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Call memory address in H and L registers if carry flag is clear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CNC addr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11001&lt;x&gt;11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CNC FFF0h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11001111</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Call given address if carry flag is clear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CZ M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Call on zero</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11010001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Call memory address in H and L registers if zero flag is set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CZ addr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">110100&lt;x&gt;1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CZ FFF0h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11010011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Call given address if zero flag is set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CNZ M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Call on no zero</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11010101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Call memory address in H and L registers if zero flag is clear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CNZ addr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">110101&lt;x&gt;1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CNZ FFF0h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11010111</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Call given address if zero flag is clear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Return unconditionally</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00000101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Return</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Return on carry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00001111</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Return if carry flag is set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RNC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Return on no carry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00010001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Return if carry flag is clear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Return on zero</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00010101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Return if zero flag is set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RNZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Return on no zero</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00011111</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Return if zero flag is clear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Call Interrupt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interrupt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INT 10h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INT int</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interrupt number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Call given interrupt</t>
+    <t xml:space="preserve">Decrement value at memory address in H and L registers by 1</t>
   </si>
 </sst>
 </file>
@@ -1519,12 +1633,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:L151"/>
+  <dimension ref="A1:L165"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="I2" activeCellId="0" sqref="I:I"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1657,7 +1771,7 @@
       </c>
       <c r="I4" s="8" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H4),2)</f>
-        <v>FE</v>
+        <v>F7</v>
       </c>
       <c r="L4" s="6" t="s">
         <v>22</v>
@@ -4896,6 +5010,264 @@
       </c>
       <c r="L151" s="6" t="s">
         <v>416</v>
+      </c>
+    </row>
+    <row r="152" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="6" t="n">
+        <v>151</v>
+      </c>
+      <c r="B152" s="6" t="s">
+        <v>417</v>
+      </c>
+      <c r="C152" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="D152" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="F152" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="G152" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="H152" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="I152" s="8" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H152),2)</f>
+        <v>F0</v>
+      </c>
+      <c r="L152" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="6" t="n">
+        <v>152</v>
+      </c>
+      <c r="C153" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="G153" s="0" t="s">
+        <v>423</v>
+      </c>
+      <c r="H153" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="I153" s="8" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H153),2)</f>
+        <v>F1</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="6" t="n">
+        <v>153</v>
+      </c>
+      <c r="G154" s="0" t="s">
+        <v>425</v>
+      </c>
+      <c r="H154" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="I154" s="8" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H154),2)</f>
+        <v>F2</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="6" t="n">
+        <v>154</v>
+      </c>
+      <c r="G155" s="0" t="s">
+        <v>427</v>
+      </c>
+      <c r="H155" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="I155" s="8" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H155),2)</f>
+        <v>F3</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="6" t="n">
+        <v>155</v>
+      </c>
+      <c r="G156" s="0" t="s">
+        <v>429</v>
+      </c>
+      <c r="H156" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="I156" s="8" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H156),2)</f>
+        <v>F4</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="6" t="n">
+        <v>156</v>
+      </c>
+      <c r="G157" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="H157" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="I157" s="8" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H157),2)</f>
+        <v>F5</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="6" t="n">
+        <v>157</v>
+      </c>
+      <c r="D158" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="G158" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="H158" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="I158" s="8" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H158),2)</f>
+        <v>F6</v>
+      </c>
+      <c r="L158" s="0" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="159" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="6" t="n">
+        <v>158</v>
+      </c>
+      <c r="B159" s="6" t="s">
+        <v>436</v>
+      </c>
+      <c r="C159" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="D159" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="F159" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="G159" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="H159" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="I159" s="8" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H159),2)</f>
+        <v>F8</v>
+      </c>
+      <c r="L159" s="6" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="6" t="n">
+        <v>159</v>
+      </c>
+      <c r="C160" s="9" t="s">
+        <v>441</v>
+      </c>
+      <c r="G160" s="0" t="s">
+        <v>442</v>
+      </c>
+      <c r="H160" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="I160" s="8" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H160),2)</f>
+        <v>F9</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="6" t="n">
+        <v>160</v>
+      </c>
+      <c r="G161" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="H161" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="I161" s="8" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H161),2)</f>
+        <v>FA</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="6" t="n">
+        <v>161</v>
+      </c>
+      <c r="G162" s="0" t="s">
+        <v>446</v>
+      </c>
+      <c r="H162" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="I162" s="8" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H162),2)</f>
+        <v>FB</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="6" t="n">
+        <v>162</v>
+      </c>
+      <c r="G163" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="H163" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="I163" s="8" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H163),2)</f>
+        <v>FC</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="6" t="n">
+        <v>163</v>
+      </c>
+      <c r="G164" s="0" t="s">
+        <v>450</v>
+      </c>
+      <c r="H164" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="I164" s="8" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H164),2)</f>
+        <v>FD</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="6" t="n">
+        <v>164</v>
+      </c>
+      <c r="D165" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="G165" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="H165" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="I165" s="8" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H165),2)</f>
+        <v>FE</v>
+      </c>
+      <c r="L165" s="0" t="s">
+        <v>454</v>
       </c>
     </row>
   </sheetData>
@@ -4922,7 +5294,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="C249" activeCellId="1" sqref="I:I C249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9034,7 +9406,7 @@
       </c>
       <c r="B242" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D242,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D242,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>INC A</v>
       </c>
       <c r="C242" s="2" t="str">
         <f aca="false">DEC2BIN(A242,8)</f>
@@ -9051,7 +9423,7 @@
       </c>
       <c r="B243" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D243,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D243,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>INC B</v>
       </c>
       <c r="C243" s="2" t="str">
         <f aca="false">DEC2BIN(A243,8)</f>
@@ -9068,7 +9440,7 @@
       </c>
       <c r="B244" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D244,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D244,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>INC C</v>
       </c>
       <c r="C244" s="2" t="str">
         <f aca="false">DEC2BIN(A244,8)</f>
@@ -9085,7 +9457,7 @@
       </c>
       <c r="B245" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D245,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D245,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>INC D</v>
       </c>
       <c r="C245" s="2" t="str">
         <f aca="false">DEC2BIN(A245,8)</f>
@@ -9102,7 +9474,7 @@
       </c>
       <c r="B246" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D246,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D246,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>INC H</v>
       </c>
       <c r="C246" s="2" t="str">
         <f aca="false">DEC2BIN(A246,8)</f>
@@ -9119,7 +9491,7 @@
       </c>
       <c r="B247" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D247,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D247,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>INC L</v>
       </c>
       <c r="C247" s="2" t="str">
         <f aca="false">DEC2BIN(A247,8)</f>
@@ -9136,7 +9508,7 @@
       </c>
       <c r="B248" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D248,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D248,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>INC M</v>
       </c>
       <c r="C248" s="2" t="str">
         <f aca="false">DEC2BIN(A248,8)</f>
@@ -9153,7 +9525,7 @@
       </c>
       <c r="B249" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D249,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D249,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>RST</v>
       </c>
       <c r="C249" s="2" t="str">
         <f aca="false">DEC2BIN(A249,8)</f>
@@ -9170,7 +9542,7 @@
       </c>
       <c r="B250" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D250,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D250,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>DEC A</v>
       </c>
       <c r="C250" s="2" t="str">
         <f aca="false">DEC2BIN(A250,8)</f>
@@ -9187,7 +9559,7 @@
       </c>
       <c r="B251" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D251,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D251,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>DEC B</v>
       </c>
       <c r="C251" s="2" t="str">
         <f aca="false">DEC2BIN(A251,8)</f>
@@ -9204,7 +9576,7 @@
       </c>
       <c r="B252" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D252,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D252,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>DEC C</v>
       </c>
       <c r="C252" s="2" t="str">
         <f aca="false">DEC2BIN(A252,8)</f>
@@ -9221,7 +9593,7 @@
       </c>
       <c r="B253" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D253,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D253,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>DEC D</v>
       </c>
       <c r="C253" s="2" t="str">
         <f aca="false">DEC2BIN(A253,8)</f>
@@ -9238,7 +9610,7 @@
       </c>
       <c r="B254" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D254,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D254,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>DEC H</v>
       </c>
       <c r="C254" s="2" t="str">
         <f aca="false">DEC2BIN(A254,8)</f>
@@ -9255,7 +9627,7 @@
       </c>
       <c r="B255" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D255,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D255,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>DEC L</v>
       </c>
       <c r="C255" s="2" t="str">
         <f aca="false">DEC2BIN(A255,8)</f>
@@ -9272,7 +9644,7 @@
       </c>
       <c r="B256" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D256,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D256,'Instruction Set'!I:I,0)))</f>
-        <v>RST</v>
+        <v>DEC M</v>
       </c>
       <c r="C256" s="2" t="str">
         <f aca="false">DEC2BIN(A256,8)</f>

</xml_diff>

<commit_message>
fix bit pattern expressions
</commit_message>
<xml_diff>
--- a/doc/instruction-set.xlsx
+++ b/doc/instruction-set.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="690">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -455,7 +455,7 @@
     <t xml:space="preserve">Load value at given address into destination register</t>
   </si>
   <si>
-    <t xml:space="preserve">1&lt;r&gt;&lt;M&gt;1</t>
+    <t xml:space="preserve">1&lt;r&gt;1101</t>
   </si>
   <si>
     <t xml:space="preserve">LDA B,addr</t>
@@ -488,7 +488,7 @@
     <t xml:space="preserve">Store value of source register into given address</t>
   </si>
   <si>
-    <t xml:space="preserve">1&lt;M&gt;&lt;r&gt;1</t>
+    <t xml:space="preserve">1110&lt;r&gt;1</t>
   </si>
   <si>
     <t xml:space="preserve">STA addr,B</t>
@@ -584,7 +584,7 @@
     <t xml:space="preserve">Add value of register to accumulator (A register)</t>
   </si>
   <si>
-    <t xml:space="preserve">0&lt;M&gt;&lt;r&gt;0</t>
+    <t xml:space="preserve">0110&lt;r&gt;0</t>
   </si>
   <si>
     <t xml:space="preserve">ADD B</t>
@@ -629,9 +629,6 @@
     <t xml:space="preserve">ADD data</t>
   </si>
   <si>
-    <t xml:space="preserve">0&lt;M&gt;&lt;data&gt;0</t>
-  </si>
-  <si>
     <t xml:space="preserve">ADD 10h</t>
   </si>
   <si>
@@ -656,7 +653,7 @@
     <t xml:space="preserve">Subtract value of register from accumulator (A register)</t>
   </si>
   <si>
-    <t xml:space="preserve">0&lt;M&gt;&lt;r&gt;1</t>
+    <t xml:space="preserve">0110&lt;r&gt;1</t>
   </si>
   <si>
     <t xml:space="preserve">SUB B</t>
@@ -701,9 +698,6 @@
     <t xml:space="preserve">SUB data</t>
   </si>
   <si>
-    <t xml:space="preserve">0&lt;M&gt;&lt;data&gt;1</t>
-  </si>
-  <si>
     <t xml:space="preserve">SUB 10h</t>
   </si>
   <si>
@@ -728,7 +722,7 @@
     <t xml:space="preserve">Compare accumulator (A register) with value of register</t>
   </si>
   <si>
-    <t xml:space="preserve">0&lt;data&gt;&lt;r&gt;0</t>
+    <t xml:space="preserve">0111&lt;r&gt;0</t>
   </si>
   <si>
     <t xml:space="preserve">CMP B</t>
@@ -773,9 +767,6 @@
     <t xml:space="preserve">CMP data</t>
   </si>
   <si>
-    <t xml:space="preserve">0&lt;data&gt;&lt;data&gt;0</t>
-  </si>
-  <si>
     <t xml:space="preserve">CMP 10h</t>
   </si>
   <si>
@@ -1070,6 +1061,9 @@
     <t xml:space="preserve">Invert all bits in value of register (ones‘ complement)</t>
   </si>
   <si>
+    <t xml:space="preserve">00001&lt;r&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">NOT B</t>
   </si>
   <si>
@@ -1115,6 +1109,9 @@
     <t xml:space="preserve">Shift all bits in value of register by 1 position to left, move MSB into CF</t>
   </si>
   <si>
+    <t xml:space="preserve">00011&lt;r&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">SHL B</t>
   </si>
   <si>
@@ -1160,6 +1157,9 @@
     <t xml:space="preserve">Shift all bits in value of register by 1 position to right, move LSB into CF</t>
   </si>
   <si>
+    <t xml:space="preserve">00101&lt;r&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">SHR B</t>
   </si>
   <si>
@@ -2000,6 +2000,9 @@
     <t xml:space="preserve">Move value from port number in H and L registers into destination register</t>
   </si>
   <si>
+    <t xml:space="preserve">01000&lt;r&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">IN B</t>
   </si>
   <si>
@@ -2043,6 +2046,9 @@
   </si>
   <si>
     <t xml:space="preserve">Move value from source register into port number in H and L registers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01001&lt;r&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">OUT B</t>
@@ -4198,20 +4204,17 @@
       <c r="B93" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="C93" s="10" t="s">
-        <v>202</v>
-      </c>
       <c r="D93" s="1" t="s">
         <v>85</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>201</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I93" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H93),2)</f>
@@ -4221,7 +4224,7 @@
         <v>88</v>
       </c>
       <c r="L93" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="94" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4229,29 +4232,29 @@
         <v>93</v>
       </c>
       <c r="B94" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C94" s="7" t="s">
         <v>206</v>
-      </c>
-      <c r="C94" s="7" t="s">
-        <v>207</v>
       </c>
       <c r="D94" s="7" t="s">
         <v>163</v>
       </c>
       <c r="F94" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="G94" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="H94" s="8" t="s">
         <v>208</v>
-      </c>
-      <c r="G94" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="H94" s="8" t="s">
-        <v>209</v>
       </c>
       <c r="I94" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H94),2)</f>
         <v>61</v>
       </c>
       <c r="L94" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4259,13 +4262,13 @@
         <v>94</v>
       </c>
       <c r="C95" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="G95" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="G95" s="1" t="s">
+      <c r="H95" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="H95" s="2" t="s">
-        <v>213</v>
       </c>
       <c r="I95" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H95),2)</f>
@@ -4277,10 +4280,10 @@
         <v>95</v>
       </c>
       <c r="G96" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="H96" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="H96" s="2" t="s">
-        <v>215</v>
       </c>
       <c r="I96" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H96),2)</f>
@@ -4292,10 +4295,10 @@
         <v>96</v>
       </c>
       <c r="G97" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="H97" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="H97" s="2" t="s">
-        <v>217</v>
       </c>
       <c r="I97" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H97),2)</f>
@@ -4307,10 +4310,10 @@
         <v>97</v>
       </c>
       <c r="G98" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="H98" s="2" t="s">
         <v>218</v>
-      </c>
-      <c r="H98" s="2" t="s">
-        <v>219</v>
       </c>
       <c r="I98" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H98),2)</f>
@@ -4322,10 +4325,10 @@
         <v>98</v>
       </c>
       <c r="G99" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="H99" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="H99" s="2" t="s">
-        <v>221</v>
       </c>
       <c r="I99" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H99),2)</f>
@@ -4337,26 +4340,26 @@
         <v>99</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F100" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="H100" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="G100" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="H100" s="2" t="s">
-        <v>223</v>
       </c>
       <c r="I100" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H100),2)</f>
         <v>6D</v>
       </c>
       <c r="L100" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4364,22 +4367,19 @@
         <v>100</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="C101" s="10" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>85</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H101" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="I101" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H101),2)</f>
@@ -4389,7 +4389,7 @@
         <v>88</v>
       </c>
       <c r="L101" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="102" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4397,29 +4397,29 @@
         <v>101</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D102" s="7" t="s">
         <v>163</v>
       </c>
       <c r="F102" s="7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G102" s="7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H102" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I102" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H102),2)</f>
         <v>70</v>
       </c>
       <c r="L102" s="7" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4427,13 +4427,13 @@
         <v>102</v>
       </c>
       <c r="C103" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="H103" s="2" t="s">
         <v>235</v>
-      </c>
-      <c r="G103" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="H103" s="2" t="s">
-        <v>237</v>
       </c>
       <c r="I103" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H103),2)</f>
@@ -4445,10 +4445,10 @@
         <v>103</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H104" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I104" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H104),2)</f>
@@ -4460,10 +4460,10 @@
         <v>104</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H105" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="I105" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H105),2)</f>
@@ -4475,10 +4475,10 @@
         <v>105</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H106" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="I106" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H106),2)</f>
@@ -4490,10 +4490,10 @@
         <v>106</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H107" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="I107" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H107),2)</f>
@@ -4505,26 +4505,26 @@
         <v>107</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="I108" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H108),2)</f>
         <v>7C</v>
       </c>
       <c r="L108" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4532,22 +4532,19 @@
         <v>108</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="C109" s="10" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>85</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="G109" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="H109" s="2" t="s">
         <v>249</v>
-      </c>
-      <c r="H109" s="2" t="s">
-        <v>252</v>
       </c>
       <c r="I109" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H109),2)</f>
@@ -4557,7 +4554,7 @@
         <v>88</v>
       </c>
       <c r="L109" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="110" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4565,29 +4562,29 @@
         <v>109</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D110" s="7" t="s">
         <v>163</v>
       </c>
       <c r="F110" s="7" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="G110" s="7" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="H110" s="8" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="I110" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H110),2)</f>
         <v>50</v>
       </c>
       <c r="L110" s="7" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4595,13 +4592,13 @@
         <v>110</v>
       </c>
       <c r="C111" s="10" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="H111" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="I111" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H111),2)</f>
@@ -4613,10 +4610,10 @@
         <v>111</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="H112" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="I112" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H112),2)</f>
@@ -4628,10 +4625,10 @@
         <v>112</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="H113" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="I113" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H113),2)</f>
@@ -4643,10 +4640,10 @@
         <v>113</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="H114" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="I114" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H114),2)</f>
@@ -4658,10 +4655,10 @@
         <v>114</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="H115" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="I115" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H115),2)</f>
@@ -4673,23 +4670,23 @@
         <v>115</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="H116" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="I116" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H116),2)</f>
         <v>56</v>
       </c>
       <c r="L116" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4697,16 +4694,16 @@
         <v>116</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="H117" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="I117" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H117),2)</f>
@@ -4716,7 +4713,7 @@
         <v>88</v>
       </c>
       <c r="L117" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="118" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4724,29 +4721,29 @@
         <v>117</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D118" s="7" t="s">
         <v>163</v>
       </c>
       <c r="F118" s="7" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="G118" s="7" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="H118" s="8" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="I118" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H118),2)</f>
         <v>58</v>
       </c>
       <c r="L118" s="7" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4754,13 +4751,13 @@
         <v>118</v>
       </c>
       <c r="C119" s="10" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="H119" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="I119" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H119),2)</f>
@@ -4772,10 +4769,10 @@
         <v>119</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="H120" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="I120" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H120),2)</f>
@@ -4787,10 +4784,10 @@
         <v>120</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="H121" s="2" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="I121" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H121),2)</f>
@@ -4802,10 +4799,10 @@
         <v>121</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="H122" s="2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="I122" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H122),2)</f>
@@ -4817,10 +4814,10 @@
         <v>122</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="H123" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I123" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H123),2)</f>
@@ -4832,23 +4829,23 @@
         <v>123</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="H124" s="2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="I124" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H124),2)</f>
         <v>5E</v>
       </c>
       <c r="L124" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4856,16 +4853,16 @@
         <v>124</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="H125" s="2" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="I125" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H125),2)</f>
@@ -4875,7 +4872,7 @@
         <v>88</v>
       </c>
       <c r="L125" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="126" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4883,29 +4880,29 @@
         <v>125</v>
       </c>
       <c r="B126" s="7" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C126" s="7" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D126" s="7" t="s">
         <v>163</v>
       </c>
       <c r="F126" s="7" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="G126" s="7" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="H126" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="I126" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H126),2)</f>
         <v>30</v>
       </c>
       <c r="L126" s="7" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4913,13 +4910,13 @@
         <v>126</v>
       </c>
       <c r="C127" s="10" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="H127" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="I127" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H127),2)</f>
@@ -4931,10 +4928,10 @@
         <v>127</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H128" s="2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="I128" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H128),2)</f>
@@ -4946,10 +4943,10 @@
         <v>128</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="H129" s="2" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="I129" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H129),2)</f>
@@ -4961,10 +4958,10 @@
         <v>129</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="H130" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="I130" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H130),2)</f>
@@ -4976,10 +4973,10 @@
         <v>130</v>
       </c>
       <c r="G131" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="H131" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I131" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H131),2)</f>
@@ -4991,19 +4988,19 @@
         <v>131</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D132" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="H132" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="I132" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H132),2)</f>
@@ -5015,19 +5012,19 @@
         <v>132</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>85</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="H133" s="2" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="I133" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H133),2)</f>
@@ -5037,7 +5034,7 @@
         <v>88</v>
       </c>
       <c r="L133" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="134" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5045,29 +5042,29 @@
         <v>133</v>
       </c>
       <c r="B134" s="7" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C134" s="7" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D134" s="7" t="s">
         <v>163</v>
       </c>
       <c r="F134" s="7" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="G134" s="7" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="H134" s="8" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="I134" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H134),2)</f>
         <v>38</v>
       </c>
       <c r="L134" s="7" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5075,13 +5072,13 @@
         <v>134</v>
       </c>
       <c r="C135" s="10" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="H135" s="2" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="I135" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H135),2)</f>
@@ -5093,10 +5090,10 @@
         <v>135</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="H136" s="2" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="I136" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H136),2)</f>
@@ -5108,10 +5105,10 @@
         <v>136</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="H137" s="2" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="I137" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H137),2)</f>
@@ -5123,10 +5120,10 @@
         <v>137</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="H138" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="I138" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H138),2)</f>
@@ -5138,10 +5135,10 @@
         <v>138</v>
       </c>
       <c r="G139" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="H139" s="2" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="I139" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H139),2)</f>
@@ -5153,19 +5150,19 @@
         <v>139</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D140" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="H140" s="2" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="I140" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H140),2)</f>
@@ -5177,19 +5174,19 @@
         <v>140</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D141" s="1" t="s">
         <v>85</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="G141" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="H141" s="2" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="I141" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H141),2)</f>
@@ -5199,7 +5196,7 @@
         <v>88</v>
       </c>
       <c r="L141" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="142" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5207,40 +5204,43 @@
         <v>141</v>
       </c>
       <c r="B142" s="7" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C142" s="7" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D142" s="7" t="s">
         <v>163</v>
       </c>
       <c r="F142" s="7" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G142" s="7" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="H142" s="8" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="I142" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H142),2)</f>
         <v>08</v>
       </c>
       <c r="L142" s="7" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="7" t="n">
         <v>142</v>
       </c>
+      <c r="C143" s="10" t="s">
+        <v>346</v>
+      </c>
       <c r="G143" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="H143" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="I143" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H143),2)</f>
@@ -5252,10 +5252,10 @@
         <v>143</v>
       </c>
       <c r="G144" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="H144" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="I144" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H144),2)</f>
@@ -5267,10 +5267,10 @@
         <v>144</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="H145" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="I145" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H145),2)</f>
@@ -5282,10 +5282,10 @@
         <v>145</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="H146" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="I146" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H146),2)</f>
@@ -5297,10 +5297,10 @@
         <v>146</v>
       </c>
       <c r="G147" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="H147" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="I147" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H147),2)</f>
@@ -5312,40 +5312,43 @@
         <v>147</v>
       </c>
       <c r="B148" s="7" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C148" s="7" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D148" s="7" t="s">
         <v>163</v>
       </c>
       <c r="F148" s="7" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="G148" s="7" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="H148" s="8" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="I148" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H148),2)</f>
         <v>18</v>
       </c>
       <c r="L148" s="7" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="7" t="n">
         <v>148</v>
       </c>
+      <c r="C149" s="10" t="s">
+        <v>362</v>
+      </c>
       <c r="G149" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="H149" s="2" t="s">
         <v>364</v>
-      </c>
-      <c r="H149" s="2" t="s">
-        <v>365</v>
       </c>
       <c r="I149" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H149),2)</f>
@@ -5357,10 +5360,10 @@
         <v>149</v>
       </c>
       <c r="G150" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="H150" s="2" t="s">
         <v>366</v>
-      </c>
-      <c r="H150" s="2" t="s">
-        <v>367</v>
       </c>
       <c r="I150" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H150),2)</f>
@@ -5372,10 +5375,10 @@
         <v>150</v>
       </c>
       <c r="G151" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="H151" s="2" t="s">
         <v>368</v>
-      </c>
-      <c r="H151" s="2" t="s">
-        <v>369</v>
       </c>
       <c r="I151" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H151),2)</f>
@@ -5387,10 +5390,10 @@
         <v>151</v>
       </c>
       <c r="G152" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="H152" s="2" t="s">
         <v>370</v>
-      </c>
-      <c r="H152" s="2" t="s">
-        <v>371</v>
       </c>
       <c r="I152" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H152),2)</f>
@@ -5402,10 +5405,10 @@
         <v>152</v>
       </c>
       <c r="G153" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="H153" s="2" t="s">
         <v>372</v>
-      </c>
-      <c r="H153" s="2" t="s">
-        <v>373</v>
       </c>
       <c r="I153" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H153),2)</f>
@@ -5417,35 +5420,38 @@
         <v>153</v>
       </c>
       <c r="B154" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="C154" s="7" t="s">
         <v>374</v>
-      </c>
-      <c r="C154" s="7" t="s">
-        <v>375</v>
       </c>
       <c r="D154" s="7" t="s">
         <v>163</v>
       </c>
       <c r="F154" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="G154" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="H154" s="8" t="s">
         <v>376</v>
-      </c>
-      <c r="G154" s="7" t="s">
-        <v>376</v>
-      </c>
-      <c r="H154" s="8" t="s">
-        <v>377</v>
       </c>
       <c r="I154" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H154),2)</f>
         <v>28</v>
       </c>
       <c r="L154" s="7" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="7" t="n">
         <v>154</v>
       </c>
+      <c r="C155" s="10" t="s">
+        <v>378</v>
+      </c>
       <c r="G155" s="1" t="s">
         <v>379</v>
       </c>
@@ -7162,7 +7168,7 @@
       <c r="A228" s="7" t="n">
         <v>227</v>
       </c>
-      <c r="C228" s="1" t="s">
+      <c r="C228" s="10" t="s">
         <v>640</v>
       </c>
       <c r="G228" s="1" t="s">
@@ -7291,11 +7297,14 @@
       <c r="A235" s="7" t="n">
         <v>234</v>
       </c>
+      <c r="C235" s="10" t="s">
+        <v>659</v>
+      </c>
       <c r="G235" s="1" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="H235" s="2" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="I235" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H235),2)</f>
@@ -7307,10 +7316,10 @@
         <v>235</v>
       </c>
       <c r="G236" s="1" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="H236" s="2" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="I236" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H236),2)</f>
@@ -7322,10 +7331,10 @@
         <v>236</v>
       </c>
       <c r="G237" s="1" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="H237" s="2" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="I237" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H237),2)</f>
@@ -7337,10 +7346,10 @@
         <v>237</v>
       </c>
       <c r="G238" s="1" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="H238" s="2" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="I238" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H238),2)</f>
@@ -7352,10 +7361,10 @@
         <v>238</v>
       </c>
       <c r="G239" s="1" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="H239" s="2" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="I239" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H239),2)</f>
@@ -7367,40 +7376,43 @@
         <v>239</v>
       </c>
       <c r="B240" s="7" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="C240" s="7" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="D240" s="7" t="s">
         <v>163</v>
       </c>
       <c r="F240" s="7" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="G240" s="7" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="H240" s="8" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="I240" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H240),2)</f>
         <v>48</v>
       </c>
       <c r="L240" s="7" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="7" t="n">
         <v>240</v>
       </c>
+      <c r="C241" s="10" t="s">
+        <v>675</v>
+      </c>
       <c r="G241" s="1" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="H241" s="2" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="I241" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H241),2)</f>
@@ -7412,10 +7424,10 @@
         <v>241</v>
       </c>
       <c r="G242" s="1" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="H242" s="2" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="I242" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H242),2)</f>
@@ -7427,10 +7439,10 @@
         <v>242</v>
       </c>
       <c r="G243" s="1" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="H243" s="2" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="I243" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H243),2)</f>
@@ -7442,10 +7454,10 @@
         <v>243</v>
       </c>
       <c r="G244" s="1" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="H244" s="2" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="I244" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H244),2)</f>
@@ -7457,10 +7469,10 @@
         <v>244</v>
       </c>
       <c r="G245" s="1" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="H245" s="2" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="I245" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H245),2)</f>
@@ -7472,19 +7484,19 @@
         <v>245</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="D246" s="1" t="s">
         <v>85</v>
       </c>
       <c r="F246" s="1" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="G246" s="1" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="H246" s="2" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="I246" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H246),2)</f>
@@ -7494,7 +7506,7 @@
         <v>88</v>
       </c>
       <c r="L246" s="1" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
     </row>
   </sheetData>
@@ -7519,9 +7531,9 @@
   <dimension ref="A1:D257"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="bottomLeft" activeCell="C74" activeCellId="0" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
- change upcode for RC, RNC, RZ and RNZ - change microcode - update microcode and bios
</commit_message>
<xml_diff>
--- a/doc/instruction-set.xlsx
+++ b/doc/instruction-set.xlsx
@@ -1718,7 +1718,7 @@
     <t xml:space="preserve">Return if carry</t>
   </si>
   <si>
-    <t xml:space="preserve">00001111</t>
+    <t xml:space="preserve">00010001</t>
   </si>
   <si>
     <t xml:space="preserve">Return if CF=1</t>
@@ -1730,7 +1730,7 @@
     <t xml:space="preserve">Return if not carry</t>
   </si>
   <si>
-    <t xml:space="preserve">00010001</t>
+    <t xml:space="preserve">00010101</t>
   </si>
   <si>
     <t xml:space="preserve">Return if CF=0</t>
@@ -1742,7 +1742,7 @@
     <t xml:space="preserve">Return if zero</t>
   </si>
   <si>
-    <t xml:space="preserve">00010101</t>
+    <t xml:space="preserve">00100001</t>
   </si>
   <si>
     <t xml:space="preserve">Return if ZF=1</t>
@@ -1754,7 +1754,7 @@
     <t xml:space="preserve">Return if not zero</t>
   </si>
   <si>
-    <t xml:space="preserve">00011111</t>
+    <t xml:space="preserve">00100011</t>
   </si>
   <si>
     <t xml:space="preserve">Return if ZF=0</t>
@@ -2343,9 +2343,9 @@
   <dimension ref="A1:L245"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A224" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A246" activeCellId="0" sqref="A246"/>
+      <selection pane="bottomLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6707,7 +6707,7 @@
       </c>
       <c r="I205" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H205),2)</f>
-        <v>0F</v>
+        <v>11</v>
       </c>
       <c r="L205" s="7" t="s">
         <v>566</v>
@@ -6734,7 +6734,7 @@
       </c>
       <c r="I206" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H206),2)</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="L206" s="7" t="s">
         <v>570</v>
@@ -6761,7 +6761,7 @@
       </c>
       <c r="I207" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H207),2)</f>
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="L207" s="7" t="s">
         <v>574</v>
@@ -6788,7 +6788,7 @@
       </c>
       <c r="I208" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H208),2)</f>
-        <v>1F</v>
+        <v>23</v>
       </c>
       <c r="L208" s="7" t="s">
         <v>578</v>
@@ -7778,7 +7778,7 @@
       </c>
       <c r="B17" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D17,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D17,'Instruction Set'!I:I,0)))</f>
-        <v>RC</v>
+        <v/>
       </c>
       <c r="C17" s="12" t="str">
         <f aca="false">DEC2BIN(A17,8)</f>
@@ -7812,7 +7812,7 @@
       </c>
       <c r="B19" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D19,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D19,'Instruction Set'!I:I,0)))</f>
-        <v>RNC</v>
+        <v>RC</v>
       </c>
       <c r="C19" s="12" t="str">
         <f aca="false">DEC2BIN(A19,8)</f>
@@ -7880,7 +7880,7 @@
       </c>
       <c r="B23" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D23,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D23,'Instruction Set'!I:I,0)))</f>
-        <v>RZ</v>
+        <v>RNC</v>
       </c>
       <c r="C23" s="12" t="str">
         <f aca="false">DEC2BIN(A23,8)</f>
@@ -8050,7 +8050,7 @@
       </c>
       <c r="B33" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D33,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D33,'Instruction Set'!I:I,0)))</f>
-        <v>RNZ</v>
+        <v/>
       </c>
       <c r="C33" s="12" t="str">
         <f aca="false">DEC2BIN(A33,8)</f>
@@ -8084,7 +8084,7 @@
       </c>
       <c r="B35" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D35,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D35,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>RZ</v>
       </c>
       <c r="C35" s="12" t="str">
         <f aca="false">DEC2BIN(A35,8)</f>
@@ -8118,7 +8118,7 @@
       </c>
       <c r="B37" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D37,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D37,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>RNZ</v>
       </c>
       <c r="C37" s="12" t="str">
         <f aca="false">DEC2BIN(A37,8)</f>

</xml_diff>

<commit_message>
add NOT, SHL and SHR
</commit_message>
<xml_diff>
--- a/doc/instruction-set.xlsx
+++ b/doc/instruction-set.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="686">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="695">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -1094,6 +1094,18 @@
     <t xml:space="preserve">00001101</t>
   </si>
   <si>
+    <t xml:space="preserve">NOT M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;r&gt; = 111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00001111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invert all bits in value at memory address in H and L registers (ones‘ complement)</t>
+  </si>
+  <si>
     <t xml:space="preserve">SHL r</t>
   </si>
   <si>
@@ -1142,6 +1154,15 @@
     <t xml:space="preserve">00011101</t>
   </si>
   <si>
+    <t xml:space="preserve">SHL M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00011111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shift all bits in value at memory address in H and L registers by 1 position to left, move MSB into CF</t>
+  </si>
+  <si>
     <t xml:space="preserve">SHR r</t>
   </si>
   <si>
@@ -1188,6 +1209,12 @@
   </si>
   <si>
     <t xml:space="preserve">00101101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHR M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00101111</t>
   </si>
   <si>
     <t xml:space="preserve">JMP M</t>
@@ -2340,7 +2367,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:L245"/>
+  <dimension ref="A1:L248"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -5295,67 +5322,82 @@
         <v>0D</v>
       </c>
     </row>
-    <row r="148" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="7" t="n">
         <v>147</v>
       </c>
-      <c r="B148" s="7" t="s">
+      <c r="B148" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="C148" s="7" t="s">
+      <c r="C148" s="10" t="s">
         <v>358</v>
       </c>
-      <c r="D148" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="F148" s="7" t="s">
+      <c r="D148" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F148" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="G148" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="H148" s="2" t="s">
         <v>359</v>
-      </c>
-      <c r="G148" s="7" t="s">
-        <v>359</v>
-      </c>
-      <c r="H148" s="8" t="s">
-        <v>360</v>
       </c>
       <c r="I148" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H148),2)</f>
-        <v>18</v>
-      </c>
-      <c r="L148" s="7" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0F</v>
+      </c>
+      <c r="L148" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="149" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="7" t="n">
         <v>148</v>
       </c>
-      <c r="C149" s="10" t="s">
+      <c r="B149" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="C149" s="7" t="s">
         <v>362</v>
       </c>
-      <c r="G149" s="1" t="s">
+      <c r="D149" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="F149" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="H149" s="2" t="s">
+      <c r="G149" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="H149" s="8" t="s">
         <v>364</v>
       </c>
       <c r="I149" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H149),2)</f>
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="L149" s="7" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="7" t="n">
         <v>149</v>
       </c>
+      <c r="C150" s="10" t="s">
+        <v>366</v>
+      </c>
       <c r="G150" s="1" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="H150" s="2" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="I150" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H150),2)</f>
-        <v>1A</v>
+        <v>19</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5363,14 +5405,14 @@
         <v>150</v>
       </c>
       <c r="G151" s="1" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="H151" s="2" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="I151" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H151),2)</f>
-        <v>1B</v>
+        <v>1A</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5378,14 +5420,14 @@
         <v>151</v>
       </c>
       <c r="G152" s="1" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="H152" s="2" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="I152" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H152),2)</f>
-        <v>1C</v>
+        <v>1B</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5393,92 +5435,107 @@
         <v>152</v>
       </c>
       <c r="G153" s="1" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="H153" s="2" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="I153" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H153),2)</f>
-        <v>1D</v>
-      </c>
-    </row>
-    <row r="154" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1C</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="7" t="n">
         <v>153</v>
       </c>
-      <c r="B154" s="7" t="s">
-        <v>373</v>
-      </c>
-      <c r="C154" s="7" t="s">
-        <v>374</v>
-      </c>
-      <c r="D154" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="F154" s="7" t="s">
+      <c r="G154" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="G154" s="7" t="s">
-        <v>375</v>
-      </c>
-      <c r="H154" s="8" t="s">
+      <c r="H154" s="2" t="s">
         <v>376</v>
       </c>
       <c r="I154" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H154),2)</f>
-        <v>28</v>
-      </c>
-      <c r="L154" s="7" t="s">
-        <v>377</v>
+        <v>1D</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="7" t="n">
         <v>154</v>
       </c>
+      <c r="B155" s="1" t="s">
+        <v>377</v>
+      </c>
       <c r="C155" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F155" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="G155" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="H155" s="2" t="s">
         <v>378</v>
-      </c>
-      <c r="G155" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="H155" s="2" t="s">
-        <v>380</v>
       </c>
       <c r="I155" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H155),2)</f>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1F</v>
+      </c>
+      <c r="L155" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="156" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="7" t="n">
         <v>155</v>
       </c>
-      <c r="G156" s="1" t="s">
+      <c r="B156" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="C156" s="7" t="s">
         <v>381</v>
       </c>
-      <c r="H156" s="2" t="s">
+      <c r="D156" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="F156" s="7" t="s">
         <v>382</v>
+      </c>
+      <c r="G156" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="H156" s="8" t="s">
+        <v>383</v>
       </c>
       <c r="I156" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H156),2)</f>
-        <v>2A</v>
+        <v>28</v>
+      </c>
+      <c r="L156" s="7" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="7" t="n">
         <v>156</v>
       </c>
+      <c r="C157" s="10" t="s">
+        <v>385</v>
+      </c>
       <c r="G157" s="1" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="H157" s="2" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="I157" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H157),2)</f>
-        <v>2B</v>
+        <v>29</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5486,14 +5543,14 @@
         <v>157</v>
       </c>
       <c r="G158" s="1" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="H158" s="2" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="I158" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H158),2)</f>
-        <v>2C</v>
+        <v>2A</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5501,517 +5558,535 @@
         <v>158</v>
       </c>
       <c r="G159" s="1" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="H159" s="2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="I159" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H159),2)</f>
-        <v>2D</v>
-      </c>
-    </row>
-    <row r="160" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2B</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="7" t="n">
         <v>159</v>
       </c>
-      <c r="B160" s="7" t="s">
-        <v>389</v>
-      </c>
-      <c r="C160" s="7" t="s">
-        <v>390</v>
-      </c>
-      <c r="D160" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F160" s="7" t="s">
-        <v>389</v>
-      </c>
-      <c r="G160" s="7" t="s">
-        <v>389</v>
-      </c>
-      <c r="H160" s="8" t="s">
-        <v>391</v>
+      <c r="G160" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="H160" s="2" t="s">
+        <v>393</v>
       </c>
       <c r="I160" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H160),2)</f>
-        <v>75</v>
-      </c>
-      <c r="L160" s="7" t="s">
-        <v>392</v>
+        <v>2C</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="7" t="n">
         <v>160</v>
       </c>
-      <c r="B161" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="C161" s="10" t="s">
+      <c r="G161" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="D161" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F161" s="1" t="s">
+      <c r="H161" s="2" t="s">
         <v>395</v>
-      </c>
-      <c r="G161" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="H161" s="2" t="s">
-        <v>396</v>
       </c>
       <c r="I161" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H161),2)</f>
-        <v>77</v>
-      </c>
-      <c r="J161" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="K161" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="L161" s="1" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="162" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2D</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="7" t="n">
         <v>161</v>
       </c>
-      <c r="B162" s="7" t="s">
-        <v>398</v>
-      </c>
-      <c r="C162" s="7" t="s">
-        <v>399</v>
-      </c>
-      <c r="D162" s="7" t="s">
+      <c r="B162" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="C162" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="D162" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F162" s="7" t="s">
-        <v>398</v>
-      </c>
-      <c r="G162" s="7" t="s">
-        <v>398</v>
-      </c>
-      <c r="H162" s="8" t="s">
-        <v>400</v>
+      <c r="F162" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="G162" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="H162" s="2" t="s">
+        <v>397</v>
       </c>
       <c r="I162" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H162),2)</f>
-        <v>79</v>
-      </c>
-      <c r="L162" s="7" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2F</v>
+      </c>
+      <c r="L162" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="163" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="7" t="n">
         <v>162</v>
       </c>
-      <c r="B163" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="C163" s="10" t="s">
-        <v>403</v>
-      </c>
-      <c r="D163" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F163" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="G163" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="H163" s="2" t="s">
-        <v>405</v>
+      <c r="B163" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="C163" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="D163" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F163" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="G163" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="H163" s="8" t="s">
+        <v>400</v>
       </c>
       <c r="I163" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H163),2)</f>
-        <v>7B</v>
-      </c>
-      <c r="J163" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="K163" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="L163" s="1" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="164" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>75</v>
+      </c>
+      <c r="L163" s="7" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="7" t="n">
         <v>163</v>
       </c>
-      <c r="B164" s="7" t="s">
-        <v>407</v>
-      </c>
-      <c r="C164" s="7" t="s">
-        <v>408</v>
-      </c>
-      <c r="D164" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F164" s="7" t="s">
-        <v>407</v>
-      </c>
-      <c r="G164" s="7" t="s">
-        <v>407</v>
-      </c>
-      <c r="H164" s="8" t="s">
-        <v>409</v>
+      <c r="B164" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C164" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F164" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="G164" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="H164" s="2" t="s">
+        <v>405</v>
       </c>
       <c r="I164" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H164),2)</f>
-        <v>7D</v>
-      </c>
-      <c r="L164" s="7" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>77</v>
+      </c>
+      <c r="J164" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K164" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L164" s="1" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="165" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="7" t="n">
         <v>164</v>
       </c>
-      <c r="B165" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="C165" s="10" t="s">
-        <v>412</v>
-      </c>
-      <c r="D165" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F165" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="G165" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="H165" s="2" t="s">
-        <v>414</v>
+      <c r="B165" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="C165" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="D165" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F165" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="G165" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="H165" s="8" t="s">
+        <v>409</v>
       </c>
       <c r="I165" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H165),2)</f>
-        <v>7F</v>
-      </c>
-      <c r="J165" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="K165" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="L165" s="1" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="166" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>79</v>
+      </c>
+      <c r="L165" s="7" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="7" t="n">
         <v>165</v>
       </c>
-      <c r="B166" s="7" t="s">
-        <v>416</v>
-      </c>
-      <c r="C166" s="7" t="s">
-        <v>417</v>
-      </c>
-      <c r="D166" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F166" s="7" t="s">
-        <v>416</v>
-      </c>
-      <c r="G166" s="7" t="s">
-        <v>416</v>
-      </c>
-      <c r="H166" s="8" t="s">
-        <v>418</v>
+      <c r="B166" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="C166" s="10" t="s">
+        <v>412</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F166" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="G166" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="H166" s="2" t="s">
+        <v>414</v>
       </c>
       <c r="I166" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H166),2)</f>
-        <v>8F</v>
-      </c>
-      <c r="L166" s="7" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7B</v>
+      </c>
+      <c r="J166" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K166" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L166" s="1" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="167" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="7" t="n">
         <v>166</v>
       </c>
-      <c r="B167" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="C167" s="10" t="s">
-        <v>421</v>
-      </c>
-      <c r="D167" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F167" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="G167" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="H167" s="2" t="s">
-        <v>423</v>
+      <c r="B167" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="C167" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="D167" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F167" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="G167" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="H167" s="8" t="s">
+        <v>418</v>
       </c>
       <c r="I167" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H167),2)</f>
-        <v>9F</v>
-      </c>
-      <c r="J167" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="K167" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="L167" s="1" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="168" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7D</v>
+      </c>
+      <c r="L167" s="7" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="7" t="n">
         <v>167</v>
       </c>
-      <c r="B168" s="7" t="s">
-        <v>425</v>
-      </c>
-      <c r="C168" s="7" t="s">
-        <v>426</v>
-      </c>
-      <c r="D168" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F168" s="7" t="s">
-        <v>425</v>
-      </c>
-      <c r="G168" s="7" t="s">
-        <v>425</v>
-      </c>
-      <c r="H168" s="8" t="s">
-        <v>427</v>
+      <c r="B168" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="C168" s="10" t="s">
+        <v>421</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F168" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="G168" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="H168" s="2" t="s">
+        <v>423</v>
       </c>
       <c r="I168" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H168),2)</f>
-        <v>AF</v>
-      </c>
-      <c r="L168" s="7" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7F</v>
+      </c>
+      <c r="J168" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K168" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L168" s="1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="169" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="7" t="n">
         <v>168</v>
       </c>
-      <c r="B169" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="C169" s="10" t="s">
-        <v>430</v>
-      </c>
-      <c r="D169" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F169" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="G169" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="H169" s="2" t="s">
-        <v>432</v>
+      <c r="B169" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="C169" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="D169" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F169" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="G169" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="H169" s="8" t="s">
+        <v>427</v>
       </c>
       <c r="I169" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H169),2)</f>
-        <v>BF</v>
-      </c>
-      <c r="J169" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="K169" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="L169" s="1" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="170" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8F</v>
+      </c>
+      <c r="L169" s="7" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="7" t="n">
         <v>169</v>
       </c>
-      <c r="B170" s="7" t="s">
-        <v>434</v>
-      </c>
-      <c r="C170" s="7" t="s">
-        <v>435</v>
-      </c>
-      <c r="D170" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F170" s="7" t="s">
-        <v>434</v>
-      </c>
-      <c r="G170" s="7" t="s">
-        <v>434</v>
-      </c>
-      <c r="H170" s="8" t="s">
-        <v>436</v>
+      <c r="B170" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="C170" s="10" t="s">
+        <v>430</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F170" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="G170" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="H170" s="2" t="s">
+        <v>432</v>
       </c>
       <c r="I170" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H170),2)</f>
-        <v>01</v>
-      </c>
-      <c r="L170" s="7" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>9F</v>
+      </c>
+      <c r="J170" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K170" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L170" s="1" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="171" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="7" t="n">
         <v>170</v>
       </c>
-      <c r="B171" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="C171" s="10" t="s">
-        <v>439</v>
-      </c>
-      <c r="D171" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F171" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="G171" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="H171" s="2" t="s">
-        <v>441</v>
+      <c r="B171" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="C171" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="D171" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F171" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="G171" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="H171" s="8" t="s">
+        <v>436</v>
       </c>
       <c r="I171" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H171),2)</f>
-        <v>03</v>
-      </c>
-      <c r="J171" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="K171" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="L171" s="1" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="172" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>AF</v>
+      </c>
+      <c r="L171" s="7" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="7" t="n">
         <v>171</v>
       </c>
-      <c r="B172" s="7" t="s">
-        <v>443</v>
-      </c>
-      <c r="C172" s="7" t="s">
-        <v>444</v>
-      </c>
-      <c r="D172" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F172" s="7" t="s">
-        <v>443</v>
-      </c>
-      <c r="G172" s="7" t="s">
-        <v>443</v>
-      </c>
-      <c r="H172" s="8" t="s">
-        <v>445</v>
+      <c r="B172" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="C172" s="10" t="s">
+        <v>439</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F172" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="G172" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="H172" s="2" t="s">
+        <v>441</v>
       </c>
       <c r="I172" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H172),2)</f>
-        <v>06</v>
-      </c>
-      <c r="L172" s="7" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>BF</v>
+      </c>
+      <c r="J172" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K172" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L172" s="1" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="173" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="7" t="n">
         <v>172</v>
       </c>
-      <c r="B173" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="C173" s="10" t="s">
-        <v>448</v>
-      </c>
-      <c r="D173" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F173" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="G173" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="H173" s="2" t="s">
-        <v>450</v>
+      <c r="B173" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="C173" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="D173" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F173" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="G173" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="H173" s="8" t="s">
+        <v>445</v>
       </c>
       <c r="I173" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H173),2)</f>
-        <v>07</v>
-      </c>
-      <c r="J173" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="K173" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="L173" s="1" t="s">
-        <v>451</v>
+        <v>01</v>
+      </c>
+      <c r="L173" s="7" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="7" t="n">
         <v>173</v>
       </c>
-      <c r="B174" s="11" t="s">
-        <v>452</v>
-      </c>
-      <c r="C174" s="11" t="s">
-        <v>453</v>
-      </c>
-      <c r="D174" s="11" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B174" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="C174" s="10" t="s">
+        <v>448</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F174" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="G174" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="H174" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="I174" s="9" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H174),2)</f>
+        <v>03</v>
+      </c>
+      <c r="J174" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K174" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L174" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="175" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="7" t="n">
         <v>174</v>
       </c>
-      <c r="B175" s="11" t="s">
+      <c r="B175" s="7" t="s">
+        <v>452</v>
+      </c>
+      <c r="C175" s="7" t="s">
+        <v>453</v>
+      </c>
+      <c r="D175" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F175" s="7" t="s">
+        <v>452</v>
+      </c>
+      <c r="G175" s="7" t="s">
+        <v>452</v>
+      </c>
+      <c r="H175" s="8" t="s">
+        <v>454</v>
+      </c>
+      <c r="I175" s="9" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H175),2)</f>
+        <v>06</v>
+      </c>
+      <c r="L175" s="7" t="s">
         <v>455</v>
-      </c>
-      <c r="C175" s="11" t="s">
-        <v>456</v>
-      </c>
-      <c r="D175" s="11" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="7" t="n">
         <v>175</v>
       </c>
-      <c r="B176" s="11" t="s">
+      <c r="B176" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="C176" s="10" t="s">
+        <v>457</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F176" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="C176" s="11" t="s">
+      <c r="G176" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="H176" s="2" t="s">
         <v>459</v>
       </c>
-      <c r="D176" s="11" t="s">
+      <c r="I176" s="9" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H176),2)</f>
+        <v>07</v>
+      </c>
+      <c r="J176" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K176" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L176" s="1" t="s">
         <v>460</v>
       </c>
     </row>
@@ -6040,7 +6115,7 @@
         <v>465</v>
       </c>
       <c r="D178" s="11" t="s">
-        <v>457</v>
+        <v>466</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6048,13 +6123,13 @@
         <v>178</v>
       </c>
       <c r="B179" s="11" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C179" s="11" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="D179" s="11" t="s">
-        <v>454</v>
+        <v>469</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6062,13 +6137,13 @@
         <v>179</v>
       </c>
       <c r="B180" s="11" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="C180" s="11" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="D180" s="11" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6076,516 +6151,516 @@
         <v>180</v>
       </c>
       <c r="B181" s="11" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="C181" s="11" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="D181" s="11" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="182" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="7" t="n">
         <v>181</v>
       </c>
-      <c r="B182" s="7" t="s">
-        <v>474</v>
-      </c>
-      <c r="C182" s="7" t="s">
+      <c r="B182" s="11" t="s">
         <v>475</v>
       </c>
-      <c r="D182" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F182" s="7" t="s">
-        <v>474</v>
-      </c>
-      <c r="G182" s="7" t="s">
-        <v>474</v>
-      </c>
-      <c r="H182" s="8" t="s">
+      <c r="C182" s="11" t="s">
         <v>476</v>
       </c>
-      <c r="I182" s="9" t="str">
-        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H182),2)</f>
-        <v>C1</v>
-      </c>
-      <c r="L182" s="7" t="s">
-        <v>477</v>
+      <c r="D182" s="11" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="7" t="n">
         <v>182</v>
       </c>
-      <c r="B183" s="1" t="s">
+      <c r="B183" s="11" t="s">
+        <v>477</v>
+      </c>
+      <c r="C183" s="11" t="s">
         <v>478</v>
       </c>
-      <c r="C183" s="10" t="s">
+      <c r="D183" s="11" t="s">
         <v>479</v>
       </c>
-      <c r="D183" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F183" s="1" t="s">
-        <v>480</v>
-      </c>
-      <c r="G183" s="1" t="s">
-        <v>478</v>
-      </c>
-      <c r="H183" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="I183" s="9" t="str">
-        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H183),2)</f>
-        <v>C3</v>
-      </c>
-      <c r="J183" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="K183" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="L183" s="1" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="184" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="7" t="n">
         <v>183</v>
       </c>
-      <c r="B184" s="7" t="s">
-        <v>483</v>
-      </c>
-      <c r="C184" s="7" t="s">
-        <v>484</v>
-      </c>
-      <c r="D184" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F184" s="7" t="s">
-        <v>483</v>
-      </c>
-      <c r="G184" s="7" t="s">
-        <v>483</v>
-      </c>
-      <c r="H184" s="8" t="s">
-        <v>485</v>
-      </c>
-      <c r="I184" s="9" t="str">
-        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H184),2)</f>
-        <v>C5</v>
-      </c>
-      <c r="L184" s="7" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B184" s="11" t="s">
+        <v>480</v>
+      </c>
+      <c r="C184" s="11" t="s">
+        <v>481</v>
+      </c>
+      <c r="D184" s="11" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="185" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="7" t="n">
         <v>184</v>
       </c>
-      <c r="B185" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="C185" s="10" t="s">
-        <v>488</v>
-      </c>
-      <c r="D185" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F185" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="G185" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="H185" s="2" t="s">
-        <v>490</v>
+      <c r="B185" s="7" t="s">
+        <v>483</v>
+      </c>
+      <c r="C185" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="D185" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F185" s="7" t="s">
+        <v>483</v>
+      </c>
+      <c r="G185" s="7" t="s">
+        <v>483</v>
+      </c>
+      <c r="H185" s="8" t="s">
+        <v>485</v>
       </c>
       <c r="I185" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H185),2)</f>
-        <v>C7</v>
-      </c>
-      <c r="J185" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="K185" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="L185" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="186" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>C1</v>
+      </c>
+      <c r="L185" s="7" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="7" t="n">
         <v>185</v>
       </c>
-      <c r="B186" s="7" t="s">
-        <v>492</v>
-      </c>
-      <c r="C186" s="7" t="s">
-        <v>493</v>
-      </c>
-      <c r="D186" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F186" s="7" t="s">
-        <v>492</v>
-      </c>
-      <c r="G186" s="7" t="s">
-        <v>492</v>
-      </c>
-      <c r="H186" s="8" t="s">
-        <v>494</v>
+      <c r="B186" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="C186" s="10" t="s">
+        <v>488</v>
+      </c>
+      <c r="D186" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F186" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="G186" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="H186" s="2" t="s">
+        <v>490</v>
       </c>
       <c r="I186" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H186),2)</f>
-        <v>CB</v>
-      </c>
-      <c r="L186" s="7" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>C3</v>
+      </c>
+      <c r="J186" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K186" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L186" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="187" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="7" t="n">
         <v>186</v>
       </c>
-      <c r="B187" s="1" t="s">
-        <v>496</v>
-      </c>
-      <c r="C187" s="10" t="s">
-        <v>497</v>
-      </c>
-      <c r="D187" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F187" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="G187" s="1" t="s">
-        <v>496</v>
-      </c>
-      <c r="H187" s="2" t="s">
-        <v>499</v>
+      <c r="B187" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="C187" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="D187" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F187" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="G187" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="H187" s="8" t="s">
+        <v>494</v>
       </c>
       <c r="I187" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H187),2)</f>
-        <v>CF</v>
-      </c>
-      <c r="J187" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="K187" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="L187" s="1" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="188" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>C5</v>
+      </c>
+      <c r="L187" s="7" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="7" t="n">
         <v>187</v>
       </c>
-      <c r="B188" s="7" t="s">
-        <v>501</v>
-      </c>
-      <c r="C188" s="7" t="s">
-        <v>502</v>
-      </c>
-      <c r="D188" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F188" s="7" t="s">
-        <v>501</v>
-      </c>
-      <c r="G188" s="7" t="s">
-        <v>501</v>
-      </c>
-      <c r="H188" s="8" t="s">
-        <v>503</v>
+      <c r="B188" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="C188" s="10" t="s">
+        <v>497</v>
+      </c>
+      <c r="D188" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F188" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="G188" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="H188" s="2" t="s">
+        <v>499</v>
       </c>
       <c r="I188" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H188),2)</f>
-        <v>D1</v>
-      </c>
-      <c r="L188" s="7" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>C7</v>
+      </c>
+      <c r="J188" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K188" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L188" s="1" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="189" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="7" t="n">
         <v>188</v>
       </c>
-      <c r="B189" s="1" t="s">
-        <v>505</v>
-      </c>
-      <c r="C189" s="10" t="s">
-        <v>506</v>
-      </c>
-      <c r="D189" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F189" s="1" t="s">
-        <v>507</v>
-      </c>
-      <c r="G189" s="1" t="s">
-        <v>505</v>
-      </c>
-      <c r="H189" s="2" t="s">
-        <v>508</v>
+      <c r="B189" s="7" t="s">
+        <v>501</v>
+      </c>
+      <c r="C189" s="7" t="s">
+        <v>502</v>
+      </c>
+      <c r="D189" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F189" s="7" t="s">
+        <v>501</v>
+      </c>
+      <c r="G189" s="7" t="s">
+        <v>501</v>
+      </c>
+      <c r="H189" s="8" t="s">
+        <v>503</v>
       </c>
       <c r="I189" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H189),2)</f>
-        <v>D3</v>
-      </c>
-      <c r="J189" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="K189" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="L189" s="1" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="190" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>CB</v>
+      </c>
+      <c r="L189" s="7" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="7" t="n">
         <v>189</v>
       </c>
-      <c r="B190" s="7" t="s">
-        <v>510</v>
-      </c>
-      <c r="C190" s="7" t="s">
-        <v>511</v>
-      </c>
-      <c r="D190" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F190" s="7" t="s">
-        <v>510</v>
-      </c>
-      <c r="G190" s="7" t="s">
-        <v>510</v>
-      </c>
-      <c r="H190" s="8" t="s">
-        <v>512</v>
+      <c r="B190" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="C190" s="10" t="s">
+        <v>506</v>
+      </c>
+      <c r="D190" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F190" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="G190" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="H190" s="2" t="s">
+        <v>508</v>
       </c>
       <c r="I190" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H190),2)</f>
-        <v>D5</v>
-      </c>
-      <c r="L190" s="7" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>CF</v>
+      </c>
+      <c r="J190" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K190" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L190" s="1" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="191" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="7" t="n">
         <v>190</v>
       </c>
-      <c r="B191" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="C191" s="10" t="s">
-        <v>515</v>
-      </c>
-      <c r="D191" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F191" s="1" t="s">
-        <v>516</v>
-      </c>
-      <c r="G191" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="H191" s="2" t="s">
-        <v>517</v>
+      <c r="B191" s="7" t="s">
+        <v>510</v>
+      </c>
+      <c r="C191" s="7" t="s">
+        <v>511</v>
+      </c>
+      <c r="D191" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F191" s="7" t="s">
+        <v>510</v>
+      </c>
+      <c r="G191" s="7" t="s">
+        <v>510</v>
+      </c>
+      <c r="H191" s="8" t="s">
+        <v>512</v>
       </c>
       <c r="I191" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H191),2)</f>
-        <v>D7</v>
-      </c>
-      <c r="J191" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="K191" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="L191" s="1" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="192" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>D1</v>
+      </c>
+      <c r="L191" s="7" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="7" t="n">
         <v>191</v>
       </c>
-      <c r="B192" s="7" t="s">
-        <v>519</v>
-      </c>
-      <c r="C192" s="7" t="s">
-        <v>520</v>
-      </c>
-      <c r="D192" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F192" s="7" t="s">
-        <v>519</v>
-      </c>
-      <c r="G192" s="7" t="s">
-        <v>519</v>
-      </c>
-      <c r="H192" s="8" t="s">
-        <v>521</v>
+      <c r="B192" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="C192" s="10" t="s">
+        <v>515</v>
+      </c>
+      <c r="D192" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F192" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="G192" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="H192" s="2" t="s">
+        <v>517</v>
       </c>
       <c r="I192" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H192),2)</f>
-        <v>12</v>
-      </c>
-      <c r="L192" s="7" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>D3</v>
+      </c>
+      <c r="J192" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K192" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L192" s="1" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="193" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="7" t="n">
         <v>192</v>
       </c>
-      <c r="B193" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="C193" s="10" t="s">
-        <v>524</v>
-      </c>
-      <c r="D193" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F193" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="G193" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="H193" s="2" t="s">
-        <v>526</v>
+      <c r="B193" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="C193" s="7" t="s">
+        <v>520</v>
+      </c>
+      <c r="D193" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F193" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="G193" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="H193" s="8" t="s">
+        <v>521</v>
       </c>
       <c r="I193" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H193),2)</f>
-        <v>13</v>
-      </c>
-      <c r="J193" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="K193" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="L193" s="1" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="194" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>D5</v>
+      </c>
+      <c r="L193" s="7" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="7" t="n">
         <v>193</v>
       </c>
-      <c r="B194" s="7" t="s">
-        <v>528</v>
-      </c>
-      <c r="C194" s="7" t="s">
-        <v>529</v>
-      </c>
-      <c r="D194" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F194" s="7" t="s">
-        <v>528</v>
-      </c>
-      <c r="G194" s="7" t="s">
-        <v>528</v>
-      </c>
-      <c r="H194" s="8" t="s">
-        <v>530</v>
+      <c r="B194" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="C194" s="10" t="s">
+        <v>524</v>
+      </c>
+      <c r="D194" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F194" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="G194" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="H194" s="2" t="s">
+        <v>526</v>
       </c>
       <c r="I194" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H194),2)</f>
-        <v>16</v>
-      </c>
-      <c r="L194" s="7" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>D7</v>
+      </c>
+      <c r="J194" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K194" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L194" s="1" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="195" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="7" t="n">
         <v>194</v>
       </c>
-      <c r="B195" s="1" t="s">
-        <v>532</v>
-      </c>
-      <c r="C195" s="10" t="s">
-        <v>533</v>
-      </c>
-      <c r="D195" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F195" s="1" t="s">
-        <v>534</v>
-      </c>
-      <c r="G195" s="1" t="s">
-        <v>532</v>
-      </c>
-      <c r="H195" s="2" t="s">
-        <v>535</v>
+      <c r="B195" s="7" t="s">
+        <v>528</v>
+      </c>
+      <c r="C195" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="D195" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F195" s="7" t="s">
+        <v>528</v>
+      </c>
+      <c r="G195" s="7" t="s">
+        <v>528</v>
+      </c>
+      <c r="H195" s="8" t="s">
+        <v>530</v>
       </c>
       <c r="I195" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H195),2)</f>
-        <v>17</v>
-      </c>
-      <c r="J195" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="K195" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="L195" s="1" t="s">
-        <v>536</v>
+        <v>12</v>
+      </c>
+      <c r="L195" s="7" t="s">
+        <v>531</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="7" t="n">
         <v>195</v>
       </c>
-      <c r="B196" s="11" t="s">
-        <v>537</v>
-      </c>
-      <c r="C196" s="11" t="s">
-        <v>538</v>
-      </c>
-      <c r="D196" s="11" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B196" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="C196" s="10" t="s">
+        <v>533</v>
+      </c>
+      <c r="D196" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F196" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="G196" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="H196" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="I196" s="9" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H196),2)</f>
+        <v>13</v>
+      </c>
+      <c r="J196" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K196" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L196" s="1" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="197" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="7" t="n">
         <v>196</v>
       </c>
-      <c r="B197" s="11" t="s">
+      <c r="B197" s="7" t="s">
+        <v>537</v>
+      </c>
+      <c r="C197" s="7" t="s">
+        <v>538</v>
+      </c>
+      <c r="D197" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F197" s="7" t="s">
+        <v>537</v>
+      </c>
+      <c r="G197" s="7" t="s">
+        <v>537</v>
+      </c>
+      <c r="H197" s="8" t="s">
+        <v>539</v>
+      </c>
+      <c r="I197" s="9" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H197),2)</f>
+        <v>16</v>
+      </c>
+      <c r="L197" s="7" t="s">
         <v>540</v>
-      </c>
-      <c r="C197" s="11" t="s">
-        <v>541</v>
-      </c>
-      <c r="D197" s="11" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="7" t="n">
         <v>197</v>
       </c>
-      <c r="B198" s="11" t="s">
+      <c r="B198" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="C198" s="10" t="s">
+        <v>542</v>
+      </c>
+      <c r="D198" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F198" s="1" t="s">
         <v>543</v>
       </c>
-      <c r="C198" s="11" t="s">
+      <c r="G198" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="H198" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="D198" s="11" t="s">
+      <c r="I198" s="9" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H198),2)</f>
+        <v>17</v>
+      </c>
+      <c r="J198" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K198" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L198" s="1" t="s">
         <v>545</v>
       </c>
     </row>
@@ -6614,7 +6689,7 @@
         <v>550</v>
       </c>
       <c r="D200" s="11" t="s">
-        <v>542</v>
+        <v>551</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6622,13 +6697,13 @@
         <v>200</v>
       </c>
       <c r="B201" s="11" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="C201" s="11" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="D201" s="11" t="s">
-        <v>539</v>
+        <v>554</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6636,13 +6711,13 @@
         <v>201</v>
       </c>
       <c r="B202" s="11" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="C202" s="11" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="D202" s="11" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6650,94 +6725,55 @@
         <v>202</v>
       </c>
       <c r="B203" s="11" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="C203" s="11" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="D203" s="11" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="204" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="7" t="n">
         <v>203</v>
       </c>
-      <c r="B204" s="7" t="s">
-        <v>559</v>
-      </c>
-      <c r="C204" s="7" t="s">
+      <c r="B204" s="11" t="s">
         <v>560</v>
       </c>
-      <c r="F204" s="7" t="s">
-        <v>559</v>
-      </c>
-      <c r="G204" s="7" t="s">
-        <v>559</v>
-      </c>
-      <c r="H204" s="8" t="s">
+      <c r="C204" s="11" t="s">
         <v>561</v>
       </c>
-      <c r="I204" s="9" t="str">
-        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H204),2)</f>
-        <v>05</v>
-      </c>
-      <c r="L204" s="7" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="205" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D204" s="11" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="7" t="n">
         <v>204</v>
       </c>
-      <c r="B205" s="7" t="s">
+      <c r="B205" s="11" t="s">
+        <v>562</v>
+      </c>
+      <c r="C205" s="11" t="s">
         <v>563</v>
       </c>
-      <c r="C205" s="7" t="s">
+      <c r="D205" s="11" t="s">
         <v>564</v>
       </c>
-      <c r="F205" s="7" t="s">
-        <v>563</v>
-      </c>
-      <c r="G205" s="7" t="s">
-        <v>563</v>
-      </c>
-      <c r="H205" s="8" t="s">
-        <v>565</v>
-      </c>
-      <c r="I205" s="9" t="str">
-        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H205),2)</f>
-        <v>11</v>
-      </c>
-      <c r="L205" s="7" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="206" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="7" t="n">
         <v>205</v>
       </c>
-      <c r="B206" s="7" t="s">
+      <c r="B206" s="11" t="s">
+        <v>565</v>
+      </c>
+      <c r="C206" s="11" t="s">
+        <v>566</v>
+      </c>
+      <c r="D206" s="11" t="s">
         <v>567</v>
-      </c>
-      <c r="C206" s="7" t="s">
-        <v>568</v>
-      </c>
-      <c r="F206" s="7" t="s">
-        <v>567</v>
-      </c>
-      <c r="G206" s="7" t="s">
-        <v>567</v>
-      </c>
-      <c r="H206" s="8" t="s">
-        <v>569</v>
-      </c>
-      <c r="I206" s="9" t="str">
-        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H206),2)</f>
-        <v>15</v>
-      </c>
-      <c r="L206" s="7" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="207" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6745,26 +6781,26 @@
         <v>206</v>
       </c>
       <c r="B207" s="7" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="C207" s="7" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="F207" s="7" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="G207" s="7" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="H207" s="8" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="I207" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H207),2)</f>
-        <v>21</v>
+        <v>05</v>
       </c>
       <c r="L207" s="7" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="208" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6772,26 +6808,26 @@
         <v>207</v>
       </c>
       <c r="B208" s="7" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="C208" s="7" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="F208" s="7" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="G208" s="7" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="H208" s="8" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="I208" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H208),2)</f>
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="L208" s="7" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
     </row>
     <row r="209" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6799,26 +6835,26 @@
         <v>208</v>
       </c>
       <c r="B209" s="7" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="C209" s="7" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="F209" s="7" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="G209" s="7" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="H209" s="8" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="I209" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H209),2)</f>
-        <v>83</v>
+        <v>15</v>
       </c>
       <c r="L209" s="7" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="210" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6826,67 +6862,106 @@
         <v>209</v>
       </c>
       <c r="B210" s="7" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="C210" s="7" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="F210" s="7" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="G210" s="7" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="H210" s="8" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="I210" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H210),2)</f>
-        <v>85</v>
+        <v>21</v>
       </c>
       <c r="L210" s="7" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="211" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="7" t="n">
         <v>210</v>
       </c>
-      <c r="B211" s="11" t="s">
+      <c r="B211" s="7" t="s">
+        <v>584</v>
+      </c>
+      <c r="C211" s="7" t="s">
+        <v>585</v>
+      </c>
+      <c r="F211" s="7" t="s">
+        <v>584</v>
+      </c>
+      <c r="G211" s="7" t="s">
+        <v>584</v>
+      </c>
+      <c r="H211" s="8" t="s">
+        <v>586</v>
+      </c>
+      <c r="I211" s="9" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H211),2)</f>
+        <v>23</v>
+      </c>
+      <c r="L211" s="7" t="s">
         <v>587</v>
       </c>
-      <c r="C211" s="11" t="s">
-        <v>588</v>
-      </c>
-      <c r="D211" s="11" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="212" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="7" t="n">
         <v>211</v>
       </c>
-      <c r="B212" s="11" t="s">
+      <c r="B212" s="7" t="s">
+        <v>588</v>
+      </c>
+      <c r="C212" s="7" t="s">
+        <v>589</v>
+      </c>
+      <c r="F212" s="7" t="s">
+        <v>588</v>
+      </c>
+      <c r="G212" s="7" t="s">
+        <v>588</v>
+      </c>
+      <c r="H212" s="8" t="s">
         <v>590</v>
       </c>
-      <c r="C212" s="11" t="s">
+      <c r="I212" s="9" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H212),2)</f>
+        <v>83</v>
+      </c>
+      <c r="L212" s="7" t="s">
         <v>591</v>
       </c>
-      <c r="D212" s="11" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="213" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="7" t="n">
         <v>212</v>
       </c>
-      <c r="B213" s="11" t="s">
+      <c r="B213" s="7" t="s">
+        <v>592</v>
+      </c>
+      <c r="C213" s="7" t="s">
         <v>593</v>
       </c>
-      <c r="C213" s="11" t="s">
+      <c r="F213" s="7" t="s">
+        <v>592</v>
+      </c>
+      <c r="G213" s="7" t="s">
+        <v>592</v>
+      </c>
+      <c r="H213" s="8" t="s">
         <v>594</v>
       </c>
-      <c r="D213" s="11" t="s">
+      <c r="I213" s="9" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H213),2)</f>
+        <v>85</v>
+      </c>
+      <c r="L213" s="7" t="s">
         <v>595</v>
       </c>
     </row>
@@ -6915,7 +6990,7 @@
         <v>600</v>
       </c>
       <c r="D215" s="11" t="s">
-        <v>592</v>
+        <v>601</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6923,13 +6998,13 @@
         <v>215</v>
       </c>
       <c r="B216" s="11" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="C216" s="11" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="D216" s="11" t="s">
-        <v>589</v>
+        <v>604</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6937,13 +7012,13 @@
         <v>216</v>
       </c>
       <c r="B217" s="11" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="C217" s="11" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="D217" s="11" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6951,139 +7026,136 @@
         <v>217</v>
       </c>
       <c r="B218" s="11" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="C218" s="11" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="D218" s="11" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="219" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="7" t="n">
         <v>218</v>
       </c>
-      <c r="B219" s="7" t="s">
-        <v>609</v>
-      </c>
-      <c r="C219" s="7" t="s">
+      <c r="B219" s="11" t="s">
         <v>610</v>
       </c>
-      <c r="D219" s="7" t="s">
+      <c r="C219" s="11" t="s">
         <v>611</v>
       </c>
-      <c r="F219" s="7" t="s">
-        <v>612</v>
-      </c>
-      <c r="G219" s="7" t="s">
-        <v>613</v>
-      </c>
-      <c r="H219" s="7" t="n">
-        <v>11011111</v>
-      </c>
-      <c r="I219" s="9" t="str">
-        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H219),2)</f>
-        <v>DF</v>
-      </c>
-      <c r="J219" s="7" t="s">
-        <v>614</v>
-      </c>
-      <c r="L219" s="7" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="220" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D219" s="11" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="7" t="n">
         <v>219</v>
       </c>
-      <c r="B220" s="7" t="s">
-        <v>616</v>
-      </c>
-      <c r="C220" s="7" t="s">
-        <v>617</v>
-      </c>
-      <c r="D220" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="F220" s="7" t="s">
-        <v>618</v>
-      </c>
-      <c r="G220" s="7" t="s">
-        <v>618</v>
-      </c>
-      <c r="H220" s="8" t="s">
-        <v>619</v>
-      </c>
-      <c r="I220" s="9" t="str">
-        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H220),2)</f>
-        <v>F0</v>
-      </c>
-      <c r="L220" s="7" t="s">
-        <v>620</v>
+      <c r="B220" s="11" t="s">
+        <v>612</v>
+      </c>
+      <c r="C220" s="11" t="s">
+        <v>613</v>
+      </c>
+      <c r="D220" s="11" t="s">
+        <v>614</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="7" t="n">
         <v>220</v>
       </c>
-      <c r="C221" s="10" t="s">
-        <v>621</v>
-      </c>
-      <c r="G221" s="1" t="s">
-        <v>622</v>
-      </c>
-      <c r="H221" s="2" t="s">
-        <v>623</v>
-      </c>
-      <c r="I221" s="9" t="str">
-        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H221),2)</f>
-        <v>F1</v>
-      </c>
-    </row>
-    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B221" s="11" t="s">
+        <v>615</v>
+      </c>
+      <c r="C221" s="11" t="s">
+        <v>616</v>
+      </c>
+      <c r="D221" s="11" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="222" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="7" t="n">
         <v>221</v>
       </c>
-      <c r="G222" s="1" t="s">
-        <v>624</v>
-      </c>
-      <c r="H222" s="2" t="s">
-        <v>625</v>
+      <c r="B222" s="7" t="s">
+        <v>618</v>
+      </c>
+      <c r="C222" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="D222" s="7" t="s">
+        <v>620</v>
+      </c>
+      <c r="F222" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="G222" s="7" t="s">
+        <v>622</v>
+      </c>
+      <c r="H222" s="7" t="n">
+        <v>11011111</v>
       </c>
       <c r="I222" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H222),2)</f>
-        <v>F2</v>
-      </c>
-    </row>
-    <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>DF</v>
+      </c>
+      <c r="J222" s="7" t="s">
+        <v>623</v>
+      </c>
+      <c r="L222" s="7" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="223" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="7" t="n">
         <v>222</v>
       </c>
-      <c r="G223" s="1" t="s">
+      <c r="B223" s="7" t="s">
+        <v>625</v>
+      </c>
+      <c r="C223" s="7" t="s">
         <v>626</v>
       </c>
-      <c r="H223" s="2" t="s">
+      <c r="D223" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="F223" s="7" t="s">
         <v>627</v>
+      </c>
+      <c r="G223" s="7" t="s">
+        <v>627</v>
+      </c>
+      <c r="H223" s="8" t="s">
+        <v>628</v>
       </c>
       <c r="I223" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H223),2)</f>
-        <v>F3</v>
+        <v>F0</v>
+      </c>
+      <c r="L223" s="7" t="s">
+        <v>629</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="7" t="n">
         <v>223</v>
       </c>
+      <c r="C224" s="10" t="s">
+        <v>630</v>
+      </c>
       <c r="G224" s="1" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="H224" s="2" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="I224" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H224),2)</f>
-        <v>F4</v>
+        <v>F1</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7091,128 +7163,128 @@
         <v>224</v>
       </c>
       <c r="G225" s="1" t="s">
-        <v>630</v>
+        <v>633</v>
       </c>
       <c r="H225" s="2" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
       <c r="I225" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H225),2)</f>
-        <v>F5</v>
+        <v>F2</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="7" t="n">
         <v>225</v>
       </c>
-      <c r="D226" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="G226" s="1" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="H226" s="2" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="I226" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H226),2)</f>
-        <v>F6</v>
-      </c>
-      <c r="L226" s="1" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="227" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>F3</v>
+      </c>
+    </row>
+    <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="7" t="n">
         <v>226</v>
       </c>
-      <c r="B227" s="7" t="s">
-        <v>635</v>
-      </c>
-      <c r="C227" s="7" t="s">
-        <v>636</v>
-      </c>
-      <c r="D227" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="F227" s="7" t="s">
+      <c r="G227" s="1" t="s">
         <v>637</v>
       </c>
-      <c r="G227" s="7" t="s">
-        <v>637</v>
-      </c>
-      <c r="H227" s="8" t="s">
+      <c r="H227" s="2" t="s">
         <v>638</v>
       </c>
       <c r="I227" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H227),2)</f>
-        <v>F8</v>
-      </c>
-      <c r="L227" s="7" t="s">
-        <v>639</v>
+        <v>F4</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="7" t="n">
         <v>227</v>
       </c>
-      <c r="C228" s="10" t="s">
+      <c r="G228" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="H228" s="2" t="s">
         <v>640</v>
-      </c>
-      <c r="G228" s="1" t="s">
-        <v>641</v>
-      </c>
-      <c r="H228" s="2" t="s">
-        <v>642</v>
       </c>
       <c r="I228" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H228),2)</f>
-        <v>F9</v>
+        <v>F5</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="7" t="n">
         <v>228</v>
       </c>
+      <c r="D229" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="G229" s="1" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="H229" s="2" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="I229" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H229),2)</f>
-        <v>FA</v>
-      </c>
-    </row>
-    <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>F6</v>
+      </c>
+      <c r="L229" s="1" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="230" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="7" t="n">
         <v>229</v>
       </c>
-      <c r="G230" s="1" t="s">
+      <c r="B230" s="7" t="s">
+        <v>644</v>
+      </c>
+      <c r="C230" s="7" t="s">
         <v>645</v>
       </c>
-      <c r="H230" s="2" t="s">
+      <c r="D230" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="F230" s="7" t="s">
         <v>646</v>
+      </c>
+      <c r="G230" s="7" t="s">
+        <v>646</v>
+      </c>
+      <c r="H230" s="8" t="s">
+        <v>647</v>
       </c>
       <c r="I230" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H230),2)</f>
-        <v>FB</v>
+        <v>F8</v>
+      </c>
+      <c r="L230" s="7" t="s">
+        <v>648</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="7" t="n">
         <v>230</v>
       </c>
+      <c r="C231" s="10" t="s">
+        <v>649</v>
+      </c>
       <c r="G231" s="1" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
       <c r="H231" s="2" t="s">
-        <v>648</v>
+        <v>651</v>
       </c>
       <c r="I231" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H231),2)</f>
-        <v>FC</v>
+        <v>F9</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7220,128 +7292,128 @@
         <v>231</v>
       </c>
       <c r="G232" s="1" t="s">
-        <v>649</v>
+        <v>652</v>
       </c>
       <c r="H232" s="2" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
       <c r="I232" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H232),2)</f>
-        <v>FD</v>
+        <v>FA</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="7" t="n">
         <v>232</v>
       </c>
-      <c r="D233" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="G233" s="1" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="H233" s="2" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
       <c r="I233" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H233),2)</f>
-        <v>FE</v>
-      </c>
-      <c r="L233" s="1" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="234" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>FB</v>
+      </c>
+    </row>
+    <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="7" t="n">
         <v>233</v>
       </c>
-      <c r="B234" s="7" t="s">
-        <v>654</v>
-      </c>
-      <c r="C234" s="7" t="s">
-        <v>655</v>
-      </c>
-      <c r="D234" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="F234" s="7" t="s">
+      <c r="G234" s="1" t="s">
         <v>656</v>
       </c>
-      <c r="G234" s="7" t="s">
-        <v>656</v>
-      </c>
-      <c r="H234" s="8" t="s">
+      <c r="H234" s="2" t="s">
         <v>657</v>
       </c>
       <c r="I234" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H234),2)</f>
-        <v>40</v>
-      </c>
-      <c r="L234" s="7" t="s">
-        <v>658</v>
+        <v>FC</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="7" t="n">
         <v>234</v>
       </c>
-      <c r="C235" s="10" t="s">
+      <c r="G235" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="H235" s="2" t="s">
         <v>659</v>
-      </c>
-      <c r="G235" s="1" t="s">
-        <v>660</v>
-      </c>
-      <c r="H235" s="2" t="s">
-        <v>661</v>
       </c>
       <c r="I235" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H235),2)</f>
-        <v>41</v>
+        <v>FD</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="7" t="n">
         <v>235</v>
       </c>
+      <c r="D236" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="G236" s="1" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="H236" s="2" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="I236" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H236),2)</f>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>FE</v>
+      </c>
+      <c r="L236" s="1" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="237" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="7" t="n">
         <v>236</v>
       </c>
-      <c r="G237" s="1" t="s">
+      <c r="B237" s="7" t="s">
+        <v>663</v>
+      </c>
+      <c r="C237" s="7" t="s">
         <v>664</v>
       </c>
-      <c r="H237" s="2" t="s">
+      <c r="D237" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="F237" s="7" t="s">
         <v>665</v>
+      </c>
+      <c r="G237" s="7" t="s">
+        <v>665</v>
+      </c>
+      <c r="H237" s="8" t="s">
+        <v>666</v>
       </c>
       <c r="I237" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H237),2)</f>
-        <v>43</v>
+        <v>40</v>
+      </c>
+      <c r="L237" s="7" t="s">
+        <v>667</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="7" t="n">
         <v>237</v>
       </c>
+      <c r="C238" s="10" t="s">
+        <v>668</v>
+      </c>
       <c r="G238" s="1" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="H238" s="2" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
       <c r="I238" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H238),2)</f>
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7349,62 +7421,44 @@
         <v>238</v>
       </c>
       <c r="G239" s="1" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
       <c r="H239" s="2" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="I239" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H239),2)</f>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="240" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="7" t="n">
         <v>239</v>
       </c>
-      <c r="B240" s="7" t="s">
-        <v>670</v>
-      </c>
-      <c r="C240" s="7" t="s">
-        <v>671</v>
-      </c>
-      <c r="D240" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="F240" s="7" t="s">
-        <v>672</v>
-      </c>
-      <c r="G240" s="7" t="s">
-        <v>672</v>
-      </c>
-      <c r="H240" s="8" t="s">
+      <c r="G240" s="1" t="s">
         <v>673</v>
+      </c>
+      <c r="H240" s="2" t="s">
+        <v>674</v>
       </c>
       <c r="I240" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H240),2)</f>
-        <v>48</v>
-      </c>
-      <c r="L240" s="7" t="s">
-        <v>674</v>
+        <v>43</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="7" t="n">
         <v>240</v>
       </c>
-      <c r="C241" s="10" t="s">
+      <c r="G241" s="1" t="s">
         <v>675</v>
       </c>
-      <c r="G241" s="1" t="s">
+      <c r="H241" s="2" t="s">
         <v>676</v>
-      </c>
-      <c r="H241" s="2" t="s">
-        <v>677</v>
       </c>
       <c r="I241" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H241),2)</f>
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7412,44 +7466,62 @@
         <v>241</v>
       </c>
       <c r="G242" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="H242" s="2" t="s">
         <v>678</v>
-      </c>
-      <c r="H242" s="2" t="s">
-        <v>679</v>
       </c>
       <c r="I242" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H242),2)</f>
-        <v>4A</v>
-      </c>
-    </row>
-    <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="243" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="7" t="n">
         <v>242</v>
       </c>
-      <c r="G243" s="1" t="s">
+      <c r="B243" s="7" t="s">
+        <v>679</v>
+      </c>
+      <c r="C243" s="7" t="s">
         <v>680</v>
       </c>
-      <c r="H243" s="2" t="s">
+      <c r="D243" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="F243" s="7" t="s">
         <v>681</v>
+      </c>
+      <c r="G243" s="7" t="s">
+        <v>681</v>
+      </c>
+      <c r="H243" s="8" t="s">
+        <v>682</v>
       </c>
       <c r="I243" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H243),2)</f>
-        <v>4B</v>
+        <v>48</v>
+      </c>
+      <c r="L243" s="7" t="s">
+        <v>683</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="7" t="n">
         <v>243</v>
       </c>
+      <c r="C244" s="10" t="s">
+        <v>684</v>
+      </c>
       <c r="G244" s="1" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
       <c r="H244" s="2" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="I244" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H244),2)</f>
-        <v>4C</v>
+        <v>49</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7457,18 +7529,63 @@
         <v>244</v>
       </c>
       <c r="G245" s="1" t="s">
-        <v>684</v>
+        <v>687</v>
       </c>
       <c r="H245" s="2" t="s">
-        <v>685</v>
+        <v>688</v>
       </c>
       <c r="I245" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H245),2)</f>
+        <v>4A</v>
+      </c>
+    </row>
+    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A246" s="7" t="n">
+        <v>245</v>
+      </c>
+      <c r="G246" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="H246" s="2" t="s">
+        <v>690</v>
+      </c>
+      <c r="I246" s="9" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H246),2)</f>
+        <v>4B</v>
+      </c>
+    </row>
+    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A247" s="7" t="n">
+        <v>246</v>
+      </c>
+      <c r="G247" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="H247" s="2" t="s">
+        <v>692</v>
+      </c>
+      <c r="I247" s="9" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H247),2)</f>
+        <v>4C</v>
+      </c>
+    </row>
+    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A248" s="7" t="n">
+        <v>247</v>
+      </c>
+      <c r="G248" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="H248" s="2" t="s">
+        <v>694</v>
+      </c>
+      <c r="I248" s="9" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H248),2)</f>
         <v>4D</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I2:I173 I182:I195 I204:I210 I219:I245">
+  <conditionalFormatting sqref="I2:I176 I185:I198 I207:I213 I222:I248">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -7489,7 +7606,7 @@
   <dimension ref="A1:D257"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="C74" activeCellId="0" sqref="C74"/>
     </sheetView>
@@ -7778,7 +7895,7 @@
       </c>
       <c r="B17" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D17,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D17,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>NOT M</v>
       </c>
       <c r="C17" s="12" t="str">
         <f aca="false">DEC2BIN(A17,8)</f>
@@ -8050,7 +8167,7 @@
       </c>
       <c r="B33" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D33,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D33,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>SHL M</v>
       </c>
       <c r="C33" s="12" t="str">
         <f aca="false">DEC2BIN(A33,8)</f>
@@ -8322,7 +8439,7 @@
       </c>
       <c r="B49" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D49,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D49,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>SHR M</v>
       </c>
       <c r="C49" s="12" t="str">
         <f aca="false">DEC2BIN(A49,8)</f>

</xml_diff>

<commit_message>
remove in and out
</commit_message>
<xml_diff>
--- a/doc/instruction-set.xlsx
+++ b/doc/instruction-set.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="695">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="663">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -2010,102 +2010,6 @@
   </si>
   <si>
     <t xml:space="preserve">Decrement value at memory address in H and L registers by 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IN r</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input from I/O port</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IN A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move value from port number in H and L registers into destination register</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01000&lt;r&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IN B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01000001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IN C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01000010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IN D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01000011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IN H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01000100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IN L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01000101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OUT r</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output to I/O port</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OUT A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01001000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move value from source register into port number in H and L registers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01001&lt;r&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OUT B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01001001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OUT C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01001010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OUT D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01001011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OUT H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01001100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OUT L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01001101</t>
   </si>
 </sst>
 </file>
@@ -2367,7 +2271,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:L248"/>
+  <dimension ref="A1:L236"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2375,15 +2279,15 @@
       <selection pane="bottomLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="9.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="12.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="26.44"/>
@@ -7368,224 +7272,8 @@
         <v>662</v>
       </c>
     </row>
-    <row r="237" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A237" s="7" t="n">
-        <v>236</v>
-      </c>
-      <c r="B237" s="7" t="s">
-        <v>663</v>
-      </c>
-      <c r="C237" s="7" t="s">
-        <v>664</v>
-      </c>
-      <c r="D237" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="F237" s="7" t="s">
-        <v>665</v>
-      </c>
-      <c r="G237" s="7" t="s">
-        <v>665</v>
-      </c>
-      <c r="H237" s="8" t="s">
-        <v>666</v>
-      </c>
-      <c r="I237" s="9" t="str">
-        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H237),2)</f>
-        <v>40</v>
-      </c>
-      <c r="L237" s="7" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A238" s="7" t="n">
-        <v>237</v>
-      </c>
-      <c r="C238" s="10" t="s">
-        <v>668</v>
-      </c>
-      <c r="G238" s="1" t="s">
-        <v>669</v>
-      </c>
-      <c r="H238" s="2" t="s">
-        <v>670</v>
-      </c>
-      <c r="I238" s="9" t="str">
-        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H238),2)</f>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A239" s="7" t="n">
-        <v>238</v>
-      </c>
-      <c r="G239" s="1" t="s">
-        <v>671</v>
-      </c>
-      <c r="H239" s="2" t="s">
-        <v>672</v>
-      </c>
-      <c r="I239" s="9" t="str">
-        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H239),2)</f>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A240" s="7" t="n">
-        <v>239</v>
-      </c>
-      <c r="G240" s="1" t="s">
-        <v>673</v>
-      </c>
-      <c r="H240" s="2" t="s">
-        <v>674</v>
-      </c>
-      <c r="I240" s="9" t="str">
-        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H240),2)</f>
-        <v>43</v>
-      </c>
-    </row>
-    <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A241" s="7" t="n">
-        <v>240</v>
-      </c>
-      <c r="G241" s="1" t="s">
-        <v>675</v>
-      </c>
-      <c r="H241" s="2" t="s">
-        <v>676</v>
-      </c>
-      <c r="I241" s="9" t="str">
-        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H241),2)</f>
-        <v>44</v>
-      </c>
-    </row>
-    <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A242" s="7" t="n">
-        <v>241</v>
-      </c>
-      <c r="G242" s="1" t="s">
-        <v>677</v>
-      </c>
-      <c r="H242" s="2" t="s">
-        <v>678</v>
-      </c>
-      <c r="I242" s="9" t="str">
-        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H242),2)</f>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="243" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A243" s="7" t="n">
-        <v>242</v>
-      </c>
-      <c r="B243" s="7" t="s">
-        <v>679</v>
-      </c>
-      <c r="C243" s="7" t="s">
-        <v>680</v>
-      </c>
-      <c r="D243" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="F243" s="7" t="s">
-        <v>681</v>
-      </c>
-      <c r="G243" s="7" t="s">
-        <v>681</v>
-      </c>
-      <c r="H243" s="8" t="s">
-        <v>682</v>
-      </c>
-      <c r="I243" s="9" t="str">
-        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H243),2)</f>
-        <v>48</v>
-      </c>
-      <c r="L243" s="7" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A244" s="7" t="n">
-        <v>243</v>
-      </c>
-      <c r="C244" s="10" t="s">
-        <v>684</v>
-      </c>
-      <c r="G244" s="1" t="s">
-        <v>685</v>
-      </c>
-      <c r="H244" s="2" t="s">
-        <v>686</v>
-      </c>
-      <c r="I244" s="9" t="str">
-        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H244),2)</f>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A245" s="7" t="n">
-        <v>244</v>
-      </c>
-      <c r="G245" s="1" t="s">
-        <v>687</v>
-      </c>
-      <c r="H245" s="2" t="s">
-        <v>688</v>
-      </c>
-      <c r="I245" s="9" t="str">
-        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H245),2)</f>
-        <v>4A</v>
-      </c>
-    </row>
-    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A246" s="7" t="n">
-        <v>245</v>
-      </c>
-      <c r="G246" s="1" t="s">
-        <v>689</v>
-      </c>
-      <c r="H246" s="2" t="s">
-        <v>690</v>
-      </c>
-      <c r="I246" s="9" t="str">
-        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H246),2)</f>
-        <v>4B</v>
-      </c>
-    </row>
-    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A247" s="7" t="n">
-        <v>246</v>
-      </c>
-      <c r="G247" s="1" t="s">
-        <v>691</v>
-      </c>
-      <c r="H247" s="2" t="s">
-        <v>692</v>
-      </c>
-      <c r="I247" s="9" t="str">
-        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H247),2)</f>
-        <v>4C</v>
-      </c>
-    </row>
-    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A248" s="7" t="n">
-        <v>247</v>
-      </c>
-      <c r="G248" s="1" t="s">
-        <v>693</v>
-      </c>
-      <c r="H248" s="2" t="s">
-        <v>694</v>
-      </c>
-      <c r="I248" s="9" t="str">
-        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H248),2)</f>
-        <v>4D</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="I2:I176 I185:I198 I207:I213 I222:I248">
+  <conditionalFormatting sqref="I2:I176 I185:I198 I207:I213 I222:I236">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -7611,13 +7299,12 @@
       <selection pane="bottomLeft" activeCell="C74" activeCellId="0" sqref="C74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.6"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="12" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="12" width="12.96"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8728,7 +8415,7 @@
       </c>
       <c r="B66" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D66,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D66,'Instruction Set'!I:I,0)))</f>
-        <v>IN A</v>
+        <v/>
       </c>
       <c r="C66" s="12" t="str">
         <f aca="false">DEC2BIN(A66,8)</f>
@@ -8745,7 +8432,7 @@
       </c>
       <c r="B67" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D67,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D67,'Instruction Set'!I:I,0)))</f>
-        <v>IN B</v>
+        <v/>
       </c>
       <c r="C67" s="12" t="str">
         <f aca="false">DEC2BIN(A67,8)</f>
@@ -8762,7 +8449,7 @@
       </c>
       <c r="B68" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D68,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D68,'Instruction Set'!I:I,0)))</f>
-        <v>IN C</v>
+        <v/>
       </c>
       <c r="C68" s="12" t="str">
         <f aca="false">DEC2BIN(A68,8)</f>
@@ -8779,7 +8466,7 @@
       </c>
       <c r="B69" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D69,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D69,'Instruction Set'!I:I,0)))</f>
-        <v>IN D</v>
+        <v/>
       </c>
       <c r="C69" s="12" t="str">
         <f aca="false">DEC2BIN(A69,8)</f>
@@ -8796,7 +8483,7 @@
       </c>
       <c r="B70" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D70,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D70,'Instruction Set'!I:I,0)))</f>
-        <v>IN H</v>
+        <v/>
       </c>
       <c r="C70" s="12" t="str">
         <f aca="false">DEC2BIN(A70,8)</f>
@@ -8813,7 +8500,7 @@
       </c>
       <c r="B71" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D71,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D71,'Instruction Set'!I:I,0)))</f>
-        <v>IN L</v>
+        <v/>
       </c>
       <c r="C71" s="12" t="str">
         <f aca="false">DEC2BIN(A71,8)</f>
@@ -8864,7 +8551,7 @@
       </c>
       <c r="B74" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D74,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D74,'Instruction Set'!I:I,0)))</f>
-        <v>OUT A</v>
+        <v/>
       </c>
       <c r="C74" s="12" t="str">
         <f aca="false">DEC2BIN(A74,8)</f>
@@ -8881,7 +8568,7 @@
       </c>
       <c r="B75" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D75,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D75,'Instruction Set'!I:I,0)))</f>
-        <v>OUT B</v>
+        <v/>
       </c>
       <c r="C75" s="12" t="str">
         <f aca="false">DEC2BIN(A75,8)</f>
@@ -8898,7 +8585,7 @@
       </c>
       <c r="B76" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D76,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D76,'Instruction Set'!I:I,0)))</f>
-        <v>OUT C</v>
+        <v/>
       </c>
       <c r="C76" s="12" t="str">
         <f aca="false">DEC2BIN(A76,8)</f>
@@ -8915,7 +8602,7 @@
       </c>
       <c r="B77" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D77,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D77,'Instruction Set'!I:I,0)))</f>
-        <v>OUT D</v>
+        <v/>
       </c>
       <c r="C77" s="12" t="str">
         <f aca="false">DEC2BIN(A77,8)</f>
@@ -8932,7 +8619,7 @@
       </c>
       <c r="B78" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D78,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D78,'Instruction Set'!I:I,0)))</f>
-        <v>OUT H</v>
+        <v/>
       </c>
       <c r="C78" s="12" t="str">
         <f aca="false">DEC2BIN(A78,8)</f>
@@ -8949,7 +8636,7 @@
       </c>
       <c r="B79" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D79,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D79,'Instruction Set'!I:I,0)))</f>
-        <v>OUT L</v>
+        <v/>
       </c>
       <c r="C79" s="12" t="str">
         <f aca="false">DEC2BIN(A79,8)</f>

</xml_diff>

<commit_message>
add PUSHF and POPF instructions
</commit_message>
<xml_diff>
--- a/doc/instruction-set.xlsx
+++ b/doc/instruction-set.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="693">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -2076,6 +2076,30 @@
   </si>
   <si>
     <t xml:space="preserve">Decrement value at memory address in H and L registers by 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUSHF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Push flags</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10000111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Push flags to stack and decrease stack pointer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POPF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pop flags</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11011001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pop flags from stack and increase stack pointer</t>
   </si>
 </sst>
 </file>
@@ -2337,7 +2361,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:L244"/>
+  <dimension ref="A1:L246"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2348,7 +2372,7 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.3"/>
@@ -7500,8 +7524,62 @@
         <v>684</v>
       </c>
     </row>
+    <row r="245" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A245" s="7" t="n">
+        <v>244</v>
+      </c>
+      <c r="B245" s="7" t="s">
+        <v>685</v>
+      </c>
+      <c r="C245" s="7" t="s">
+        <v>686</v>
+      </c>
+      <c r="F245" s="7" t="s">
+        <v>685</v>
+      </c>
+      <c r="G245" s="7" t="s">
+        <v>685</v>
+      </c>
+      <c r="H245" s="8" t="s">
+        <v>687</v>
+      </c>
+      <c r="I245" s="9" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H245),2)</f>
+        <v>87</v>
+      </c>
+      <c r="L245" s="7" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="246" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A246" s="7" t="n">
+        <v>245</v>
+      </c>
+      <c r="B246" s="7" t="s">
+        <v>689</v>
+      </c>
+      <c r="C246" s="7" t="s">
+        <v>690</v>
+      </c>
+      <c r="F246" s="7" t="s">
+        <v>689</v>
+      </c>
+      <c r="G246" s="7" t="s">
+        <v>689</v>
+      </c>
+      <c r="H246" s="8" t="s">
+        <v>691</v>
+      </c>
+      <c r="I246" s="9" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H246),2)</f>
+        <v>D9</v>
+      </c>
+      <c r="L246" s="7" t="s">
+        <v>692</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="I2:I184 I193:I206 I215:I221 I230:I244">
+  <conditionalFormatting sqref="I2:I184 I193:I206 I215:I221 I230:I246">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -7527,11 +7605,11 @@
       <selection pane="bottomLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.6"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="12" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="12" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="12" width="12.96"/>
   </cols>
   <sheetData>
@@ -9850,7 +9928,7 @@
       </c>
       <c r="B137" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D137,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D137,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>PUSHF</v>
       </c>
       <c r="C137" s="12" t="str">
         <f aca="false">DEC2BIN(A137,8)</f>
@@ -11244,7 +11322,7 @@
       </c>
       <c r="B219" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D219,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D219,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>POPF</v>
       </c>
       <c r="C219" s="12" t="str">
         <f aca="false">DEC2BIN(A219,8)</f>

</xml_diff>

<commit_message>
add INCHL and DECHL instructions
</commit_message>
<xml_diff>
--- a/doc/instruction-set.xlsx
+++ b/doc/instruction-set.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="697">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="705">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -2033,6 +2033,18 @@
     <t xml:space="preserve">Increment value at memory address in H and L registers by 1</t>
   </si>
   <si>
+    <t xml:space="preserve">INCHL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increment HL register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10010111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increment HL register by 1 (carry from L to H if needed)</t>
+  </si>
+  <si>
     <t xml:space="preserve">DEC r</t>
   </si>
   <si>
@@ -2088,6 +2100,18 @@
   </si>
   <si>
     <t xml:space="preserve">Decrement value at memory address in H and L registers by 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DECHL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decrement HL register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10100111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decrement HL register by 1 (borrow from H to L if needed)</t>
   </si>
   <si>
     <t xml:space="preserve">PUSHF</t>
@@ -2373,7 +2397,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:L247"/>
+  <dimension ref="A1:L249"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7444,57 +7468,69 @@
       <c r="C239" s="7" t="s">
         <v>671</v>
       </c>
-      <c r="D239" s="7" t="s">
-        <v>163</v>
-      </c>
       <c r="F239" s="7" t="s">
+        <v>670</v>
+      </c>
+      <c r="G239" s="7" t="s">
+        <v>670</v>
+      </c>
+      <c r="H239" s="8" t="s">
         <v>672</v>
-      </c>
-      <c r="G239" s="7" t="s">
-        <v>672</v>
-      </c>
-      <c r="H239" s="8" t="s">
-        <v>673</v>
       </c>
       <c r="I239" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H239),2)</f>
-        <v>F8</v>
+        <v>97</v>
       </c>
       <c r="L239" s="7" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="240" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="7" t="n">
         <v>239</v>
       </c>
-      <c r="C240" s="10" t="s">
+      <c r="B240" s="7" t="s">
+        <v>674</v>
+      </c>
+      <c r="C240" s="7" t="s">
         <v>675</v>
       </c>
-      <c r="G240" s="1" t="s">
+      <c r="D240" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="F240" s="7" t="s">
         <v>676</v>
       </c>
-      <c r="H240" s="2" t="s">
+      <c r="G240" s="7" t="s">
+        <v>676</v>
+      </c>
+      <c r="H240" s="8" t="s">
         <v>677</v>
       </c>
       <c r="I240" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H240),2)</f>
-        <v>F9</v>
+        <v>F8</v>
+      </c>
+      <c r="L240" s="7" t="s">
+        <v>678</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="7" t="n">
         <v>240</v>
       </c>
+      <c r="C241" s="10" t="s">
+        <v>679</v>
+      </c>
       <c r="G241" s="1" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="H241" s="2" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="I241" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H241),2)</f>
-        <v>FA</v>
+        <v>F9</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7502,14 +7538,14 @@
         <v>241</v>
       </c>
       <c r="G242" s="1" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="H242" s="2" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="I242" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H242),2)</f>
-        <v>FB</v>
+        <v>FA</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7517,14 +7553,14 @@
         <v>242</v>
       </c>
       <c r="G243" s="1" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="H243" s="2" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="I243" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H243),2)</f>
-        <v>FC</v>
+        <v>FB</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7532,61 +7568,49 @@
         <v>243</v>
       </c>
       <c r="G244" s="1" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="H244" s="2" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="I244" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H244),2)</f>
-        <v>FD</v>
+        <v>FC</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="7" t="n">
         <v>244</v>
       </c>
-      <c r="D245" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="G245" s="1" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="H245" s="2" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="I245" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H245),2)</f>
-        <v>FE</v>
-      </c>
-      <c r="L245" s="1" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="246" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>FD</v>
+      </c>
+    </row>
+    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="7" t="n">
         <v>245</v>
       </c>
-      <c r="B246" s="7" t="s">
-        <v>689</v>
-      </c>
-      <c r="C246" s="7" t="s">
+      <c r="D246" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G246" s="1" t="s">
         <v>690</v>
       </c>
-      <c r="F246" s="7" t="s">
-        <v>689</v>
-      </c>
-      <c r="G246" s="7" t="s">
-        <v>689</v>
-      </c>
-      <c r="H246" s="8" t="s">
+      <c r="H246" s="2" t="s">
         <v>691</v>
       </c>
       <c r="I246" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H246),2)</f>
-        <v>87</v>
-      </c>
-      <c r="L246" s="7" t="s">
+        <v>FE</v>
+      </c>
+      <c r="L246" s="1" t="s">
         <v>692</v>
       </c>
     </row>
@@ -7611,14 +7635,68 @@
       </c>
       <c r="I247" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H247),2)</f>
-        <v>D9</v>
+        <v>A7</v>
       </c>
       <c r="L247" s="7" t="s">
         <v>696</v>
       </c>
     </row>
+    <row r="248" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A248" s="7" t="n">
+        <v>247</v>
+      </c>
+      <c r="B248" s="7" t="s">
+        <v>697</v>
+      </c>
+      <c r="C248" s="7" t="s">
+        <v>698</v>
+      </c>
+      <c r="F248" s="7" t="s">
+        <v>697</v>
+      </c>
+      <c r="G248" s="7" t="s">
+        <v>697</v>
+      </c>
+      <c r="H248" s="8" t="s">
+        <v>699</v>
+      </c>
+      <c r="I248" s="9" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H248),2)</f>
+        <v>87</v>
+      </c>
+      <c r="L248" s="7" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="249" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="7" t="n">
+        <v>248</v>
+      </c>
+      <c r="B249" s="7" t="s">
+        <v>701</v>
+      </c>
+      <c r="C249" s="7" t="s">
+        <v>702</v>
+      </c>
+      <c r="F249" s="7" t="s">
+        <v>701</v>
+      </c>
+      <c r="G249" s="7" t="s">
+        <v>701</v>
+      </c>
+      <c r="H249" s="8" t="s">
+        <v>703</v>
+      </c>
+      <c r="I249" s="9" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H249),2)</f>
+        <v>D9</v>
+      </c>
+      <c r="L249" s="7" t="s">
+        <v>704</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="I2:I184 I193:I206 I215:I221 I230:I247">
+  <conditionalFormatting sqref="I2:I184 I193:I206 I215:I221 I230:I249">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -7644,7 +7722,7 @@
       <selection pane="bottomLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.6"/>
@@ -10239,7 +10317,7 @@
       </c>
       <c r="B153" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D153,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D153,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>INCHL</v>
       </c>
       <c r="C153" s="12" t="str">
         <f aca="false">DEC2BIN(A153,8)</f>
@@ -10511,7 +10589,7 @@
       </c>
       <c r="B169" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D169,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D169,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>DECHL</v>
       </c>
       <c r="C169" s="12" t="str">
         <f aca="false">DEC2BIN(A169,8)</f>

</xml_diff>

<commit_message>
re-org instruction set overview
</commit_message>
<xml_diff>
--- a/doc/instruction-set.xlsx
+++ b/doc/instruction-set.xlsx
@@ -2033,6 +2033,63 @@
     <t xml:space="preserve">Increment value at memory address in H and L registers by 1</t>
   </si>
   <si>
+    <t xml:space="preserve">DEC r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decrement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEC A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11111000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decrement register by 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11111&lt;r&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEC B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11111001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEC C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11111010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEC D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11111011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEC H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11111100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEC L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11111101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEC M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11111110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decrement value at memory address in H and L registers by 1</t>
+  </si>
+  <si>
     <t xml:space="preserve">INCHL</t>
   </si>
   <si>
@@ -2043,63 +2100,6 @@
   </si>
   <si>
     <t xml:space="preserve">Increment HL register by 1 (carry from L to H if needed)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEC r</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Decrement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEC A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11111000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Decrement register by 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11111&lt;r&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEC B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11111001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEC C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11111010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEC D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11111011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEC H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11111100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEC L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11111101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEC M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11111110</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Decrement value at memory address in H and L registers by 1</t>
   </si>
   <si>
     <t xml:space="preserve">DECHL</t>
@@ -7468,69 +7468,57 @@
       <c r="C239" s="7" t="s">
         <v>671</v>
       </c>
+      <c r="D239" s="7" t="s">
+        <v>163</v>
+      </c>
       <c r="F239" s="7" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="G239" s="7" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="H239" s="8" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="I239" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H239),2)</f>
-        <v>97</v>
+        <v>F8</v>
       </c>
       <c r="L239" s="7" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="240" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="7" t="n">
         <v>239</v>
       </c>
-      <c r="B240" s="7" t="s">
-        <v>674</v>
-      </c>
-      <c r="C240" s="7" t="s">
+      <c r="C240" s="10" t="s">
         <v>675</v>
       </c>
-      <c r="D240" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="F240" s="7" t="s">
+      <c r="G240" s="1" t="s">
         <v>676</v>
       </c>
-      <c r="G240" s="7" t="s">
-        <v>676</v>
-      </c>
-      <c r="H240" s="8" t="s">
+      <c r="H240" s="2" t="s">
         <v>677</v>
       </c>
       <c r="I240" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H240),2)</f>
-        <v>F8</v>
-      </c>
-      <c r="L240" s="7" t="s">
-        <v>678</v>
+        <v>F9</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="7" t="n">
         <v>240</v>
       </c>
-      <c r="C241" s="10" t="s">
+      <c r="G241" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="H241" s="2" t="s">
         <v>679</v>
-      </c>
-      <c r="G241" s="1" t="s">
-        <v>680</v>
-      </c>
-      <c r="H241" s="2" t="s">
-        <v>681</v>
       </c>
       <c r="I241" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H241),2)</f>
-        <v>F9</v>
+        <v>FA</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7538,14 +7526,14 @@
         <v>241</v>
       </c>
       <c r="G242" s="1" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="H242" s="2" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="I242" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H242),2)</f>
-        <v>FA</v>
+        <v>FB</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7553,14 +7541,14 @@
         <v>242</v>
       </c>
       <c r="G243" s="1" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="H243" s="2" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="I243" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H243),2)</f>
-        <v>FB</v>
+        <v>FC</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7568,49 +7556,61 @@
         <v>243</v>
       </c>
       <c r="G244" s="1" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="H244" s="2" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="I244" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H244),2)</f>
-        <v>FC</v>
+        <v>FD</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="7" t="n">
         <v>244</v>
       </c>
+      <c r="D245" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="G245" s="1" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="H245" s="2" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="I245" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H245),2)</f>
-        <v>FD</v>
-      </c>
-    </row>
-    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>FE</v>
+      </c>
+      <c r="L245" s="1" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="246" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="7" t="n">
         <v>245</v>
       </c>
-      <c r="D246" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G246" s="1" t="s">
+      <c r="B246" s="7" t="s">
+        <v>689</v>
+      </c>
+      <c r="C246" s="7" t="s">
         <v>690</v>
       </c>
-      <c r="H246" s="2" t="s">
+      <c r="F246" s="7" t="s">
+        <v>689</v>
+      </c>
+      <c r="G246" s="7" t="s">
+        <v>689</v>
+      </c>
+      <c r="H246" s="8" t="s">
         <v>691</v>
       </c>
       <c r="I246" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H246),2)</f>
-        <v>FE</v>
-      </c>
-      <c r="L246" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="L246" s="7" t="s">
         <v>692</v>
       </c>
     </row>
@@ -7722,7 +7722,7 @@
       <selection pane="bottomLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.6"/>

</xml_diff>

<commit_message>
add PUSHHL and POPHL
</commit_message>
<xml_diff>
--- a/doc/instruction-set.xlsx
+++ b/doc/instruction-set.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="705">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="713">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -2112,6 +2112,30 @@
   </si>
   <si>
     <t xml:space="preserve">Decrement HL register by 1 (borrow from H to L if needed)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUSHHL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Push HL register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10010001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Push HL register to stack and decrease stack pointer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POPHL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pop HL register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10010101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pop HL register from stack and increase stack pointer</t>
   </si>
   <si>
     <t xml:space="preserve">PUSHF</t>
@@ -2397,7 +2421,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:L249"/>
+  <dimension ref="A1:L251"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7662,7 +7686,7 @@
       </c>
       <c r="I248" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H248),2)</f>
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="L248" s="7" t="s">
         <v>700</v>
@@ -7689,14 +7713,68 @@
       </c>
       <c r="I249" s="9" t="str">
         <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H249),2)</f>
-        <v>D9</v>
+        <v>95</v>
       </c>
       <c r="L249" s="7" t="s">
         <v>704</v>
       </c>
     </row>
+    <row r="250" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A250" s="7" t="n">
+        <v>249</v>
+      </c>
+      <c r="B250" s="7" t="s">
+        <v>705</v>
+      </c>
+      <c r="C250" s="7" t="s">
+        <v>706</v>
+      </c>
+      <c r="F250" s="7" t="s">
+        <v>705</v>
+      </c>
+      <c r="G250" s="7" t="s">
+        <v>705</v>
+      </c>
+      <c r="H250" s="8" t="s">
+        <v>707</v>
+      </c>
+      <c r="I250" s="9" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H250),2)</f>
+        <v>87</v>
+      </c>
+      <c r="L250" s="7" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="251" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A251" s="7" t="n">
+        <v>250</v>
+      </c>
+      <c r="B251" s="7" t="s">
+        <v>709</v>
+      </c>
+      <c r="C251" s="7" t="s">
+        <v>710</v>
+      </c>
+      <c r="F251" s="7" t="s">
+        <v>709</v>
+      </c>
+      <c r="G251" s="7" t="s">
+        <v>709</v>
+      </c>
+      <c r="H251" s="8" t="s">
+        <v>711</v>
+      </c>
+      <c r="I251" s="9" t="str">
+        <f aca="false">BIN2HEX(_xlfn.NUMBERVALUE(H251),2)</f>
+        <v>D9</v>
+      </c>
+      <c r="L251" s="7" t="s">
+        <v>712</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="I2:I184 I193:I206 I215:I221 I230:I249">
+  <conditionalFormatting sqref="I2:I184 I193:I206 I215:I221 I230:I251">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -7717,12 +7795,12 @@
   <dimension ref="A1:D257"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="B147" activeCellId="0" sqref="B147"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.6"/>
@@ -10215,7 +10293,7 @@
       </c>
       <c r="B147" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D147,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D147,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>PUSHHL</v>
       </c>
       <c r="C147" s="12" t="str">
         <f aca="false">DEC2BIN(A147,8)</f>
@@ -10283,7 +10361,7 @@
       </c>
       <c r="B151" s="0" t="str">
         <f aca="false">IF(ISERROR(INDEX('Instruction Set'!G:G,MATCH(D151,'Instruction Set'!I:I,0))),"",INDEX('Instruction Set'!G:G,MATCH(D151,'Instruction Set'!I:I,0)))</f>
-        <v/>
+        <v>POPHL</v>
       </c>
       <c r="C151" s="12" t="str">
         <f aca="false">DEC2BIN(A151,8)</f>

</xml_diff>